<commit_message>
data up to 27th
</commit_message>
<xml_diff>
--- a/away3-6hours.xlsx
+++ b/away3-6hours.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="234">
   <si>
     <t>Alaska</t>
   </si>
@@ -681,6 +681,42 @@
   <si>
     <t>15 07 2020</t>
   </si>
+  <si>
+    <t>16 07 2020</t>
+  </si>
+  <si>
+    <t>17 07 2020</t>
+  </si>
+  <si>
+    <t>18 07 2020</t>
+  </si>
+  <si>
+    <t>19 07 2020</t>
+  </si>
+  <si>
+    <t>20 07 2020</t>
+  </si>
+  <si>
+    <t>21 07 2020</t>
+  </si>
+  <si>
+    <t>22 07 2020</t>
+  </si>
+  <si>
+    <t>23 07 2020</t>
+  </si>
+  <si>
+    <t>24 07 2020</t>
+  </si>
+  <si>
+    <t>25 07 2020</t>
+  </si>
+  <si>
+    <t>26 07 2020</t>
+  </si>
+  <si>
+    <t>27 07 2020</t>
+  </si>
 </sst>
 </file>
 
@@ -1011,7 +1047,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BE167"/>
+  <dimension ref="A1:BE179"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -13310,6 +13346,9 @@
       <c r="D72">
         <v>0.046383489176654</v>
       </c>
+      <c r="E72">
+        <v>0.125</v>
+      </c>
       <c r="F72">
         <v>0.04917785881492</v>
       </c>
@@ -13480,6 +13519,9 @@
       <c r="D73">
         <v>0.040598003135225</v>
       </c>
+      <c r="E73">
+        <v>0.066666666666667</v>
+      </c>
       <c r="F73">
         <v>0.04962085582709</v>
       </c>
@@ -13650,6 +13692,9 @@
       <c r="D74">
         <v>0.075087768365804</v>
       </c>
+      <c r="E74">
+        <v>0.16666666666667</v>
+      </c>
       <c r="F74">
         <v>0.05651969309226</v>
       </c>
@@ -13820,6 +13865,9 @@
       <c r="D75">
         <v>0.079605116208637</v>
       </c>
+      <c r="E75">
+        <v>0.13392857142857</v>
+      </c>
       <c r="F75">
         <v>0.07302491978987199</v>
       </c>
@@ -13990,6 +14038,9 @@
       <c r="D76">
         <v>0.08125475388135101</v>
       </c>
+      <c r="E76">
+        <v>0.20261437908497</v>
+      </c>
       <c r="F76">
         <v>0.066555005443107</v>
       </c>
@@ -14160,6 +14211,9 @@
       <c r="D77">
         <v>0.08645823167080199</v>
       </c>
+      <c r="E77">
+        <v>0.12521043771044</v>
+      </c>
       <c r="F77">
         <v>0.061464595410973</v>
       </c>
@@ -14330,6 +14384,9 @@
       <c r="D78">
         <v>0.085693926726507</v>
       </c>
+      <c r="E78">
+        <v>0.087121212121212</v>
+      </c>
       <c r="F78">
         <v>0.075992503285555</v>
       </c>
@@ -14500,6 +14557,9 @@
       <c r="D79">
         <v>0.053612739069274</v>
       </c>
+      <c r="E79">
+        <v>0.10714285714286</v>
+      </c>
       <c r="F79">
         <v>0.056345599811811</v>
       </c>
@@ -14670,6 +14730,9 @@
       <c r="D80">
         <v>0.043137683724926</v>
       </c>
+      <c r="E80">
+        <v>0.12222222222222</v>
+      </c>
       <c r="F80">
         <v>0.042417454654857</v>
       </c>
@@ -28771,25 +28834,2065 @@
       <c r="A163" t="s">
         <v>217</v>
       </c>
+      <c r="B163">
+        <v>0.07357828806314901</v>
+      </c>
+      <c r="C163">
+        <v>0.073454748122011</v>
+      </c>
+      <c r="D163">
+        <v>0.06504071429965599</v>
+      </c>
+      <c r="F163">
+        <v>0.061359074786194</v>
+      </c>
+      <c r="G163">
+        <v>0.067088515270048</v>
+      </c>
+      <c r="H163">
+        <v>0.06986990090801599</v>
+      </c>
+      <c r="I163">
+        <v>0.046524023847164</v>
+      </c>
+      <c r="J163">
+        <v>0.04588643561482</v>
+      </c>
+      <c r="K163">
+        <v>0.050046189901838</v>
+      </c>
+      <c r="L163">
+        <v>0.045807447024644</v>
+      </c>
+      <c r="M163">
+        <v>0.05073853581601</v>
+      </c>
+      <c r="N163">
+        <v>0.071375508855436</v>
+      </c>
+      <c r="O163">
+        <v>0.053518094172258</v>
+      </c>
+      <c r="P163">
+        <v>0.060433039023674</v>
+      </c>
+      <c r="Q163">
+        <v>0.06455689428617099</v>
+      </c>
+      <c r="R163">
+        <v>0.049781455961207</v>
+      </c>
+      <c r="S163">
+        <v>0.054917595207966</v>
+      </c>
+      <c r="T163">
+        <v>0.056336690476947</v>
+      </c>
+      <c r="U163">
+        <v>0.055667424558545</v>
+      </c>
+      <c r="V163">
+        <v>0.061299786877144</v>
+      </c>
+      <c r="W163">
+        <v>0.05266479064929</v>
+      </c>
+      <c r="X163">
+        <v>0.048423081488713</v>
+      </c>
+      <c r="Y163">
+        <v>0.051463246989976</v>
+      </c>
+      <c r="Z163">
+        <v>0.059367113434331</v>
+      </c>
+      <c r="AA163">
+        <v>0.058578407031025</v>
+      </c>
+      <c r="AB163">
+        <v>0.06936034723645999</v>
+      </c>
+      <c r="AC163">
+        <v>0.12720859387526</v>
+      </c>
+      <c r="AD163">
+        <v>0.073585976364741</v>
+      </c>
+      <c r="AE163">
+        <v>0.084803035974069</v>
+      </c>
+      <c r="AF163">
+        <v>0.060164453526664</v>
+      </c>
+      <c r="AG163">
+        <v>0.061179880750493</v>
+      </c>
+      <c r="AH163">
+        <v>0.07296322154825299</v>
+      </c>
+      <c r="AI163">
+        <v>0.058615738912874</v>
+      </c>
+      <c r="AJ163">
+        <v>0.055102265139803</v>
+      </c>
+      <c r="AK163">
+        <v>0.07285999933819599</v>
+      </c>
+      <c r="AL163">
+        <v>0.070046620359308</v>
+      </c>
+      <c r="AM163">
+        <v>0.051605465772156</v>
+      </c>
+      <c r="AN163">
+        <v>0.057254836742012</v>
+      </c>
+      <c r="AO163">
+        <v>0.061618177173335</v>
+      </c>
+      <c r="AP163">
+        <v>0.065996965015092</v>
+      </c>
+      <c r="AQ163">
+        <v>0.054839093577295</v>
+      </c>
+      <c r="AR163">
+        <v>0.049222736787526</v>
+      </c>
+      <c r="AS163">
+        <v>0.057377237006707</v>
+      </c>
+      <c r="AT163">
+        <v>0.063441335521883</v>
+      </c>
+      <c r="AU163">
+        <v>0.070584642811219</v>
+      </c>
+      <c r="AV163">
+        <v>0.06193064486074</v>
+      </c>
+      <c r="AW163">
+        <v>0.054433006881984</v>
+      </c>
+      <c r="AX163">
+        <v>0.07495932825552799</v>
+      </c>
+      <c r="AY163">
+        <v>0.054531538344058</v>
+      </c>
+      <c r="AZ163">
+        <v>0.083157303268729</v>
+      </c>
+      <c r="BA163">
+        <v>0.049788443564221</v>
+      </c>
+      <c r="BB163">
+        <v>0.059903999327954</v>
+      </c>
+      <c r="BC163">
+        <v>0.05925811045613</v>
+      </c>
+      <c r="BD163">
+        <v>0.054844293294785</v>
+      </c>
+      <c r="BE163">
+        <v>0.07827668358694299</v>
+      </c>
     </row>
     <row r="164" spans="1:57">
       <c r="A164" t="s">
         <v>218</v>
       </c>
+      <c r="B164">
+        <v>0.05199043359566</v>
+      </c>
+      <c r="C164">
+        <v>0.040912046044947</v>
+      </c>
+      <c r="D164">
+        <v>0.047429151017146</v>
+      </c>
+      <c r="F164">
+        <v>0.047735587425188</v>
+      </c>
+      <c r="G164">
+        <v>0.055974707216074</v>
+      </c>
+      <c r="H164">
+        <v>0.064968427778718</v>
+      </c>
+      <c r="I164">
+        <v>0.057481223618301</v>
+      </c>
+      <c r="J164">
+        <v>0.055667506796959</v>
+      </c>
+      <c r="K164">
+        <v>0.057368245188502</v>
+      </c>
+      <c r="L164">
+        <v>0.047163438750165</v>
+      </c>
+      <c r="M164">
+        <v>0.048898923284863</v>
+      </c>
+      <c r="N164">
+        <v>0.064565525213695</v>
+      </c>
+      <c r="O164">
+        <v>0.054111348086843</v>
+      </c>
+      <c r="P164">
+        <v>0.053687423005062</v>
+      </c>
+      <c r="Q164">
+        <v>0.060468139390961</v>
+      </c>
+      <c r="R164">
+        <v>0.04879204819758</v>
+      </c>
+      <c r="S164">
+        <v>0.048414878779433</v>
+      </c>
+      <c r="T164">
+        <v>0.051221211277398</v>
+      </c>
+      <c r="U164">
+        <v>0.047749821953009</v>
+      </c>
+      <c r="V164">
+        <v>0.053788062639107</v>
+      </c>
+      <c r="W164">
+        <v>0.054694355229024</v>
+      </c>
+      <c r="X164">
+        <v>0.045647001517295</v>
+      </c>
+      <c r="Y164">
+        <v>0.054400683876097</v>
+      </c>
+      <c r="Z164">
+        <v>0.046033581716599</v>
+      </c>
+      <c r="AA164">
+        <v>0.04413304740427</v>
+      </c>
+      <c r="AB164">
+        <v>0.052811190150157</v>
+      </c>
+      <c r="AC164">
+        <v>0.13610500610501</v>
+      </c>
+      <c r="AD164">
+        <v>0.051252150193068</v>
+      </c>
+      <c r="AE164">
+        <v>0.060225143254442</v>
+      </c>
+      <c r="AF164">
+        <v>0.049540601781322</v>
+      </c>
+      <c r="AG164">
+        <v>0.048982164317608</v>
+      </c>
+      <c r="AH164">
+        <v>0.052615803634576</v>
+      </c>
+      <c r="AI164">
+        <v>0.052195138475411</v>
+      </c>
+      <c r="AJ164">
+        <v>0.051925163537934</v>
+      </c>
+      <c r="AK164">
+        <v>0.054307854491073</v>
+      </c>
+      <c r="AL164">
+        <v>0.050982759861603</v>
+      </c>
+      <c r="AM164">
+        <v>0.049535196084735</v>
+      </c>
+      <c r="AN164">
+        <v>0.046493205877214</v>
+      </c>
+      <c r="AO164">
+        <v>0.048524672892075</v>
+      </c>
+      <c r="AP164">
+        <v>0.049226618177234</v>
+      </c>
+      <c r="AQ164">
+        <v>0.047764615141643</v>
+      </c>
+      <c r="AR164">
+        <v>0.042442431692096</v>
+      </c>
+      <c r="AS164">
+        <v>0.05859710549265</v>
+      </c>
+      <c r="AT164">
+        <v>0.04958228347399</v>
+      </c>
+      <c r="AU164">
+        <v>0.056373088151248</v>
+      </c>
+      <c r="AV164">
+        <v>0.046508259215169</v>
+      </c>
+      <c r="AW164">
+        <v>0.042755029871542</v>
+      </c>
+      <c r="AX164">
+        <v>0.054470583674963</v>
+      </c>
+      <c r="AY164">
+        <v>0.04846356151042</v>
+      </c>
+      <c r="AZ164">
+        <v>0.07716212152008201</v>
+      </c>
+      <c r="BA164">
+        <v>0.049052778799732</v>
+      </c>
+      <c r="BB164">
+        <v>0.049672369702941</v>
+      </c>
+      <c r="BC164">
+        <v>0.051287369361708</v>
+      </c>
+      <c r="BD164">
+        <v>0.049485825351865</v>
+      </c>
+      <c r="BE164">
+        <v>0.065509638146594</v>
+      </c>
     </row>
     <row r="165" spans="1:57">
       <c r="A165" t="s">
         <v>219</v>
       </c>
+      <c r="B165">
+        <v>0.094868933073836</v>
+      </c>
+      <c r="C165">
+        <v>0.10981476904738</v>
+      </c>
+      <c r="D165">
+        <v>0.11377863618376</v>
+      </c>
+      <c r="F165">
+        <v>0.088311771490418</v>
+      </c>
+      <c r="G165">
+        <v>0.076169284540871</v>
+      </c>
+      <c r="H165">
+        <v>0.081885292218769</v>
+      </c>
+      <c r="I165">
+        <v>0.069617455940142</v>
+      </c>
+      <c r="J165">
+        <v>0.053588723013136</v>
+      </c>
+      <c r="K165">
+        <v>0.06921345124210899</v>
+      </c>
+      <c r="L165">
+        <v>0.074284552546491</v>
+      </c>
+      <c r="M165">
+        <v>0.084069921499804</v>
+      </c>
+      <c r="N165">
+        <v>0.061066540398087</v>
+      </c>
+      <c r="O165">
+        <v>0.088826356675153</v>
+      </c>
+      <c r="P165">
+        <v>0.082294835458062</v>
+      </c>
+      <c r="Q165">
+        <v>0.090883446001004</v>
+      </c>
+      <c r="R165">
+        <v>0.067348956041096</v>
+      </c>
+      <c r="S165">
+        <v>0.075819897214276</v>
+      </c>
+      <c r="T165">
+        <v>0.082990630468582</v>
+      </c>
+      <c r="U165">
+        <v>0.07618819710944599</v>
+      </c>
+      <c r="V165">
+        <v>0.083168859310918</v>
+      </c>
+      <c r="W165">
+        <v>0.056906954075184</v>
+      </c>
+      <c r="X165">
+        <v>0.056865894469985</v>
+      </c>
+      <c r="Y165">
+        <v>0.06515880392868301</v>
+      </c>
+      <c r="Z165">
+        <v>0.06626948378514599</v>
+      </c>
+      <c r="AA165">
+        <v>0.064057379279614</v>
+      </c>
+      <c r="AB165">
+        <v>0.082546048902744</v>
+      </c>
+      <c r="AC165">
+        <v>0.12113095238095</v>
+      </c>
+      <c r="AD165">
+        <v>0.09717926610729399</v>
+      </c>
+      <c r="AE165">
+        <v>0.089893008810407</v>
+      </c>
+      <c r="AF165">
+        <v>0.080941994373339</v>
+      </c>
+      <c r="AG165">
+        <v>0.091392389036242</v>
+      </c>
+      <c r="AH165">
+        <v>0.088767550980847</v>
+      </c>
+      <c r="AI165">
+        <v>0.06701497405745201</v>
+      </c>
+      <c r="AJ165">
+        <v>0.062439855528944</v>
+      </c>
+      <c r="AK165">
+        <v>0.076176787049182</v>
+      </c>
+      <c r="AL165">
+        <v>0.0694377437276</v>
+      </c>
+      <c r="AM165">
+        <v>0.058626324709352</v>
+      </c>
+      <c r="AN165">
+        <v>0.073881907690242</v>
+      </c>
+      <c r="AO165">
+        <v>0.091495863695799</v>
+      </c>
+      <c r="AP165">
+        <v>0.07676357941034199</v>
+      </c>
+      <c r="AQ165">
+        <v>0.069688422597472</v>
+      </c>
+      <c r="AR165">
+        <v>0.052783842487489</v>
+      </c>
+      <c r="AS165">
+        <v>0.07361821317524</v>
+      </c>
+      <c r="AT165">
+        <v>0.09002512740320499</v>
+      </c>
+      <c r="AU165">
+        <v>0.09593282123791801</v>
+      </c>
+      <c r="AV165">
+        <v>0.089827418501487</v>
+      </c>
+      <c r="AW165">
+        <v>0.077449247638868</v>
+      </c>
+      <c r="AX165">
+        <v>0.089288614336421</v>
+      </c>
+      <c r="AY165">
+        <v>0.06914441968648601</v>
+      </c>
+      <c r="AZ165">
+        <v>0.079094075789321</v>
+      </c>
+      <c r="BA165">
+        <v>0.06716746307357099</v>
+      </c>
+      <c r="BB165">
+        <v>0.068695547558575</v>
+      </c>
+      <c r="BC165">
+        <v>0.071601375483986</v>
+      </c>
+      <c r="BD165">
+        <v>0.06911905701213999</v>
+      </c>
+      <c r="BE165">
+        <v>0.09575590473010399</v>
+      </c>
     </row>
     <row r="166" spans="1:57">
       <c r="A166" t="s">
         <v>220</v>
       </c>
+      <c r="B166">
+        <v>0.10990639625142</v>
+      </c>
+      <c r="C166">
+        <v>0.12784454130919</v>
+      </c>
+      <c r="D166">
+        <v>0.1041543102503</v>
+      </c>
+      <c r="F166">
+        <v>0.079721047461786</v>
+      </c>
+      <c r="G166">
+        <v>0.06975351892328301</v>
+      </c>
+      <c r="H166">
+        <v>0.08363888846669</v>
+      </c>
+      <c r="I166">
+        <v>0.07202457669781499</v>
+      </c>
+      <c r="J166">
+        <v>0.053059739874937</v>
+      </c>
+      <c r="K166">
+        <v>0.073843291437391</v>
+      </c>
+      <c r="L166">
+        <v>0.074563708475087</v>
+      </c>
+      <c r="M166">
+        <v>0.087951079837185</v>
+      </c>
+      <c r="N166">
+        <v>0.071108465572246</v>
+      </c>
+      <c r="O166">
+        <v>0.092275917652859</v>
+      </c>
+      <c r="P166">
+        <v>0.079689313243804</v>
+      </c>
+      <c r="Q166">
+        <v>0.09701505208014399</v>
+      </c>
+      <c r="R166">
+        <v>0.073300741610253</v>
+      </c>
+      <c r="S166">
+        <v>0.07931895762609099</v>
+      </c>
+      <c r="T166">
+        <v>0.08135903925141701</v>
+      </c>
+      <c r="U166">
+        <v>0.07609277446673</v>
+      </c>
+      <c r="V166">
+        <v>0.085795852240015</v>
+      </c>
+      <c r="W166">
+        <v>0.060715729670925</v>
+      </c>
+      <c r="X166">
+        <v>0.059647632998931</v>
+      </c>
+      <c r="Y166">
+        <v>0.06487323763792301</v>
+      </c>
+      <c r="Z166">
+        <v>0.071101654624792</v>
+      </c>
+      <c r="AA166">
+        <v>0.06598852170979801</v>
+      </c>
+      <c r="AB166">
+        <v>0.08574790310407999</v>
+      </c>
+      <c r="AC166">
+        <v>0.12606272812155</v>
+      </c>
+      <c r="AD166">
+        <v>0.10435722676736</v>
+      </c>
+      <c r="AE166">
+        <v>0.094928630285183</v>
+      </c>
+      <c r="AF166">
+        <v>0.086999170829711</v>
+      </c>
+      <c r="AG166">
+        <v>0.10037416487085</v>
+      </c>
+      <c r="AH166">
+        <v>0.091138282283092</v>
+      </c>
+      <c r="AI166">
+        <v>0.06648694914584</v>
+      </c>
+      <c r="AJ166">
+        <v>0.068137562922755</v>
+      </c>
+      <c r="AK166">
+        <v>0.074623589421111</v>
+      </c>
+      <c r="AL166">
+        <v>0.0696698021648</v>
+      </c>
+      <c r="AM166">
+        <v>0.06384008657154</v>
+      </c>
+      <c r="AN166">
+        <v>0.08140962355428499</v>
+      </c>
+      <c r="AO166">
+        <v>0.10089647639174</v>
+      </c>
+      <c r="AP166">
+        <v>0.084054479350108</v>
+      </c>
+      <c r="AQ166">
+        <v>0.074766585853803</v>
+      </c>
+      <c r="AR166">
+        <v>0.055017715532478</v>
+      </c>
+      <c r="AS166">
+        <v>0.073178510730892</v>
+      </c>
+      <c r="AT166">
+        <v>0.09224329954149001</v>
+      </c>
+      <c r="AU166">
+        <v>0.09317498203121501</v>
+      </c>
+      <c r="AV166">
+        <v>0.090788613691399</v>
+      </c>
+      <c r="AW166">
+        <v>0.076523797166571</v>
+      </c>
+      <c r="AX166">
+        <v>0.08837002058387</v>
+      </c>
+      <c r="AY166">
+        <v>0.070821034133445</v>
+      </c>
+      <c r="AZ166">
+        <v>0.081732081195076</v>
+      </c>
+      <c r="BA166">
+        <v>0.06508191767949401</v>
+      </c>
+      <c r="BB166">
+        <v>0.071134965086065</v>
+      </c>
+      <c r="BC166">
+        <v>0.070837722311476</v>
+      </c>
+      <c r="BD166">
+        <v>0.075711958204442</v>
+      </c>
+      <c r="BE166">
+        <v>0.10029608389581</v>
+      </c>
     </row>
     <row r="167" spans="1:57">
       <c r="A167" t="s">
         <v>221</v>
+      </c>
+      <c r="B167">
+        <v>0.074195742643827</v>
+      </c>
+      <c r="C167">
+        <v>0.10007420426689</v>
+      </c>
+      <c r="D167">
+        <v>0.09707257220043</v>
+      </c>
+      <c r="F167">
+        <v>0.066618868942434</v>
+      </c>
+      <c r="G167">
+        <v>0.074210808405474</v>
+      </c>
+      <c r="H167">
+        <v>0.08574625546178601</v>
+      </c>
+      <c r="I167">
+        <v>0.06941873671320301</v>
+      </c>
+      <c r="J167">
+        <v>0.050743240673257</v>
+      </c>
+      <c r="K167">
+        <v>0.070568708513377</v>
+      </c>
+      <c r="L167">
+        <v>0.07192823531407</v>
+      </c>
+      <c r="M167">
+        <v>0.08559476273821801</v>
+      </c>
+      <c r="N167">
+        <v>0.086331214078897</v>
+      </c>
+      <c r="O167">
+        <v>0.090019611754991</v>
+      </c>
+      <c r="P167">
+        <v>0.082596786750661</v>
+      </c>
+      <c r="Q167">
+        <v>0.09956588459015001</v>
+      </c>
+      <c r="R167">
+        <v>0.07262314963795501</v>
+      </c>
+      <c r="S167">
+        <v>0.080225153216867</v>
+      </c>
+      <c r="T167">
+        <v>0.084105935467674</v>
+      </c>
+      <c r="U167">
+        <v>0.079771485727696</v>
+      </c>
+      <c r="V167">
+        <v>0.09047869599455099</v>
+      </c>
+      <c r="W167">
+        <v>0.066732887701939</v>
+      </c>
+      <c r="X167">
+        <v>0.06397201606689901</v>
+      </c>
+      <c r="Y167">
+        <v>0.073806112915192</v>
+      </c>
+      <c r="Z167">
+        <v>0.072761692554508</v>
+      </c>
+      <c r="AA167">
+        <v>0.072421113871062</v>
+      </c>
+      <c r="AB167">
+        <v>0.082415412536615</v>
+      </c>
+      <c r="AC167">
+        <v>0.13436688311688</v>
+      </c>
+      <c r="AD167">
+        <v>0.1022767086071</v>
+      </c>
+      <c r="AE167">
+        <v>0.091659764343074</v>
+      </c>
+      <c r="AF167">
+        <v>0.085056774406918</v>
+      </c>
+      <c r="AG167">
+        <v>0.096354230213942</v>
+      </c>
+      <c r="AH167">
+        <v>0.089188643031165</v>
+      </c>
+      <c r="AI167">
+        <v>0.06777611713172001</v>
+      </c>
+      <c r="AJ167">
+        <v>0.06425772794783</v>
+      </c>
+      <c r="AK167">
+        <v>0.072894006706824</v>
+      </c>
+      <c r="AL167">
+        <v>0.06813033595583801</v>
+      </c>
+      <c r="AM167">
+        <v>0.062410334743582</v>
+      </c>
+      <c r="AN167">
+        <v>0.07702829936598</v>
+      </c>
+      <c r="AO167">
+        <v>0.096954585838116</v>
+      </c>
+      <c r="AP167">
+        <v>0.079348000175258</v>
+      </c>
+      <c r="AQ167">
+        <v>0.07064362694560899</v>
+      </c>
+      <c r="AR167">
+        <v>0.062105576144032</v>
+      </c>
+      <c r="AS167">
+        <v>0.06970322297216899</v>
+      </c>
+      <c r="AT167">
+        <v>0.09114091775023</v>
+      </c>
+      <c r="AU167">
+        <v>0.10025174482016</v>
+      </c>
+      <c r="AV167">
+        <v>0.09059512196896199</v>
+      </c>
+      <c r="AW167">
+        <v>0.080318804015343</v>
+      </c>
+      <c r="AX167">
+        <v>0.098060011643282</v>
+      </c>
+      <c r="AY167">
+        <v>0.076213058954491</v>
+      </c>
+      <c r="AZ167">
+        <v>0.09800378051068601</v>
+      </c>
+      <c r="BA167">
+        <v>0.072485273895061</v>
+      </c>
+      <c r="BB167">
+        <v>0.077984370368504</v>
+      </c>
+      <c r="BC167">
+        <v>0.075761057188745</v>
+      </c>
+      <c r="BD167">
+        <v>0.079997743263083</v>
+      </c>
+      <c r="BE167">
+        <v>0.10541946432686</v>
+      </c>
+    </row>
+    <row r="168" spans="1:57">
+      <c r="A168" t="s">
+        <v>222</v>
+      </c>
+      <c r="B168">
+        <v>0.096427354591913</v>
+      </c>
+      <c r="C168">
+        <v>0.1197601509534</v>
+      </c>
+      <c r="D168">
+        <v>0.11177047121803</v>
+      </c>
+      <c r="F168">
+        <v>0.078242073957833</v>
+      </c>
+      <c r="G168">
+        <v>0.084964145617409</v>
+      </c>
+      <c r="H168">
+        <v>0.082502505002285</v>
+      </c>
+      <c r="I168">
+        <v>0.06804215851979301</v>
+      </c>
+      <c r="J168">
+        <v>0.047572388431175</v>
+      </c>
+      <c r="K168">
+        <v>0.066764283442923</v>
+      </c>
+      <c r="L168">
+        <v>0.072369345231622</v>
+      </c>
+      <c r="M168">
+        <v>0.083233348105047</v>
+      </c>
+      <c r="N168">
+        <v>0.08091449377125801</v>
+      </c>
+      <c r="O168">
+        <v>0.08611171934105701</v>
+      </c>
+      <c r="P168">
+        <v>0.08769279293078899</v>
+      </c>
+      <c r="Q168">
+        <v>0.08742124626950901</v>
+      </c>
+      <c r="R168">
+        <v>0.066432789448697</v>
+      </c>
+      <c r="S168">
+        <v>0.075351404976344</v>
+      </c>
+      <c r="T168">
+        <v>0.08592268541749799</v>
+      </c>
+      <c r="U168">
+        <v>0.079466327567704</v>
+      </c>
+      <c r="V168">
+        <v>0.088211785164065</v>
+      </c>
+      <c r="W168">
+        <v>0.065200609561181</v>
+      </c>
+      <c r="X168">
+        <v>0.061483782083588</v>
+      </c>
+      <c r="Y168">
+        <v>0.07297915905492799</v>
+      </c>
+      <c r="Z168">
+        <v>0.065820418761803</v>
+      </c>
+      <c r="AA168">
+        <v>0.065436111524591</v>
+      </c>
+      <c r="AB168">
+        <v>0.081140409880728</v>
+      </c>
+      <c r="AC168">
+        <v>0.1593352354716</v>
+      </c>
+      <c r="AD168">
+        <v>0.09865639767636</v>
+      </c>
+      <c r="AE168">
+        <v>0.089257940109294</v>
+      </c>
+      <c r="AF168">
+        <v>0.082797543327968</v>
+      </c>
+      <c r="AG168">
+        <v>0.09292924267268</v>
+      </c>
+      <c r="AH168">
+        <v>0.090632856378336</v>
+      </c>
+      <c r="AI168">
+        <v>0.07066207276585</v>
+      </c>
+      <c r="AJ168">
+        <v>0.06583557017437799</v>
+      </c>
+      <c r="AK168">
+        <v>0.077921239286178</v>
+      </c>
+      <c r="AL168">
+        <v>0.066897940702519</v>
+      </c>
+      <c r="AM168">
+        <v>0.06337666110288701</v>
+      </c>
+      <c r="AN168">
+        <v>0.071602794562185</v>
+      </c>
+      <c r="AO168">
+        <v>0.09146549404875499</v>
+      </c>
+      <c r="AP168">
+        <v>0.071599297628933</v>
+      </c>
+      <c r="AQ168">
+        <v>0.061622199897816</v>
+      </c>
+      <c r="AR168">
+        <v>0.059388657875956</v>
+      </c>
+      <c r="AS168">
+        <v>0.066155266626611</v>
+      </c>
+      <c r="AT168">
+        <v>0.087018765224297</v>
+      </c>
+      <c r="AU168">
+        <v>0.092897375622208</v>
+      </c>
+      <c r="AV168">
+        <v>0.084669993959365</v>
+      </c>
+      <c r="AW168">
+        <v>0.076270704169788</v>
+      </c>
+      <c r="AX168">
+        <v>0.09166049922823501</v>
+      </c>
+      <c r="AY168">
+        <v>0.069854218655178</v>
+      </c>
+      <c r="AZ168">
+        <v>0.08151880684879501</v>
+      </c>
+      <c r="BA168">
+        <v>0.062217085819654</v>
+      </c>
+      <c r="BB168">
+        <v>0.069842324180119</v>
+      </c>
+      <c r="BC168">
+        <v>0.074305639573404</v>
+      </c>
+      <c r="BD168">
+        <v>0.07234304010723699</v>
+      </c>
+      <c r="BE168">
+        <v>0.098819677075087</v>
+      </c>
+    </row>
+    <row r="169" spans="1:57">
+      <c r="A169" t="s">
+        <v>223</v>
+      </c>
+      <c r="B169">
+        <v>0.057294170490318</v>
+      </c>
+      <c r="C169">
+        <v>0.08931989327985899</v>
+      </c>
+      <c r="D169">
+        <v>0.09363931775591899</v>
+      </c>
+      <c r="F169">
+        <v>0.057711488489476</v>
+      </c>
+      <c r="G169">
+        <v>0.072787610547955</v>
+      </c>
+      <c r="H169">
+        <v>0.075435049422743</v>
+      </c>
+      <c r="I169">
+        <v>0.059299640882405</v>
+      </c>
+      <c r="J169">
+        <v>0.049620923506569</v>
+      </c>
+      <c r="K169">
+        <v>0.06157240960739</v>
+      </c>
+      <c r="L169">
+        <v>0.069066719143727</v>
+      </c>
+      <c r="M169">
+        <v>0.08008360036734501</v>
+      </c>
+      <c r="N169">
+        <v>0.12408448413356</v>
+      </c>
+      <c r="O169">
+        <v>0.083213802202458</v>
+      </c>
+      <c r="P169">
+        <v>0.082661262066764</v>
+      </c>
+      <c r="Q169">
+        <v>0.082394612111083</v>
+      </c>
+      <c r="R169">
+        <v>0.06571417694997</v>
+      </c>
+      <c r="S169">
+        <v>0.073920339716827</v>
+      </c>
+      <c r="T169">
+        <v>0.083157902264959</v>
+      </c>
+      <c r="U169">
+        <v>0.078572360083132</v>
+      </c>
+      <c r="V169">
+        <v>0.091610214799083</v>
+      </c>
+      <c r="W169">
+        <v>0.072232598596339</v>
+      </c>
+      <c r="X169">
+        <v>0.06910207826145399</v>
+      </c>
+      <c r="Y169">
+        <v>0.07585382460267</v>
+      </c>
+      <c r="Z169">
+        <v>0.082034341912706</v>
+      </c>
+      <c r="AA169">
+        <v>0.071883083978799</v>
+      </c>
+      <c r="AB169">
+        <v>0.08975807578006501</v>
+      </c>
+      <c r="AC169">
+        <v>0.1277922843972</v>
+      </c>
+      <c r="AD169">
+        <v>0.10661829710997</v>
+      </c>
+      <c r="AE169">
+        <v>0.098241670617842</v>
+      </c>
+      <c r="AF169">
+        <v>0.086705414950886</v>
+      </c>
+      <c r="AG169">
+        <v>0.09011286919969499</v>
+      </c>
+      <c r="AH169">
+        <v>0.096724458043211</v>
+      </c>
+      <c r="AI169">
+        <v>0.075568325837834</v>
+      </c>
+      <c r="AJ169">
+        <v>0.06936386858988999</v>
+      </c>
+      <c r="AK169">
+        <v>0.085756378636672</v>
+      </c>
+      <c r="AL169">
+        <v>0.08008973512328101</v>
+      </c>
+      <c r="AM169">
+        <v>0.06949166288524999</v>
+      </c>
+      <c r="AN169">
+        <v>0.079047520732324</v>
+      </c>
+      <c r="AO169">
+        <v>0.096917659056987</v>
+      </c>
+      <c r="AP169">
+        <v>0.07982495784958001</v>
+      </c>
+      <c r="AQ169">
+        <v>0.069295500968676</v>
+      </c>
+      <c r="AR169">
+        <v>0.062276044363729</v>
+      </c>
+      <c r="AS169">
+        <v>0.071342754740367</v>
+      </c>
+      <c r="AT169">
+        <v>0.087594979670166</v>
+      </c>
+      <c r="AU169">
+        <v>0.093710644026747</v>
+      </c>
+      <c r="AV169">
+        <v>0.087645586983413</v>
+      </c>
+      <c r="AW169">
+        <v>0.077024814614139</v>
+      </c>
+      <c r="AX169">
+        <v>0.090707393145075</v>
+      </c>
+      <c r="AY169">
+        <v>0.071750993886786</v>
+      </c>
+      <c r="AZ169">
+        <v>0.095999944827691</v>
+      </c>
+      <c r="BA169">
+        <v>0.067496049423617</v>
+      </c>
+      <c r="BB169">
+        <v>0.072307232199185</v>
+      </c>
+      <c r="BC169">
+        <v>0.07436718168317399</v>
+      </c>
+      <c r="BD169">
+        <v>0.074865523670919</v>
+      </c>
+      <c r="BE169">
+        <v>0.099043927502874</v>
+      </c>
+    </row>
+    <row r="170" spans="1:57">
+      <c r="A170" t="s">
+        <v>224</v>
+      </c>
+      <c r="B170">
+        <v>0.056641666594487</v>
+      </c>
+      <c r="C170">
+        <v>0.07324112045199201</v>
+      </c>
+      <c r="D170">
+        <v>0.055975777455836</v>
+      </c>
+      <c r="F170">
+        <v>0.050120651001956</v>
+      </c>
+      <c r="G170">
+        <v>0.059985347963805</v>
+      </c>
+      <c r="H170">
+        <v>0.06378756827075401</v>
+      </c>
+      <c r="I170">
+        <v>0.053206203254912</v>
+      </c>
+      <c r="J170">
+        <v>0.044092568438982</v>
+      </c>
+      <c r="K170">
+        <v>0.051662705356349</v>
+      </c>
+      <c r="L170">
+        <v>0.047357001006383</v>
+      </c>
+      <c r="M170">
+        <v>0.054221425048864</v>
+      </c>
+      <c r="N170">
+        <v>0.098298535594286</v>
+      </c>
+      <c r="O170">
+        <v>0.057098258726681</v>
+      </c>
+      <c r="P170">
+        <v>0.064940199120439</v>
+      </c>
+      <c r="Q170">
+        <v>0.068504846735023</v>
+      </c>
+      <c r="R170">
+        <v>0.054779712535385</v>
+      </c>
+      <c r="S170">
+        <v>0.056534573865526</v>
+      </c>
+      <c r="T170">
+        <v>0.06043144886473</v>
+      </c>
+      <c r="U170">
+        <v>0.059647522487377</v>
+      </c>
+      <c r="V170">
+        <v>0.067978710635016</v>
+      </c>
+      <c r="W170">
+        <v>0.0672999508983</v>
+      </c>
+      <c r="X170">
+        <v>0.055688391946827</v>
+      </c>
+      <c r="Y170">
+        <v>0.066602466649342</v>
+      </c>
+      <c r="Z170">
+        <v>0.058206617014975</v>
+      </c>
+      <c r="AA170">
+        <v>0.049469455458282</v>
+      </c>
+      <c r="AB170">
+        <v>0.063686582470042</v>
+      </c>
+      <c r="AC170">
+        <v>0.12778580540967</v>
+      </c>
+      <c r="AD170">
+        <v>0.06843265159843399</v>
+      </c>
+      <c r="AE170">
+        <v>0.070364116477655</v>
+      </c>
+      <c r="AF170">
+        <v>0.058666392579753</v>
+      </c>
+      <c r="AG170">
+        <v>0.055785602476446</v>
+      </c>
+      <c r="AH170">
+        <v>0.065096393067202</v>
+      </c>
+      <c r="AI170">
+        <v>0.061907268232315</v>
+      </c>
+      <c r="AJ170">
+        <v>0.05754635348848</v>
+      </c>
+      <c r="AK170">
+        <v>0.065007500376549</v>
+      </c>
+      <c r="AL170">
+        <v>0.062080448330605</v>
+      </c>
+      <c r="AM170">
+        <v>0.057260514654409</v>
+      </c>
+      <c r="AN170">
+        <v>0.058367089490878</v>
+      </c>
+      <c r="AO170">
+        <v>0.062145890501375</v>
+      </c>
+      <c r="AP170">
+        <v>0.06301089486995499</v>
+      </c>
+      <c r="AQ170">
+        <v>0.057736324460772</v>
+      </c>
+      <c r="AR170">
+        <v>0.061103138335208</v>
+      </c>
+      <c r="AS170">
+        <v>0.064040922394175</v>
+      </c>
+      <c r="AT170">
+        <v>0.058433172082391</v>
+      </c>
+      <c r="AU170">
+        <v>0.066242476804156</v>
+      </c>
+      <c r="AV170">
+        <v>0.061916746147213</v>
+      </c>
+      <c r="AW170">
+        <v>0.052660458017649</v>
+      </c>
+      <c r="AX170">
+        <v>0.07420828527637099</v>
+      </c>
+      <c r="AY170">
+        <v>0.055424396076283</v>
+      </c>
+      <c r="AZ170">
+        <v>0.10981962839678</v>
+      </c>
+      <c r="BA170">
+        <v>0.06174908896516</v>
+      </c>
+      <c r="BB170">
+        <v>0.064488213376349</v>
+      </c>
+      <c r="BC170">
+        <v>0.06174581414946</v>
+      </c>
+      <c r="BD170">
+        <v>0.063998717491899</v>
+      </c>
+      <c r="BE170">
+        <v>0.08056479904981199</v>
+      </c>
+    </row>
+    <row r="171" spans="1:57">
+      <c r="A171" t="s">
+        <v>225</v>
+      </c>
+      <c r="B171">
+        <v>0.054603880241866</v>
+      </c>
+      <c r="C171">
+        <v>0.054396324722786</v>
+      </c>
+      <c r="D171">
+        <v>0.046885241691612</v>
+      </c>
+      <c r="F171">
+        <v>0.04629699042119</v>
+      </c>
+      <c r="G171">
+        <v>0.054839298778744</v>
+      </c>
+      <c r="H171">
+        <v>0.063294884156717</v>
+      </c>
+      <c r="I171">
+        <v>0.054981125326842</v>
+      </c>
+      <c r="J171">
+        <v>0.051846053652918</v>
+      </c>
+      <c r="K171">
+        <v>0.048959639251978</v>
+      </c>
+      <c r="L171">
+        <v>0.042811318877784</v>
+      </c>
+      <c r="M171">
+        <v>0.042940247331048</v>
+      </c>
+      <c r="N171">
+        <v>0.073111979450041</v>
+      </c>
+      <c r="O171">
+        <v>0.047157854897062</v>
+      </c>
+      <c r="P171">
+        <v>0.046102312533859</v>
+      </c>
+      <c r="Q171">
+        <v>0.054542959366413</v>
+      </c>
+      <c r="R171">
+        <v>0.039713762887762</v>
+      </c>
+      <c r="S171">
+        <v>0.042773575352385</v>
+      </c>
+      <c r="T171">
+        <v>0.043156319501804</v>
+      </c>
+      <c r="U171">
+        <v>0.046094583717653</v>
+      </c>
+      <c r="V171">
+        <v>0.049573770500195</v>
+      </c>
+      <c r="W171">
+        <v>0.054897742363939</v>
+      </c>
+      <c r="X171">
+        <v>0.040828927131395</v>
+      </c>
+      <c r="Y171">
+        <v>0.054266060192735</v>
+      </c>
+      <c r="Z171">
+        <v>0.041955098534167</v>
+      </c>
+      <c r="AA171">
+        <v>0.043479640790787</v>
+      </c>
+      <c r="AB171">
+        <v>0.052095956048892</v>
+      </c>
+      <c r="AC171">
+        <v>0.10494984706207</v>
+      </c>
+      <c r="AD171">
+        <v>0.052854872964836</v>
+      </c>
+      <c r="AE171">
+        <v>0.064801157942874</v>
+      </c>
+      <c r="AF171">
+        <v>0.050302374054402</v>
+      </c>
+      <c r="AG171">
+        <v>0.050844786933326</v>
+      </c>
+      <c r="AH171">
+        <v>0.049446131151078</v>
+      </c>
+      <c r="AI171">
+        <v>0.056581697134821</v>
+      </c>
+      <c r="AJ171">
+        <v>0.052176337596214</v>
+      </c>
+      <c r="AK171">
+        <v>0.056214582776985</v>
+      </c>
+      <c r="AL171">
+        <v>0.053216927221275</v>
+      </c>
+      <c r="AM171">
+        <v>0.051481995861715</v>
+      </c>
+      <c r="AN171">
+        <v>0.051641932202347</v>
+      </c>
+      <c r="AO171">
+        <v>0.055390655004779</v>
+      </c>
+      <c r="AP171">
+        <v>0.05720187934817</v>
+      </c>
+      <c r="AQ171">
+        <v>0.053195985600475</v>
+      </c>
+      <c r="AR171">
+        <v>0.041650435557012</v>
+      </c>
+      <c r="AS171">
+        <v>0.063761105444748</v>
+      </c>
+      <c r="AT171">
+        <v>0.05256899550567</v>
+      </c>
+      <c r="AU171">
+        <v>0.055128800584126</v>
+      </c>
+      <c r="AV171">
+        <v>0.051985913156353</v>
+      </c>
+      <c r="AW171">
+        <v>0.043762587753534</v>
+      </c>
+      <c r="AX171">
+        <v>0.058239320114721</v>
+      </c>
+      <c r="AY171">
+        <v>0.047894516244035</v>
+      </c>
+      <c r="AZ171">
+        <v>0.060903963582306</v>
+      </c>
+      <c r="BA171">
+        <v>0.053965897539903</v>
+      </c>
+      <c r="BB171">
+        <v>0.055514939156896</v>
+      </c>
+      <c r="BC171">
+        <v>0.049243555477996</v>
+      </c>
+      <c r="BD171">
+        <v>0.052243980888119</v>
+      </c>
+      <c r="BE171">
+        <v>0.062200197950817</v>
+      </c>
+    </row>
+    <row r="172" spans="1:57">
+      <c r="A172" t="s">
+        <v>226</v>
+      </c>
+      <c r="B172">
+        <v>0.071102401541992</v>
+      </c>
+      <c r="C172">
+        <v>0.09637351720392</v>
+      </c>
+      <c r="D172">
+        <v>0.1011830270438</v>
+      </c>
+      <c r="F172">
+        <v>0.06983112143025</v>
+      </c>
+      <c r="G172">
+        <v>0.071280119999731</v>
+      </c>
+      <c r="H172">
+        <v>0.08514215145655001</v>
+      </c>
+      <c r="I172">
+        <v>0.07077948044629</v>
+      </c>
+      <c r="J172">
+        <v>0.054850443983304</v>
+      </c>
+      <c r="K172">
+        <v>0.067229035066462</v>
+      </c>
+      <c r="L172">
+        <v>0.073148698823332</v>
+      </c>
+      <c r="M172">
+        <v>0.08747207870611</v>
+      </c>
+      <c r="N172">
+        <v>0.08027264586118001</v>
+      </c>
+      <c r="O172">
+        <v>0.09286210173342201</v>
+      </c>
+      <c r="P172">
+        <v>0.093704436316529</v>
+      </c>
+      <c r="Q172">
+        <v>0.098692325967092</v>
+      </c>
+      <c r="R172">
+        <v>0.075075474003682</v>
+      </c>
+      <c r="S172">
+        <v>0.084691280657792</v>
+      </c>
+      <c r="T172">
+        <v>0.090978861053267</v>
+      </c>
+      <c r="U172">
+        <v>0.08775679320906001</v>
+      </c>
+      <c r="V172">
+        <v>0.096423931674625</v>
+      </c>
+      <c r="W172">
+        <v>0.07296376793683</v>
+      </c>
+      <c r="X172">
+        <v>0.069304068842108</v>
+      </c>
+      <c r="Y172">
+        <v>0.083139965281589</v>
+      </c>
+      <c r="Z172">
+        <v>0.07517057967728701</v>
+      </c>
+      <c r="AA172">
+        <v>0.074420059278963</v>
+      </c>
+      <c r="AB172">
+        <v>0.081357283760876</v>
+      </c>
+      <c r="AC172">
+        <v>0.096040877544041</v>
+      </c>
+      <c r="AD172">
+        <v>0.10147103462537</v>
+      </c>
+      <c r="AE172">
+        <v>0.093542397353122</v>
+      </c>
+      <c r="AF172">
+        <v>0.080458509330757</v>
+      </c>
+      <c r="AG172">
+        <v>0.093524907284254</v>
+      </c>
+      <c r="AH172">
+        <v>0.09051606097072799</v>
+      </c>
+      <c r="AI172">
+        <v>0.071186176207806</v>
+      </c>
+      <c r="AJ172">
+        <v>0.065040206589684</v>
+      </c>
+      <c r="AK172">
+        <v>0.078829288381072</v>
+      </c>
+      <c r="AL172">
+        <v>0.068534803043877</v>
+      </c>
+      <c r="AM172">
+        <v>0.06219193485513</v>
+      </c>
+      <c r="AN172">
+        <v>0.071571883077216</v>
+      </c>
+      <c r="AO172">
+        <v>0.092972165319391</v>
+      </c>
+      <c r="AP172">
+        <v>0.07543703496561401</v>
+      </c>
+      <c r="AQ172">
+        <v>0.06532915163682899</v>
+      </c>
+      <c r="AR172">
+        <v>0.058699800156384</v>
+      </c>
+      <c r="AS172">
+        <v>0.06946571494040001</v>
+      </c>
+      <c r="AT172">
+        <v>0.086836461836463</v>
+      </c>
+      <c r="AU172">
+        <v>0.098283210044355</v>
+      </c>
+      <c r="AV172">
+        <v>0.08704255123776</v>
+      </c>
+      <c r="AW172">
+        <v>0.07507032690731801</v>
+      </c>
+      <c r="AX172">
+        <v>0.089708524140781</v>
+      </c>
+      <c r="AY172">
+        <v>0.06760336952107</v>
+      </c>
+      <c r="AZ172">
+        <v>0.08561089767501399</v>
+      </c>
+      <c r="BA172">
+        <v>0.062338573765324</v>
+      </c>
+      <c r="BB172">
+        <v>0.07062664491585199</v>
+      </c>
+      <c r="BC172">
+        <v>0.073681294107398</v>
+      </c>
+      <c r="BD172">
+        <v>0.072283401958322</v>
+      </c>
+      <c r="BE172">
+        <v>0.10161248207755</v>
+      </c>
+    </row>
+    <row r="173" spans="1:57">
+      <c r="A173" t="s">
+        <v>227</v>
+      </c>
+      <c r="B173">
+        <v>0.064567408058452</v>
+      </c>
+      <c r="C173">
+        <v>0.099936761065073</v>
+      </c>
+      <c r="D173">
+        <v>0.098323282254897</v>
+      </c>
+      <c r="F173">
+        <v>0.059858457047038</v>
+      </c>
+      <c r="G173">
+        <v>0.081598304007268</v>
+      </c>
+      <c r="H173">
+        <v>0.084588436261176</v>
+      </c>
+      <c r="I173">
+        <v>0.071007087985286</v>
+      </c>
+      <c r="J173">
+        <v>0.050093990263707</v>
+      </c>
+      <c r="K173">
+        <v>0.06808401902721301</v>
+      </c>
+      <c r="L173">
+        <v>0.072173861375691</v>
+      </c>
+      <c r="M173">
+        <v>0.08446782846384999</v>
+      </c>
+      <c r="N173">
+        <v>0.082868291059414</v>
+      </c>
+      <c r="O173">
+        <v>0.086016974356334</v>
+      </c>
+      <c r="P173">
+        <v>0.09340218110522699</v>
+      </c>
+      <c r="Q173">
+        <v>0.092157656251629</v>
+      </c>
+      <c r="R173">
+        <v>0.070881335910581</v>
+      </c>
+      <c r="S173">
+        <v>0.081497551921933</v>
+      </c>
+      <c r="T173">
+        <v>0.09027161142076399</v>
+      </c>
+      <c r="U173">
+        <v>0.084340058701607</v>
+      </c>
+      <c r="V173">
+        <v>0.093415228352644</v>
+      </c>
+      <c r="W173">
+        <v>0.072300478702195</v>
+      </c>
+      <c r="X173">
+        <v>0.065646219268519</v>
+      </c>
+      <c r="Y173">
+        <v>0.079961179331863</v>
+      </c>
+      <c r="Z173">
+        <v>0.073476129862557</v>
+      </c>
+      <c r="AA173">
+        <v>0.07031139228772</v>
+      </c>
+      <c r="AB173">
+        <v>0.084980012075906</v>
+      </c>
+      <c r="AC173">
+        <v>0.11427049567854</v>
+      </c>
+      <c r="AD173">
+        <v>0.10318526961086</v>
+      </c>
+      <c r="AE173">
+        <v>0.09679540379851501</v>
+      </c>
+      <c r="AF173">
+        <v>0.08669190158387299</v>
+      </c>
+      <c r="AG173">
+        <v>0.099841331843669</v>
+      </c>
+      <c r="AH173">
+        <v>0.096140588950942</v>
+      </c>
+      <c r="AI173">
+        <v>0.07712846954236199</v>
+      </c>
+      <c r="AJ173">
+        <v>0.07186418075866099</v>
+      </c>
+      <c r="AK173">
+        <v>0.08212772638938499</v>
+      </c>
+      <c r="AL173">
+        <v>0.072331339600107</v>
+      </c>
+      <c r="AM173">
+        <v>0.06773311173593199</v>
+      </c>
+      <c r="AN173">
+        <v>0.079927550882152</v>
+      </c>
+      <c r="AO173">
+        <v>0.10146793601781</v>
+      </c>
+      <c r="AP173">
+        <v>0.08413602258915</v>
+      </c>
+      <c r="AQ173">
+        <v>0.07421676795695099</v>
+      </c>
+      <c r="AR173">
+        <v>0.062460551070368</v>
+      </c>
+      <c r="AS173">
+        <v>0.07912582309786099</v>
+      </c>
+      <c r="AT173">
+        <v>0.094086871311057</v>
+      </c>
+      <c r="AU173">
+        <v>0.10358464145425</v>
+      </c>
+      <c r="AV173">
+        <v>0.09320379110572</v>
+      </c>
+      <c r="AW173">
+        <v>0.081577725349219</v>
+      </c>
+      <c r="AX173">
+        <v>0.098102790321207</v>
+      </c>
+      <c r="AY173">
+        <v>0.075158059369146</v>
+      </c>
+      <c r="AZ173">
+        <v>0.08932092281687801</v>
+      </c>
+      <c r="BA173">
+        <v>0.0783897392125</v>
+      </c>
+      <c r="BB173">
+        <v>0.07920582820840601</v>
+      </c>
+      <c r="BC173">
+        <v>0.08213944619097199</v>
+      </c>
+      <c r="BD173">
+        <v>0.083750118315949</v>
+      </c>
+      <c r="BE173">
+        <v>0.1079080748028</v>
+      </c>
+    </row>
+    <row r="174" spans="1:57">
+      <c r="A174" t="s">
+        <v>228</v>
+      </c>
+      <c r="B174">
+        <v>0.075608283078689</v>
+      </c>
+      <c r="C174">
+        <v>0.098292741838247</v>
+      </c>
+      <c r="D174">
+        <v>0.10168709730255</v>
+      </c>
+      <c r="F174">
+        <v>0.070619303383335</v>
+      </c>
+      <c r="G174">
+        <v>0.07777592615319</v>
+      </c>
+      <c r="H174">
+        <v>0.085394510977314</v>
+      </c>
+      <c r="I174">
+        <v>0.069714501537392</v>
+      </c>
+      <c r="J174">
+        <v>0.049547329944685</v>
+      </c>
+      <c r="K174">
+        <v>0.06914233934142899</v>
+      </c>
+      <c r="L174">
+        <v>0.074679994419535</v>
+      </c>
+      <c r="M174">
+        <v>0.08676019109238101</v>
+      </c>
+      <c r="N174">
+        <v>0.083779524061782</v>
+      </c>
+      <c r="O174">
+        <v>0.088837594930084</v>
+      </c>
+      <c r="P174">
+        <v>0.09959280574025001</v>
+      </c>
+      <c r="Q174">
+        <v>0.093898569029588</v>
+      </c>
+      <c r="R174">
+        <v>0.075251401000337</v>
+      </c>
+      <c r="S174">
+        <v>0.08465814828073</v>
+      </c>
+      <c r="T174">
+        <v>0.097784766205045</v>
+      </c>
+      <c r="U174">
+        <v>0.087461669525257</v>
+      </c>
+      <c r="V174">
+        <v>0.097272711182415</v>
+      </c>
+      <c r="W174">
+        <v>0.066236620619691</v>
+      </c>
+      <c r="X174">
+        <v>0.064975825521648</v>
+      </c>
+      <c r="Y174">
+        <v>0.077595935378518</v>
+      </c>
+      <c r="Z174">
+        <v>0.070809257016688</v>
+      </c>
+      <c r="AA174">
+        <v>0.07500282332903099</v>
+      </c>
+      <c r="AB174">
+        <v>0.088991576226605</v>
+      </c>
+      <c r="AC174">
+        <v>0.09745377244698</v>
+      </c>
+      <c r="AD174">
+        <v>0.10502543895217</v>
+      </c>
+      <c r="AE174">
+        <v>0.099694097276383</v>
+      </c>
+      <c r="AF174">
+        <v>0.086644542285279</v>
+      </c>
+      <c r="AG174">
+        <v>0.09805477980336599</v>
+      </c>
+      <c r="AH174">
+        <v>0.10202022650496</v>
+      </c>
+      <c r="AI174">
+        <v>0.078324744257429</v>
+      </c>
+      <c r="AJ174">
+        <v>0.0711806934189</v>
+      </c>
+      <c r="AK174">
+        <v>0.08792928462946099</v>
+      </c>
+      <c r="AL174">
+        <v>0.076827768115312</v>
+      </c>
+      <c r="AM174">
+        <v>0.067443128869922</v>
+      </c>
+      <c r="AN174">
+        <v>0.07285811016276</v>
+      </c>
+      <c r="AO174">
+        <v>0.09506512939200901</v>
+      </c>
+      <c r="AP174">
+        <v>0.075428239490464</v>
+      </c>
+      <c r="AQ174">
+        <v>0.06580648704080901</v>
+      </c>
+      <c r="AR174">
+        <v>0.059007857938793</v>
+      </c>
+      <c r="AS174">
+        <v>0.067508500894695</v>
+      </c>
+      <c r="AT174">
+        <v>0.090083986893054</v>
+      </c>
+      <c r="AU174">
+        <v>0.099264178068311</v>
+      </c>
+      <c r="AV174">
+        <v>0.088130664220856</v>
+      </c>
+      <c r="AW174">
+        <v>0.079160562678393</v>
+      </c>
+      <c r="AX174">
+        <v>0.08930679196382101</v>
+      </c>
+      <c r="AY174">
+        <v>0.06829402739278299</v>
+      </c>
+      <c r="AZ174">
+        <v>0.085556810743602</v>
+      </c>
+      <c r="BA174">
+        <v>0.06892631527731601</v>
+      </c>
+      <c r="BB174">
+        <v>0.069739808665986</v>
+      </c>
+      <c r="BC174">
+        <v>0.075425446348965</v>
+      </c>
+      <c r="BD174">
+        <v>0.07120550799709</v>
+      </c>
+      <c r="BE174">
+        <v>0.10116350429747</v>
+      </c>
+    </row>
+    <row r="175" spans="1:57">
+      <c r="A175" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="176" spans="1:57">
+      <c r="A176" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1">
+      <c r="A177" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1">
+      <c r="A178" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1">
+      <c r="A179" t="s">
+        <v>233</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data up to 5th
</commit_message>
<xml_diff>
--- a/away3-6hours.xlsx
+++ b/away3-6hours.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="243">
   <si>
     <t>Alaska</t>
   </si>
@@ -717,6 +717,33 @@
   <si>
     <t>27 07 2020</t>
   </si>
+  <si>
+    <t>28 07 2020</t>
+  </si>
+  <si>
+    <t>29 07 2020</t>
+  </si>
+  <si>
+    <t>30 07 2020</t>
+  </si>
+  <si>
+    <t>31 07 2020</t>
+  </si>
+  <si>
+    <t>01 08 2020</t>
+  </si>
+  <si>
+    <t>02 08 2020</t>
+  </si>
+  <si>
+    <t>03 08 2020</t>
+  </si>
+  <si>
+    <t>04 08 2020</t>
+  </si>
+  <si>
+    <t>05 08 2020</t>
+  </si>
 </sst>
 </file>
 
@@ -1047,7 +1074,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BE179"/>
+  <dimension ref="A1:BE188"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -14903,6 +14930,9 @@
       <c r="D81">
         <v>0.07659710020492599</v>
       </c>
+      <c r="E81">
+        <v>0.087037037037037</v>
+      </c>
       <c r="F81">
         <v>0.058608730579851</v>
       </c>
@@ -15073,6 +15103,9 @@
       <c r="D82">
         <v>0.08722700864938999</v>
       </c>
+      <c r="E82">
+        <v>0.18799603174603</v>
+      </c>
       <c r="F82">
         <v>0.059742693526136</v>
       </c>
@@ -15243,6 +15276,9 @@
       <c r="D83">
         <v>0.066716435879489</v>
       </c>
+      <c r="E83">
+        <v>0.10355616605617</v>
+      </c>
       <c r="F83">
         <v>0.053458300834484</v>
       </c>
@@ -15413,6 +15449,9 @@
       <c r="D84">
         <v>0.082573362766321</v>
       </c>
+      <c r="E84">
+        <v>0.12984848484848</v>
+      </c>
       <c r="F84">
         <v>0.076137582865783</v>
       </c>
@@ -15583,6 +15622,9 @@
       <c r="D85">
         <v>0.084403868586855</v>
       </c>
+      <c r="E85">
+        <v>0.14384920634921</v>
+      </c>
       <c r="F85">
         <v>0.07162019712508</v>
       </c>
@@ -15753,6 +15795,9 @@
       <c r="D86">
         <v>0.057395881560666</v>
       </c>
+      <c r="E86">
+        <v>0.12917756846328</v>
+      </c>
       <c r="F86">
         <v>0.055813385408535</v>
       </c>
@@ -15923,6 +15968,9 @@
       <c r="D87">
         <v>0.041564272619337</v>
       </c>
+      <c r="E87">
+        <v>0.12136243386243</v>
+      </c>
       <c r="F87">
         <v>0.049728382657919</v>
       </c>
@@ -16093,6 +16141,9 @@
       <c r="D88">
         <v>0.087788617107841</v>
       </c>
+      <c r="E88">
+        <v>0.17564033189033</v>
+      </c>
       <c r="F88">
         <v>0.06447697846252599</v>
       </c>
@@ -16263,6 +16314,9 @@
       <c r="D89">
         <v>0.084200400219914</v>
       </c>
+      <c r="E89">
+        <v>0.16615646258503</v>
+      </c>
       <c r="F89">
         <v>0.061809252833454</v>
       </c>
@@ -30874,25 +30928,1555 @@
       <c r="A175" t="s">
         <v>229</v>
       </c>
+      <c r="B175">
+        <v>0.091458246866035</v>
+      </c>
+      <c r="C175">
+        <v>0.10042257685039</v>
+      </c>
+      <c r="D175">
+        <v>0.09680995635166099</v>
+      </c>
+      <c r="F175">
+        <v>0.074771340577754</v>
+      </c>
+      <c r="G175">
+        <v>0.067215194661626</v>
+      </c>
+      <c r="H175">
+        <v>0.089073050468453</v>
+      </c>
+      <c r="I175">
+        <v>0.071598583733389</v>
+      </c>
+      <c r="J175">
+        <v>0.055634538656747</v>
+      </c>
+      <c r="K175">
+        <v>0.072600890483504</v>
+      </c>
+      <c r="L175">
+        <v>0.07714013979143899</v>
+      </c>
+      <c r="M175">
+        <v>0.092183696335009</v>
+      </c>
+      <c r="N175">
+        <v>0.072720186192856</v>
+      </c>
+      <c r="O175">
+        <v>0.09628424533141899</v>
+      </c>
+      <c r="P175">
+        <v>0.097966157822363</v>
+      </c>
+      <c r="Q175">
+        <v>0.09686071777861199</v>
+      </c>
+      <c r="R175">
+        <v>0.080045219985991</v>
+      </c>
+      <c r="S175">
+        <v>0.087775064435762</v>
+      </c>
+      <c r="T175">
+        <v>0.097006976641496</v>
+      </c>
+      <c r="U175">
+        <v>0.082884916344689</v>
+      </c>
+      <c r="V175">
+        <v>0.09302791923606001</v>
+      </c>
+      <c r="W175">
+        <v>0.06663561530437299</v>
+      </c>
+      <c r="X175">
+        <v>0.064391088046493</v>
+      </c>
+      <c r="Y175">
+        <v>0.07407183215014899</v>
+      </c>
+      <c r="Z175">
+        <v>0.076162848351707</v>
+      </c>
+      <c r="AA175">
+        <v>0.078567607714185</v>
+      </c>
+      <c r="AB175">
+        <v>0.093245118598415</v>
+      </c>
+      <c r="AC175">
+        <v>0.08881613136027899</v>
+      </c>
+      <c r="AD175">
+        <v>0.10979603655837</v>
+      </c>
+      <c r="AE175">
+        <v>0.10043062019695</v>
+      </c>
+      <c r="AF175">
+        <v>0.085950742897552</v>
+      </c>
+      <c r="AG175">
+        <v>0.09290511787446901</v>
+      </c>
+      <c r="AH175">
+        <v>0.10568370799549</v>
+      </c>
+      <c r="AI175">
+        <v>0.079227624486431</v>
+      </c>
+      <c r="AJ175">
+        <v>0.070767919557579</v>
+      </c>
+      <c r="AK175">
+        <v>0.089247745762015</v>
+      </c>
+      <c r="AL175">
+        <v>0.07805874490469999</v>
+      </c>
+      <c r="AM175">
+        <v>0.06688337706339501</v>
+      </c>
+      <c r="AN175">
+        <v>0.073602318210729</v>
+      </c>
+      <c r="AO175">
+        <v>0.096364267465232</v>
+      </c>
+      <c r="AP175">
+        <v>0.075028169748834</v>
+      </c>
+      <c r="AQ175">
+        <v>0.06497732355201701</v>
+      </c>
+      <c r="AR175">
+        <v>0.060164775728839</v>
+      </c>
+      <c r="AS175">
+        <v>0.067857999236765</v>
+      </c>
+      <c r="AT175">
+        <v>0.08861872769467501</v>
+      </c>
+      <c r="AU175">
+        <v>0.097094351475772</v>
+      </c>
+      <c r="AV175">
+        <v>0.087322919050363</v>
+      </c>
+      <c r="AW175">
+        <v>0.079958228738382</v>
+      </c>
+      <c r="AX175">
+        <v>0.091024054455201</v>
+      </c>
+      <c r="AY175">
+        <v>0.06949551218977899</v>
+      </c>
+      <c r="AZ175">
+        <v>0.07662552917852</v>
+      </c>
+      <c r="BA175">
+        <v>0.06782380048935401</v>
+      </c>
+      <c r="BB175">
+        <v>0.069177200819483</v>
+      </c>
+      <c r="BC175">
+        <v>0.073545015665007</v>
+      </c>
+      <c r="BD175">
+        <v>0.068726323513329</v>
+      </c>
+      <c r="BE175">
+        <v>0.09880258697587301</v>
+      </c>
     </row>
     <row r="176" spans="1:57">
       <c r="A176" t="s">
         <v>230</v>
       </c>
+      <c r="B176">
+        <v>0.083608277548819</v>
+      </c>
+      <c r="C176">
+        <v>0.09150707884403</v>
+      </c>
+      <c r="D176">
+        <v>0.11143856653526</v>
+      </c>
+      <c r="F176">
+        <v>0.07968853927856601</v>
+      </c>
+      <c r="G176">
+        <v>0.07507391313392001</v>
+      </c>
+      <c r="H176">
+        <v>0.071934786829656</v>
+      </c>
+      <c r="I176">
+        <v>0.05990377586319</v>
+      </c>
+      <c r="J176">
+        <v>0.053809093976966</v>
+      </c>
+      <c r="K176">
+        <v>0.05668448722743</v>
+      </c>
+      <c r="L176">
+        <v>0.07229180217664199</v>
+      </c>
+      <c r="M176">
+        <v>0.08411645904968799</v>
+      </c>
+      <c r="N176">
+        <v>0.082066656067487</v>
+      </c>
+      <c r="O176">
+        <v>0.086048284362345</v>
+      </c>
+      <c r="P176">
+        <v>0.09150647285911</v>
+      </c>
+      <c r="Q176">
+        <v>0.089813869398397</v>
+      </c>
+      <c r="R176">
+        <v>0.072652700131403</v>
+      </c>
+      <c r="S176">
+        <v>0.083387118636611</v>
+      </c>
+      <c r="T176">
+        <v>0.089278665276065</v>
+      </c>
+      <c r="U176">
+        <v>0.080273085762296</v>
+      </c>
+      <c r="V176">
+        <v>0.08691075499432301</v>
+      </c>
+      <c r="W176">
+        <v>0.063356263237433</v>
+      </c>
+      <c r="X176">
+        <v>0.058688518498149</v>
+      </c>
+      <c r="Y176">
+        <v>0.074135407473406</v>
+      </c>
+      <c r="Z176">
+        <v>0.067328806321329</v>
+      </c>
+      <c r="AA176">
+        <v>0.065846532816912</v>
+      </c>
+      <c r="AB176">
+        <v>0.08257526925246</v>
+      </c>
+      <c r="AC176">
+        <v>0.10087415592616</v>
+      </c>
+      <c r="AD176">
+        <v>0.095298201846771</v>
+      </c>
+      <c r="AE176">
+        <v>0.086671382183617</v>
+      </c>
+      <c r="AF176">
+        <v>0.083914331743544</v>
+      </c>
+      <c r="AG176">
+        <v>0.09139996673209499</v>
+      </c>
+      <c r="AH176">
+        <v>0.090653438975573</v>
+      </c>
+      <c r="AI176">
+        <v>0.073325778147564</v>
+      </c>
+      <c r="AJ176">
+        <v>0.06422609670520001</v>
+      </c>
+      <c r="AK176">
+        <v>0.083701526221063</v>
+      </c>
+      <c r="AL176">
+        <v>0.072097874343571</v>
+      </c>
+      <c r="AM176">
+        <v>0.067745004570075</v>
+      </c>
+      <c r="AN176">
+        <v>0.07933430639035099</v>
+      </c>
+      <c r="AO176">
+        <v>0.096873653626395</v>
+      </c>
+      <c r="AP176">
+        <v>0.080655678221842</v>
+      </c>
+      <c r="AQ176">
+        <v>0.070713977174393</v>
+      </c>
+      <c r="AR176">
+        <v>0.06818068278110299</v>
+      </c>
+      <c r="AS176">
+        <v>0.07678882637199699</v>
+      </c>
+      <c r="AT176">
+        <v>0.090164414013438</v>
+      </c>
+      <c r="AU176">
+        <v>0.096469793436034</v>
+      </c>
+      <c r="AV176">
+        <v>0.089905380924806</v>
+      </c>
+      <c r="AW176">
+        <v>0.079739328539945</v>
+      </c>
+      <c r="AX176">
+        <v>0.08372972816589</v>
+      </c>
+      <c r="AY176">
+        <v>0.073234037681613</v>
+      </c>
+      <c r="AZ176">
+        <v>0.10085549287963</v>
+      </c>
+      <c r="BA176">
+        <v>0.07779629987176399</v>
+      </c>
+      <c r="BB176">
+        <v>0.07682486876627601</v>
+      </c>
+      <c r="BC176">
+        <v>0.08015450137017301</v>
+      </c>
+      <c r="BD176">
+        <v>0.07908229077236301</v>
+      </c>
+      <c r="BE176">
+        <v>0.10585063327043</v>
+      </c>
     </row>
-    <row r="177" spans="1:1">
+    <row r="177" spans="1:57">
       <c r="A177" t="s">
         <v>231</v>
       </c>
+      <c r="B177">
+        <v>0.052744959059107</v>
+      </c>
+      <c r="C177">
+        <v>0.061204150489061</v>
+      </c>
+      <c r="D177">
+        <v>0.069712963631926</v>
+      </c>
+      <c r="F177">
+        <v>0.061393284392912</v>
+      </c>
+      <c r="G177">
+        <v>0.06798350396995501</v>
+      </c>
+      <c r="H177">
+        <v>0.078392517139631</v>
+      </c>
+      <c r="I177">
+        <v>0.06297368658897499</v>
+      </c>
+      <c r="J177">
+        <v>0.054394798736857</v>
+      </c>
+      <c r="K177">
+        <v>0.057562636004518</v>
+      </c>
+      <c r="L177">
+        <v>0.05439713562791</v>
+      </c>
+      <c r="M177">
+        <v>0.055418933529331</v>
+      </c>
+      <c r="N177">
+        <v>0.067139892425961</v>
+      </c>
+      <c r="O177">
+        <v>0.055316371528026</v>
+      </c>
+      <c r="P177">
+        <v>0.06379396231803799</v>
+      </c>
+      <c r="Q177">
+        <v>0.07242800000466799</v>
+      </c>
+      <c r="R177">
+        <v>0.05717056821124</v>
+      </c>
+      <c r="S177">
+        <v>0.056304571256359</v>
+      </c>
+      <c r="T177">
+        <v>0.059086330563379</v>
+      </c>
+      <c r="U177">
+        <v>0.054059195554318</v>
+      </c>
+      <c r="V177">
+        <v>0.055855303481789</v>
+      </c>
+      <c r="W177">
+        <v>0.058246196738494</v>
+      </c>
+      <c r="X177">
+        <v>0.048710430648845</v>
+      </c>
+      <c r="Y177">
+        <v>0.060040376229633</v>
+      </c>
+      <c r="Z177">
+        <v>0.055795980396908</v>
+      </c>
+      <c r="AA177">
+        <v>0.051383494084837</v>
+      </c>
+      <c r="AB177">
+        <v>0.064758562740897</v>
+      </c>
+      <c r="AC177">
+        <v>0.092742949877004</v>
+      </c>
+      <c r="AD177">
+        <v>0.062701445737568</v>
+      </c>
+      <c r="AE177">
+        <v>0.077091115848994</v>
+      </c>
+      <c r="AF177">
+        <v>0.061392562844317</v>
+      </c>
+      <c r="AG177">
+        <v>0.061563045215078</v>
+      </c>
+      <c r="AH177">
+        <v>0.067883682010281</v>
+      </c>
+      <c r="AI177">
+        <v>0.062638227918798</v>
+      </c>
+      <c r="AJ177">
+        <v>0.059511816621017</v>
+      </c>
+      <c r="AK177">
+        <v>0.069384070170177</v>
+      </c>
+      <c r="AL177">
+        <v>0.063385028592388</v>
+      </c>
+      <c r="AM177">
+        <v>0.059682699085214</v>
+      </c>
+      <c r="AN177">
+        <v>0.061146821329705</v>
+      </c>
+      <c r="AO177">
+        <v>0.06480682185617199</v>
+      </c>
+      <c r="AP177">
+        <v>0.065288426558634</v>
+      </c>
+      <c r="AQ177">
+        <v>0.058037775405992</v>
+      </c>
+      <c r="AR177">
+        <v>0.056661981165989</v>
+      </c>
+      <c r="AS177">
+        <v>0.064622077324406</v>
+      </c>
+      <c r="AT177">
+        <v>0.060125288376589</v>
+      </c>
+      <c r="AU177">
+        <v>0.067176777056944</v>
+      </c>
+      <c r="AV177">
+        <v>0.062286223622527</v>
+      </c>
+      <c r="AW177">
+        <v>0.051737011719378</v>
+      </c>
+      <c r="AX177">
+        <v>0.072578436512529</v>
+      </c>
+      <c r="AY177">
+        <v>0.052954424881212</v>
+      </c>
+      <c r="AZ177">
+        <v>0.073314529212195</v>
+      </c>
+      <c r="BA177">
+        <v>0.058028322234728</v>
+      </c>
+      <c r="BB177">
+        <v>0.059762073309151</v>
+      </c>
+      <c r="BC177">
+        <v>0.058952030940848</v>
+      </c>
+      <c r="BD177">
+        <v>0.053589786265902</v>
+      </c>
+      <c r="BE177">
+        <v>0.07442092788271</v>
+      </c>
     </row>
-    <row r="178" spans="1:1">
+    <row r="178" spans="1:57">
       <c r="A178" t="s">
         <v>232</v>
       </c>
+      <c r="B178">
+        <v>0.051311151461459</v>
+      </c>
+      <c r="C178">
+        <v>0.051754981251809</v>
+      </c>
+      <c r="D178">
+        <v>0.050156016070014</v>
+      </c>
+      <c r="F178">
+        <v>0.047565755632083</v>
+      </c>
+      <c r="G178">
+        <v>0.050886163884279</v>
+      </c>
+      <c r="H178">
+        <v>0.06290978738153299</v>
+      </c>
+      <c r="I178">
+        <v>0.056037434303138</v>
+      </c>
+      <c r="J178">
+        <v>0.052515581859876</v>
+      </c>
+      <c r="K178">
+        <v>0.054558921063099</v>
+      </c>
+      <c r="L178">
+        <v>0.048031617577904</v>
+      </c>
+      <c r="M178">
+        <v>0.049903620711082</v>
+      </c>
+      <c r="N178">
+        <v>0.07793455120579899</v>
+      </c>
+      <c r="O178">
+        <v>0.042927575280842</v>
+      </c>
+      <c r="P178">
+        <v>0.051262559871176</v>
+      </c>
+      <c r="Q178">
+        <v>0.063934527235861</v>
+      </c>
+      <c r="R178">
+        <v>0.05356021663805</v>
+      </c>
+      <c r="S178">
+        <v>0.053082401921519</v>
+      </c>
+      <c r="T178">
+        <v>0.052405692469722</v>
+      </c>
+      <c r="U178">
+        <v>0.050641287416225</v>
+      </c>
+      <c r="V178">
+        <v>0.052164487420802</v>
+      </c>
+      <c r="W178">
+        <v>0.061041315271449</v>
+      </c>
+      <c r="X178">
+        <v>0.047933879430957</v>
+      </c>
+      <c r="Y178">
+        <v>0.05761019457534</v>
+      </c>
+      <c r="Z178">
+        <v>0.053218423201051</v>
+      </c>
+      <c r="AA178">
+        <v>0.047570361314616</v>
+      </c>
+      <c r="AB178">
+        <v>0.058443963743702</v>
+      </c>
+      <c r="AC178">
+        <v>0.10643096328391</v>
+      </c>
+      <c r="AD178">
+        <v>0.054862874218741</v>
+      </c>
+      <c r="AE178">
+        <v>0.071692768226394</v>
+      </c>
+      <c r="AF178">
+        <v>0.048452133178397</v>
+      </c>
+      <c r="AG178">
+        <v>0.049954093580638</v>
+      </c>
+      <c r="AH178">
+        <v>0.05423270308626</v>
+      </c>
+      <c r="AI178">
+        <v>0.060289760017985</v>
+      </c>
+      <c r="AJ178">
+        <v>0.054021929038148</v>
+      </c>
+      <c r="AK178">
+        <v>0.060589406378004</v>
+      </c>
+      <c r="AL178">
+        <v>0.05573260856009</v>
+      </c>
+      <c r="AM178">
+        <v>0.05181806525602</v>
+      </c>
+      <c r="AN178">
+        <v>0.049645846522928</v>
+      </c>
+      <c r="AO178">
+        <v>0.052671274247593</v>
+      </c>
+      <c r="AP178">
+        <v>0.055577648214957</v>
+      </c>
+      <c r="AQ178">
+        <v>0.052357690178505</v>
+      </c>
+      <c r="AR178">
+        <v>0.051682471175521</v>
+      </c>
+      <c r="AS178">
+        <v>0.062516921006219</v>
+      </c>
+      <c r="AT178">
+        <v>0.054938422624171</v>
+      </c>
+      <c r="AU178">
+        <v>0.055488445347852</v>
+      </c>
+      <c r="AV178">
+        <v>0.05455786996013</v>
+      </c>
+      <c r="AW178">
+        <v>0.044161417860077</v>
+      </c>
+      <c r="AX178">
+        <v>0.059795236001822</v>
+      </c>
+      <c r="AY178">
+        <v>0.049738379515533</v>
+      </c>
+      <c r="AZ178">
+        <v>0.060491779164767</v>
+      </c>
+      <c r="BA178">
+        <v>0.055916847828756</v>
+      </c>
+      <c r="BB178">
+        <v>0.056943906193513</v>
+      </c>
+      <c r="BC178">
+        <v>0.051736839974124</v>
+      </c>
+      <c r="BD178">
+        <v>0.052980833646452</v>
+      </c>
+      <c r="BE178">
+        <v>0.06834307050739299</v>
+      </c>
     </row>
-    <row r="179" spans="1:1">
+    <row r="179" spans="1:57">
       <c r="A179" t="s">
         <v>233</v>
+      </c>
+      <c r="B179">
+        <v>0.059274606625541</v>
+      </c>
+      <c r="C179">
+        <v>0.09052163817485</v>
+      </c>
+      <c r="D179">
+        <v>0.092770028359831</v>
+      </c>
+      <c r="F179">
+        <v>0.057629914988337</v>
+      </c>
+      <c r="G179">
+        <v>0.077642594931825</v>
+      </c>
+      <c r="H179">
+        <v>0.081302410006498</v>
+      </c>
+      <c r="I179">
+        <v>0.06822828731799099</v>
+      </c>
+      <c r="J179">
+        <v>0.053038958209052</v>
+      </c>
+      <c r="K179">
+        <v>0.068724170653243</v>
+      </c>
+      <c r="L179">
+        <v>0.070303446925343</v>
+      </c>
+      <c r="M179">
+        <v>0.08686008117867999</v>
+      </c>
+      <c r="N179">
+        <v>0.081831977435354</v>
+      </c>
+      <c r="O179">
+        <v>0.071333352770706</v>
+      </c>
+      <c r="P179">
+        <v>0.09185603636876701</v>
+      </c>
+      <c r="Q179">
+        <v>0.09138097244799</v>
+      </c>
+      <c r="R179">
+        <v>0.06966386061251199</v>
+      </c>
+      <c r="S179">
+        <v>0.082124749780008</v>
+      </c>
+      <c r="T179">
+        <v>0.091374370139212</v>
+      </c>
+      <c r="U179">
+        <v>0.08654990431317</v>
+      </c>
+      <c r="V179">
+        <v>0.09578554278081</v>
+      </c>
+      <c r="W179">
+        <v>0.083853497628733</v>
+      </c>
+      <c r="X179">
+        <v>0.07316266213452401</v>
+      </c>
+      <c r="Y179">
+        <v>0.083895936665433</v>
+      </c>
+      <c r="Z179">
+        <v>0.082701685909182</v>
+      </c>
+      <c r="AA179">
+        <v>0.08141851597289899</v>
+      </c>
+      <c r="AB179">
+        <v>0.090101347176498</v>
+      </c>
+      <c r="AC179">
+        <v>0.096348643684038</v>
+      </c>
+      <c r="AD179">
+        <v>0.10838841643289</v>
+      </c>
+      <c r="AE179">
+        <v>0.1037275126138</v>
+      </c>
+      <c r="AF179">
+        <v>0.09060012935326101</v>
+      </c>
+      <c r="AG179">
+        <v>0.10211817891198</v>
+      </c>
+      <c r="AH179">
+        <v>0.10318681944994</v>
+      </c>
+      <c r="AI179">
+        <v>0.082856121512386</v>
+      </c>
+      <c r="AJ179">
+        <v>0.074432042652974</v>
+      </c>
+      <c r="AK179">
+        <v>0.090756607608036</v>
+      </c>
+      <c r="AL179">
+        <v>0.076824685345651</v>
+      </c>
+      <c r="AM179">
+        <v>0.075072220700904</v>
+      </c>
+      <c r="AN179">
+        <v>0.079102410967512</v>
+      </c>
+      <c r="AO179">
+        <v>0.09829058577272699</v>
+      </c>
+      <c r="AP179">
+        <v>0.077090295701225</v>
+      </c>
+      <c r="AQ179">
+        <v>0.06879544610431899</v>
+      </c>
+      <c r="AR179">
+        <v>0.073075412151086</v>
+      </c>
+      <c r="AS179">
+        <v>0.072975885974511</v>
+      </c>
+      <c r="AT179">
+        <v>0.088749038386917</v>
+      </c>
+      <c r="AU179">
+        <v>0.09724174203795399</v>
+      </c>
+      <c r="AV179">
+        <v>0.08707435008582801</v>
+      </c>
+      <c r="AW179">
+        <v>0.077028303553418</v>
+      </c>
+      <c r="AX179">
+        <v>0.091593457007939</v>
+      </c>
+      <c r="AY179">
+        <v>0.07142437529029901</v>
+      </c>
+      <c r="AZ179">
+        <v>0.10158957410487</v>
+      </c>
+      <c r="BA179">
+        <v>0.066857620519701</v>
+      </c>
+      <c r="BB179">
+        <v>0.073964552049556</v>
+      </c>
+      <c r="BC179">
+        <v>0.077803054065833</v>
+      </c>
+      <c r="BD179">
+        <v>0.075786101564519</v>
+      </c>
+      <c r="BE179">
+        <v>0.10848506034686</v>
+      </c>
+    </row>
+    <row r="180" spans="1:57">
+      <c r="A180" t="s">
+        <v>234</v>
+      </c>
+      <c r="B180">
+        <v>0.067122999809183</v>
+      </c>
+      <c r="C180">
+        <v>0.10285509805388</v>
+      </c>
+      <c r="D180">
+        <v>0.10113355677104</v>
+      </c>
+      <c r="F180">
+        <v>0.063041226052097</v>
+      </c>
+      <c r="G180">
+        <v>0.072220001940992</v>
+      </c>
+      <c r="H180">
+        <v>0.07891803027059301</v>
+      </c>
+      <c r="I180">
+        <v>0.067860073672754</v>
+      </c>
+      <c r="J180">
+        <v>0.057524270310794</v>
+      </c>
+      <c r="K180">
+        <v>0.069021808248835</v>
+      </c>
+      <c r="L180">
+        <v>0.07585026861638799</v>
+      </c>
+      <c r="M180">
+        <v>0.091859645254214</v>
+      </c>
+      <c r="N180">
+        <v>0.11634179370084</v>
+      </c>
+      <c r="O180">
+        <v>0.090940358977482</v>
+      </c>
+      <c r="P180">
+        <v>0.09107504011658001</v>
+      </c>
+      <c r="Q180">
+        <v>0.10195267924879</v>
+      </c>
+      <c r="R180">
+        <v>0.077643547231416</v>
+      </c>
+      <c r="S180">
+        <v>0.084171905012929</v>
+      </c>
+      <c r="T180">
+        <v>0.09126995507623301</v>
+      </c>
+      <c r="U180">
+        <v>0.08007715665524801</v>
+      </c>
+      <c r="V180">
+        <v>0.09050294013056399</v>
+      </c>
+      <c r="W180">
+        <v>0.070984536404093</v>
+      </c>
+      <c r="X180">
+        <v>0.065412432688759</v>
+      </c>
+      <c r="Y180">
+        <v>0.07396705257065</v>
+      </c>
+      <c r="Z180">
+        <v>0.08042879056751299</v>
+      </c>
+      <c r="AA180">
+        <v>0.08167554851467</v>
+      </c>
+      <c r="AB180">
+        <v>0.0935306885145</v>
+      </c>
+      <c r="AC180">
+        <v>0.13490266757174</v>
+      </c>
+      <c r="AD180">
+        <v>0.10995309798214</v>
+      </c>
+      <c r="AE180">
+        <v>0.10346273433232</v>
+      </c>
+      <c r="AF180">
+        <v>0.08335789431724901</v>
+      </c>
+      <c r="AG180">
+        <v>0.098368969566031</v>
+      </c>
+      <c r="AH180">
+        <v>0.10198467294568</v>
+      </c>
+      <c r="AI180">
+        <v>0.07770035044172099</v>
+      </c>
+      <c r="AJ180">
+        <v>0.072209488218162</v>
+      </c>
+      <c r="AK180">
+        <v>0.085533965250343</v>
+      </c>
+      <c r="AL180">
+        <v>0.078705006873994</v>
+      </c>
+      <c r="AM180">
+        <v>0.064805419352995</v>
+      </c>
+      <c r="AN180">
+        <v>0.07558800704134599</v>
+      </c>
+      <c r="AO180">
+        <v>0.096219613078284</v>
+      </c>
+      <c r="AP180">
+        <v>0.08018893056010799</v>
+      </c>
+      <c r="AQ180">
+        <v>0.07142003268128901</v>
+      </c>
+      <c r="AR180">
+        <v>0.054798239882338</v>
+      </c>
+      <c r="AS180">
+        <v>0.07708505086522401</v>
+      </c>
+      <c r="AT180">
+        <v>0.09426403142362599</v>
+      </c>
+      <c r="AU180">
+        <v>0.10468321604373</v>
+      </c>
+      <c r="AV180">
+        <v>0.093812874440256</v>
+      </c>
+      <c r="AW180">
+        <v>0.083078905914308</v>
+      </c>
+      <c r="AX180">
+        <v>0.095627295093103</v>
+      </c>
+      <c r="AY180">
+        <v>0.074368566376718</v>
+      </c>
+      <c r="AZ180">
+        <v>0.0673555847891</v>
+      </c>
+      <c r="BA180">
+        <v>0.073733650441794</v>
+      </c>
+      <c r="BB180">
+        <v>0.074814008051535</v>
+      </c>
+      <c r="BC180">
+        <v>0.07780048466395</v>
+      </c>
+      <c r="BD180">
+        <v>0.07527166295278501</v>
+      </c>
+      <c r="BE180">
+        <v>0.10800342974051</v>
+      </c>
+    </row>
+    <row r="181" spans="1:57">
+      <c r="A181" t="s">
+        <v>235</v>
+      </c>
+      <c r="B181">
+        <v>0.08939612243413</v>
+      </c>
+      <c r="C181">
+        <v>0.11420959997082</v>
+      </c>
+      <c r="D181">
+        <v>0.10392867455851</v>
+      </c>
+      <c r="F181">
+        <v>0.07634013883171201</v>
+      </c>
+      <c r="G181">
+        <v>0.070599061316867</v>
+      </c>
+      <c r="H181">
+        <v>0.080805948682953</v>
+      </c>
+      <c r="I181">
+        <v>0.067492793004216</v>
+      </c>
+      <c r="J181">
+        <v>0.047291485165072</v>
+      </c>
+      <c r="K181">
+        <v>0.067968115712519</v>
+      </c>
+      <c r="L181">
+        <v>0.07151227367577601</v>
+      </c>
+      <c r="M181">
+        <v>0.088548569389548</v>
+      </c>
+      <c r="N181">
+        <v>0.083037899804493</v>
+      </c>
+      <c r="O181">
+        <v>0.092065790501851</v>
+      </c>
+      <c r="P181">
+        <v>0.10266008158504</v>
+      </c>
+      <c r="Q181">
+        <v>0.094060295743364</v>
+      </c>
+      <c r="R181">
+        <v>0.079293452237544</v>
+      </c>
+      <c r="S181">
+        <v>0.09581443658727</v>
+      </c>
+      <c r="T181">
+        <v>0.09889664739003599</v>
+      </c>
+      <c r="U181">
+        <v>0.09253194114181</v>
+      </c>
+      <c r="V181">
+        <v>0.10065886460378</v>
+      </c>
+      <c r="W181">
+        <v>0.074144263109672</v>
+      </c>
+      <c r="X181">
+        <v>0.06902775751564499</v>
+      </c>
+      <c r="Y181">
+        <v>0.085583202094255</v>
+      </c>
+      <c r="Z181">
+        <v>0.07856955746479299</v>
+      </c>
+      <c r="AA181">
+        <v>0.078840603638066</v>
+      </c>
+      <c r="AB181">
+        <v>0.089646606774684</v>
+      </c>
+      <c r="AC181">
+        <v>0.088002482069325</v>
+      </c>
+      <c r="AD181">
+        <v>0.11077502654213</v>
+      </c>
+      <c r="AE181">
+        <v>0.10026341555415</v>
+      </c>
+      <c r="AF181">
+        <v>0.08553380406939901</v>
+      </c>
+      <c r="AG181">
+        <v>0.094737275331858</v>
+      </c>
+      <c r="AH181">
+        <v>0.098439484523383</v>
+      </c>
+      <c r="AI181">
+        <v>0.078828176813267</v>
+      </c>
+      <c r="AJ181">
+        <v>0.073763836247485</v>
+      </c>
+      <c r="AK181">
+        <v>0.085068251699008</v>
+      </c>
+      <c r="AL181">
+        <v>0.078540415991221</v>
+      </c>
+      <c r="AM181">
+        <v>0.068287459829381</v>
+      </c>
+      <c r="AN181">
+        <v>0.07642534346221801</v>
+      </c>
+      <c r="AO181">
+        <v>0.0938194620164</v>
+      </c>
+      <c r="AP181">
+        <v>0.076272895916869</v>
+      </c>
+      <c r="AQ181">
+        <v>0.067417882130978</v>
+      </c>
+      <c r="AR181">
+        <v>0.066136278730914</v>
+      </c>
+      <c r="AS181">
+        <v>0.07029198357370001</v>
+      </c>
+      <c r="AT181">
+        <v>0.08915616941882</v>
+      </c>
+      <c r="AU181">
+        <v>0.093144100794417</v>
+      </c>
+      <c r="AV181">
+        <v>0.089740413026433</v>
+      </c>
+      <c r="AW181">
+        <v>0.07970069227120501</v>
+      </c>
+      <c r="AX181">
+        <v>0.093703271477989</v>
+      </c>
+      <c r="AY181">
+        <v>0.073176046484622</v>
+      </c>
+      <c r="AZ181">
+        <v>0.071368961947447</v>
+      </c>
+      <c r="BA181">
+        <v>0.070032362133628</v>
+      </c>
+      <c r="BB181">
+        <v>0.07390300807352899</v>
+      </c>
+      <c r="BC181">
+        <v>0.078394736711208</v>
+      </c>
+      <c r="BD181">
+        <v>0.076378158700334</v>
+      </c>
+      <c r="BE181">
+        <v>0.10815988300845</v>
+      </c>
+    </row>
+    <row r="182" spans="1:57">
+      <c r="A182" t="s">
+        <v>236</v>
+      </c>
+      <c r="B182">
+        <v>0.09722791421917799</v>
+      </c>
+      <c r="C182">
+        <v>0.12168370882663</v>
+      </c>
+      <c r="D182">
+        <v>0.10697264821431</v>
+      </c>
+      <c r="F182">
+        <v>0.082517962514128</v>
+      </c>
+      <c r="G182">
+        <v>0.07264864774758199</v>
+      </c>
+      <c r="H182">
+        <v>0.09327824373617</v>
+      </c>
+      <c r="I182">
+        <v>0.078252137831583</v>
+      </c>
+      <c r="J182">
+        <v>0.055685481108603</v>
+      </c>
+      <c r="K182">
+        <v>0.07528202671716</v>
+      </c>
+      <c r="L182">
+        <v>0.079137086617453</v>
+      </c>
+      <c r="M182">
+        <v>0.090666739912593</v>
+      </c>
+      <c r="N182">
+        <v>0.13977290349788</v>
+      </c>
+      <c r="O182">
+        <v>0.089488262530221</v>
+      </c>
+      <c r="P182">
+        <v>0.08900726616249401</v>
+      </c>
+      <c r="Q182">
+        <v>0.09034540988996601</v>
+      </c>
+      <c r="R182">
+        <v>0.068459554483719</v>
+      </c>
+      <c r="S182">
+        <v>0.078473827432053</v>
+      </c>
+      <c r="T182">
+        <v>0.086522700833459</v>
+      </c>
+      <c r="U182">
+        <v>0.07760693990637201</v>
+      </c>
+      <c r="V182">
+        <v>0.093323024589786</v>
+      </c>
+      <c r="W182">
+        <v>0.068824320722527</v>
+      </c>
+      <c r="X182">
+        <v>0.06397898554756699</v>
+      </c>
+      <c r="Y182">
+        <v>0.07585295103388499</v>
+      </c>
+      <c r="Z182">
+        <v>0.072938531326841</v>
+      </c>
+      <c r="AA182">
+        <v>0.070812453428751</v>
+      </c>
+      <c r="AB182">
+        <v>0.079609962009761</v>
+      </c>
+      <c r="AC182">
+        <v>0.14108064825041</v>
+      </c>
+      <c r="AD182">
+        <v>0.10279102769671</v>
+      </c>
+      <c r="AE182">
+        <v>0.08992891256753199</v>
+      </c>
+      <c r="AF182">
+        <v>0.08635085571850901</v>
+      </c>
+      <c r="AG182">
+        <v>0.097844107584</v>
+      </c>
+      <c r="AH182">
+        <v>0.089335152719605</v>
+      </c>
+      <c r="AI182">
+        <v>0.0719301612252</v>
+      </c>
+      <c r="AJ182">
+        <v>0.064078458957465</v>
+      </c>
+      <c r="AK182">
+        <v>0.07965659074005201</v>
+      </c>
+      <c r="AL182">
+        <v>0.06746080972277201</v>
+      </c>
+      <c r="AM182">
+        <v>0.06308076484929399</v>
+      </c>
+      <c r="AN182">
+        <v>0.075283787861659</v>
+      </c>
+      <c r="AO182">
+        <v>0.09949580002486</v>
+      </c>
+      <c r="AP182">
+        <v>0.079785328782219</v>
+      </c>
+      <c r="AQ182">
+        <v>0.073324104587929</v>
+      </c>
+      <c r="AR182">
+        <v>0.05807169048432</v>
+      </c>
+      <c r="AS182">
+        <v>0.078738305982733</v>
+      </c>
+      <c r="AT182">
+        <v>0.097170251588945</v>
+      </c>
+      <c r="AU182">
+        <v>0.10566342371248</v>
+      </c>
+      <c r="AV182">
+        <v>0.095132447976778</v>
+      </c>
+      <c r="AW182">
+        <v>0.088700587461168</v>
+      </c>
+      <c r="AX182">
+        <v>0.10130430577187</v>
+      </c>
+      <c r="AY182">
+        <v>0.078165115050122</v>
+      </c>
+      <c r="AZ182">
+        <v>0.082670469251774</v>
+      </c>
+      <c r="BA182">
+        <v>0.076647604024857</v>
+      </c>
+      <c r="BB182">
+        <v>0.07815593555516499</v>
+      </c>
+      <c r="BC182">
+        <v>0.080651700509581</v>
+      </c>
+      <c r="BD182">
+        <v>0.079921616323872</v>
+      </c>
+      <c r="BE182">
+        <v>0.10785062688819</v>
+      </c>
+    </row>
+    <row r="183" spans="1:57">
+      <c r="A183" t="s">
+        <v>237</v>
+      </c>
+      <c r="B183">
+        <v>0.1007676133328</v>
+      </c>
+      <c r="C183">
+        <v>0.10831840454102</v>
+      </c>
+      <c r="D183">
+        <v>0.09643335785285</v>
+      </c>
+      <c r="F183">
+        <v>0.086084694581833</v>
+      </c>
+      <c r="G183">
+        <v>0.069683031201631</v>
+      </c>
+      <c r="H183">
+        <v>0.084463195585367</v>
+      </c>
+      <c r="I183">
+        <v>0.067442409235714</v>
+      </c>
+      <c r="J183">
+        <v>0.054036296883488</v>
+      </c>
+      <c r="K183">
+        <v>0.064976413316315</v>
+      </c>
+      <c r="L183">
+        <v>0.072720078663687</v>
+      </c>
+      <c r="M183">
+        <v>0.08761489821164301</v>
+      </c>
+      <c r="N183">
+        <v>0.12922307227408</v>
+      </c>
+      <c r="O183">
+        <v>0.093989622069603</v>
+      </c>
+      <c r="P183">
+        <v>0.090352880445793</v>
+      </c>
+      <c r="Q183">
+        <v>0.095656218477152</v>
+      </c>
+      <c r="R183">
+        <v>0.074096500308146</v>
+      </c>
+      <c r="S183">
+        <v>0.081414384197791</v>
+      </c>
+      <c r="T183">
+        <v>0.087031271708326</v>
+      </c>
+      <c r="U183">
+        <v>0.077297802093464</v>
+      </c>
+      <c r="V183">
+        <v>0.09015617314334699</v>
+      </c>
+      <c r="W183">
+        <v>0.069452005183693</v>
+      </c>
+      <c r="X183">
+        <v>0.060298345079513</v>
+      </c>
+      <c r="Y183">
+        <v>0.074298413293701</v>
+      </c>
+      <c r="Z183">
+        <v>0.07528055850907001</v>
+      </c>
+      <c r="AA183">
+        <v>0.074131041436339</v>
+      </c>
+      <c r="AB183">
+        <v>0.08509777033062001</v>
+      </c>
+      <c r="AC183">
+        <v>0.11906287165647</v>
+      </c>
+      <c r="AD183">
+        <v>0.10505136359221</v>
+      </c>
+      <c r="AE183">
+        <v>0.09836864626451799</v>
+      </c>
+      <c r="AF183">
+        <v>0.081959912368713</v>
+      </c>
+      <c r="AG183">
+        <v>0.08628759324350201</v>
+      </c>
+      <c r="AH183">
+        <v>0.09594466019617801</v>
+      </c>
+      <c r="AI183">
+        <v>0.076938207553329</v>
+      </c>
+      <c r="AJ183">
+        <v>0.063474881057569</v>
+      </c>
+      <c r="AK183">
+        <v>0.08275373149225999</v>
+      </c>
+      <c r="AL183">
+        <v>0.077690852940671</v>
+      </c>
+      <c r="AM183">
+        <v>0.063202080884323</v>
+      </c>
+      <c r="AN183">
+        <v>0.072633475097033</v>
+      </c>
+      <c r="AO183">
+        <v>0.092305514420238</v>
+      </c>
+      <c r="AP183">
+        <v>0.074181089948106</v>
+      </c>
+      <c r="AQ183">
+        <v>0.06296160975092401</v>
+      </c>
+      <c r="AR183">
+        <v>0.07287901348697499</v>
+      </c>
+      <c r="AS183">
+        <v>0.065771306284319</v>
+      </c>
+      <c r="AT183">
+        <v>0.08466129360355</v>
+      </c>
+      <c r="AU183">
+        <v>0.09261920355073799</v>
+      </c>
+      <c r="AV183">
+        <v>0.085248699122471</v>
+      </c>
+      <c r="AW183">
+        <v>0.07765028266072201</v>
+      </c>
+      <c r="AX183">
+        <v>0.095227919365378</v>
+      </c>
+      <c r="AY183">
+        <v>0.066458416794272</v>
+      </c>
+      <c r="AZ183">
+        <v>0.095051855956043</v>
+      </c>
+      <c r="BA183">
+        <v>0.071589620507841</v>
+      </c>
+      <c r="BB183">
+        <v>0.07172738936022301</v>
+      </c>
+      <c r="BC183">
+        <v>0.071267790357563</v>
+      </c>
+      <c r="BD183">
+        <v>0.06756717228979101</v>
+      </c>
+      <c r="BE183">
+        <v>0.099698058019648</v>
+      </c>
+    </row>
+    <row r="184" spans="1:57">
+      <c r="A184" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="185" spans="1:57">
+      <c r="A185" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="186" spans="1:57">
+      <c r="A186" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="187" spans="1:57">
+      <c r="A187" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="188" spans="1:57">
+      <c r="A188" t="s">
+        <v>242</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data up to 10th
</commit_message>
<xml_diff>
--- a/away3-6hours.xlsx
+++ b/away3-6hours.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="248">
   <si>
     <t>Alaska</t>
   </si>
@@ -744,6 +744,21 @@
   <si>
     <t>05 08 2020</t>
   </si>
+  <si>
+    <t>06 08 2020</t>
+  </si>
+  <si>
+    <t>07 08 2020</t>
+  </si>
+  <si>
+    <t>08 08 2020</t>
+  </si>
+  <si>
+    <t>09 08 2020</t>
+  </si>
+  <si>
+    <t>10 08 2020</t>
+  </si>
 </sst>
 </file>
 
@@ -1074,7 +1089,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BE188"/>
+  <dimension ref="A1:BE193"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -16487,6 +16502,9 @@
       <c r="D90">
         <v>0.082548196850063</v>
       </c>
+      <c r="E90">
+        <v>0.11762681762682</v>
+      </c>
       <c r="F90">
         <v>0.06294503996748201</v>
       </c>
@@ -16657,6 +16675,9 @@
       <c r="D91">
         <v>0.089231190278811</v>
       </c>
+      <c r="E91">
+        <v>0.12646103896104</v>
+      </c>
       <c r="F91">
         <v>0.071150657323595</v>
       </c>
@@ -16827,6 +16848,9 @@
       <c r="D92">
         <v>0.07516723883398201</v>
       </c>
+      <c r="E92">
+        <v>0.15536315536316</v>
+      </c>
       <c r="F92">
         <v>0.055004093424559</v>
       </c>
@@ -16997,6 +17021,9 @@
       <c r="D93">
         <v>0.059468315476632</v>
       </c>
+      <c r="E93">
+        <v>0.19444444444444</v>
+      </c>
       <c r="F93">
         <v>0.057262512237183</v>
       </c>
@@ -17167,6 +17194,9 @@
       <c r="D94">
         <v>0.046944996258256</v>
       </c>
+      <c r="E94">
+        <v>0.11825396825397</v>
+      </c>
       <c r="F94">
         <v>0.044193040604608</v>
       </c>
@@ -32458,25 +32488,875 @@
       <c r="A184" t="s">
         <v>238</v>
       </c>
+      <c r="B184">
+        <v>0.076436333590527</v>
+      </c>
+      <c r="C184">
+        <v>0.070493328690589</v>
+      </c>
+      <c r="D184">
+        <v>0.062323286146406</v>
+      </c>
+      <c r="F184">
+        <v>0.066492995665994</v>
+      </c>
+      <c r="G184">
+        <v>0.05482500355099</v>
+      </c>
+      <c r="H184">
+        <v>0.066251497359363</v>
+      </c>
+      <c r="I184">
+        <v>0.058588400624574</v>
+      </c>
+      <c r="J184">
+        <v>0.051838027941349</v>
+      </c>
+      <c r="K184">
+        <v>0.056429124609332</v>
+      </c>
+      <c r="L184">
+        <v>0.051866411379361</v>
+      </c>
+      <c r="M184">
+        <v>0.057522731592719</v>
+      </c>
+      <c r="N184">
+        <v>0.065558643370766</v>
+      </c>
+      <c r="O184">
+        <v>0.056282133458982</v>
+      </c>
+      <c r="P184">
+        <v>0.059644129817532</v>
+      </c>
+      <c r="Q184">
+        <v>0.067662669923942</v>
+      </c>
+      <c r="R184">
+        <v>0.052422683395611</v>
+      </c>
+      <c r="S184">
+        <v>0.049648632612831</v>
+      </c>
+      <c r="T184">
+        <v>0.053652735861181</v>
+      </c>
+      <c r="U184">
+        <v>0.04578304242305</v>
+      </c>
+      <c r="V184">
+        <v>0.054816975700815</v>
+      </c>
+      <c r="W184">
+        <v>0.056684182278314</v>
+      </c>
+      <c r="X184">
+        <v>0.044706949126838</v>
+      </c>
+      <c r="Y184">
+        <v>0.055555957837512</v>
+      </c>
+      <c r="Z184">
+        <v>0.053639281068254</v>
+      </c>
+      <c r="AA184">
+        <v>0.052848493447133</v>
+      </c>
+      <c r="AB184">
+        <v>0.058096191016408</v>
+      </c>
+      <c r="AC184">
+        <v>0.077336772276886</v>
+      </c>
+      <c r="AD184">
+        <v>0.064434466361474</v>
+      </c>
+      <c r="AE184">
+        <v>0.069779213866266</v>
+      </c>
+      <c r="AF184">
+        <v>0.056533870850582</v>
+      </c>
+      <c r="AG184">
+        <v>0.056923978130727</v>
+      </c>
+      <c r="AH184">
+        <v>0.066353951120719</v>
+      </c>
+      <c r="AI184">
+        <v>0.061879254192375</v>
+      </c>
+      <c r="AJ184">
+        <v>0.058752794246043</v>
+      </c>
+      <c r="AK184">
+        <v>0.06653057017163</v>
+      </c>
+      <c r="AL184">
+        <v>0.060311582778679</v>
+      </c>
+      <c r="AM184">
+        <v>0.057367102006891</v>
+      </c>
+      <c r="AN184">
+        <v>0.051755122361175</v>
+      </c>
+      <c r="AO184">
+        <v>0.058451133695989</v>
+      </c>
+      <c r="AP184">
+        <v>0.057509943126288</v>
+      </c>
+      <c r="AQ184">
+        <v>0.053658524132969</v>
+      </c>
+      <c r="AR184">
+        <v>0.062339364043975</v>
+      </c>
+      <c r="AS184">
+        <v>0.063637440618334</v>
+      </c>
+      <c r="AT184">
+        <v>0.059764738977201</v>
+      </c>
+      <c r="AU184">
+        <v>0.065442609227615</v>
+      </c>
+      <c r="AV184">
+        <v>0.056742558680475</v>
+      </c>
+      <c r="AW184">
+        <v>0.051330394589238</v>
+      </c>
+      <c r="AX184">
+        <v>0.06773395237829</v>
+      </c>
+      <c r="AY184">
+        <v>0.045336236755141</v>
+      </c>
+      <c r="AZ184">
+        <v>0.054998454246246</v>
+      </c>
+      <c r="BA184">
+        <v>0.051246364060736</v>
+      </c>
+      <c r="BB184">
+        <v>0.049597124052313</v>
+      </c>
+      <c r="BC184">
+        <v>0.050935057775126</v>
+      </c>
+      <c r="BD184">
+        <v>0.044193640163265</v>
+      </c>
+      <c r="BE184">
+        <v>0.062923088996558</v>
+      </c>
     </row>
     <row r="185" spans="1:57">
       <c r="A185" t="s">
         <v>239</v>
       </c>
+      <c r="B185">
+        <v>0.054124264025565</v>
+      </c>
+      <c r="C185">
+        <v>0.055117639020507</v>
+      </c>
+      <c r="D185">
+        <v>0.06416650134123</v>
+      </c>
+      <c r="F185">
+        <v>0.057644228336931</v>
+      </c>
+      <c r="G185">
+        <v>0.065275938155212</v>
+      </c>
+      <c r="H185">
+        <v>0.058661642774864</v>
+      </c>
+      <c r="I185">
+        <v>0.042972325234784</v>
+      </c>
+      <c r="J185">
+        <v>0.040424881716329</v>
+      </c>
+      <c r="K185">
+        <v>0.04500729435753</v>
+      </c>
+      <c r="L185">
+        <v>0.034979720109028</v>
+      </c>
+      <c r="M185">
+        <v>0.041518381883286</v>
+      </c>
+      <c r="N185">
+        <v>0.067063724933891</v>
+      </c>
+      <c r="O185">
+        <v>0.044252702768139</v>
+      </c>
+      <c r="P185">
+        <v>0.05177956408543</v>
+      </c>
+      <c r="Q185">
+        <v>0.056014335418566</v>
+      </c>
+      <c r="R185">
+        <v>0.043553628486967</v>
+      </c>
+      <c r="S185">
+        <v>0.045986851465373</v>
+      </c>
+      <c r="T185">
+        <v>0.051100065100899</v>
+      </c>
+      <c r="U185">
+        <v>0.04984345331077</v>
+      </c>
+      <c r="V185">
+        <v>0.058856443844999</v>
+      </c>
+      <c r="W185">
+        <v>0.057008981095378</v>
+      </c>
+      <c r="X185">
+        <v>0.049084786067812</v>
+      </c>
+      <c r="Y185">
+        <v>0.056929430724886</v>
+      </c>
+      <c r="Z185">
+        <v>0.045751329350938</v>
+      </c>
+      <c r="AA185">
+        <v>0.045655493276351</v>
+      </c>
+      <c r="AB185">
+        <v>0.049581235581171</v>
+      </c>
+      <c r="AC185">
+        <v>0.077402129619607</v>
+      </c>
+      <c r="AD185">
+        <v>0.052065561125204</v>
+      </c>
+      <c r="AE185">
+        <v>0.058982600077502</v>
+      </c>
+      <c r="AF185">
+        <v>0.050112075549664</v>
+      </c>
+      <c r="AG185">
+        <v>0.047722876499328</v>
+      </c>
+      <c r="AH185">
+        <v>0.051077061641307</v>
+      </c>
+      <c r="AI185">
+        <v>0.049481433241623</v>
+      </c>
+      <c r="AJ185">
+        <v>0.045414558740715</v>
+      </c>
+      <c r="AK185">
+        <v>0.060171697246022</v>
+      </c>
+      <c r="AL185">
+        <v>0.050737271249347</v>
+      </c>
+      <c r="AM185">
+        <v>0.04969181025952</v>
+      </c>
+      <c r="AN185">
+        <v>0.044402141840993</v>
+      </c>
+      <c r="AO185">
+        <v>0.05022527281716</v>
+      </c>
+      <c r="AP185">
+        <v>0.049090990869217</v>
+      </c>
+      <c r="AQ185">
+        <v>0.0432391283909</v>
+      </c>
+      <c r="AR185">
+        <v>0.067561273457852</v>
+      </c>
+      <c r="AS185">
+        <v>0.05034352057283</v>
+      </c>
+      <c r="AT185">
+        <v>0.048020940399804</v>
+      </c>
+      <c r="AU185">
+        <v>0.053597411923995</v>
+      </c>
+      <c r="AV185">
+        <v>0.050071335731822</v>
+      </c>
+      <c r="AW185">
+        <v>0.045181139811424</v>
+      </c>
+      <c r="AX185">
+        <v>0.055113897125296</v>
+      </c>
+      <c r="AY185">
+        <v>0.047192796464783</v>
+      </c>
+      <c r="AZ185">
+        <v>0.07010943429699899</v>
+      </c>
+      <c r="BA185">
+        <v>0.047172516620228</v>
+      </c>
+      <c r="BB185">
+        <v>0.050418399330215</v>
+      </c>
+      <c r="BC185">
+        <v>0.048827890542825</v>
+      </c>
+      <c r="BD185">
+        <v>0.047466481968798</v>
+      </c>
+      <c r="BE185">
+        <v>0.062244894556552</v>
+      </c>
     </row>
     <row r="186" spans="1:57">
       <c r="A186" t="s">
         <v>240</v>
       </c>
+      <c r="B186">
+        <v>0.089048400519762</v>
+      </c>
+      <c r="C186">
+        <v>0.10023830635236</v>
+      </c>
+      <c r="D186">
+        <v>0.10625293179318</v>
+      </c>
+      <c r="F186">
+        <v>0.08029015016720301</v>
+      </c>
+      <c r="G186">
+        <v>0.081057037873541</v>
+      </c>
+      <c r="H186">
+        <v>0.084315299337547</v>
+      </c>
+      <c r="I186">
+        <v>0.070642558949588</v>
+      </c>
+      <c r="J186">
+        <v>0.057591003008516</v>
+      </c>
+      <c r="K186">
+        <v>0.067459719126278</v>
+      </c>
+      <c r="L186">
+        <v>0.07124749978988699</v>
+      </c>
+      <c r="M186">
+        <v>0.088286416294619</v>
+      </c>
+      <c r="N186">
+        <v>0.12414696287448</v>
+      </c>
+      <c r="O186">
+        <v>0.08803827492068</v>
+      </c>
+      <c r="P186">
+        <v>0.082585418403836</v>
+      </c>
+      <c r="Q186">
+        <v>0.088748150331162</v>
+      </c>
+      <c r="R186">
+        <v>0.06391911438995</v>
+      </c>
+      <c r="S186">
+        <v>0.073620848194757</v>
+      </c>
+      <c r="T186">
+        <v>0.08286683210821399</v>
+      </c>
+      <c r="U186">
+        <v>0.073481242882493</v>
+      </c>
+      <c r="V186">
+        <v>0.08609908282230801</v>
+      </c>
+      <c r="W186">
+        <v>0.062798382855239</v>
+      </c>
+      <c r="X186">
+        <v>0.05648004557771</v>
+      </c>
+      <c r="Y186">
+        <v>0.066361203619201</v>
+      </c>
+      <c r="Z186">
+        <v>0.06784263115787401</v>
+      </c>
+      <c r="AA186">
+        <v>0.07110415132304999</v>
+      </c>
+      <c r="AB186">
+        <v>0.08647154737886099</v>
+      </c>
+      <c r="AC186">
+        <v>0.1327346700609</v>
+      </c>
+      <c r="AD186">
+        <v>0.10896298545042</v>
+      </c>
+      <c r="AE186">
+        <v>0.096842600897769</v>
+      </c>
+      <c r="AF186">
+        <v>0.07993994794760501</v>
+      </c>
+      <c r="AG186">
+        <v>0.092296975196289</v>
+      </c>
+      <c r="AH186">
+        <v>0.09832289672833899</v>
+      </c>
+      <c r="AI186">
+        <v>0.07546998716511</v>
+      </c>
+      <c r="AJ186">
+        <v>0.069909881292365</v>
+      </c>
+      <c r="AK186">
+        <v>0.082158723268485</v>
+      </c>
+      <c r="AL186">
+        <v>0.074761910047597</v>
+      </c>
+      <c r="AM186">
+        <v>0.06564103653282399</v>
+      </c>
+      <c r="AN186">
+        <v>0.074868108311404</v>
+      </c>
+      <c r="AO186">
+        <v>0.097835152275963</v>
+      </c>
+      <c r="AP186">
+        <v>0.078970738342328</v>
+      </c>
+      <c r="AQ186">
+        <v>0.067591948040383</v>
+      </c>
+      <c r="AR186">
+        <v>0.079277206460109</v>
+      </c>
+      <c r="AS186">
+        <v>0.070262393112221</v>
+      </c>
+      <c r="AT186">
+        <v>0.084838998871181</v>
+      </c>
+      <c r="AU186">
+        <v>0.09603257035762899</v>
+      </c>
+      <c r="AV186">
+        <v>0.088476768395417</v>
+      </c>
+      <c r="AW186">
+        <v>0.079920414610419</v>
+      </c>
+      <c r="AX186">
+        <v>0.089209316381511</v>
+      </c>
+      <c r="AY186">
+        <v>0.067299185717288</v>
+      </c>
+      <c r="AZ186">
+        <v>0.073844559627635</v>
+      </c>
+      <c r="BA186">
+        <v>0.064237170558158</v>
+      </c>
+      <c r="BB186">
+        <v>0.068389337678137</v>
+      </c>
+      <c r="BC186">
+        <v>0.07055682613604999</v>
+      </c>
+      <c r="BD186">
+        <v>0.06868528957787499</v>
+      </c>
+      <c r="BE186">
+        <v>0.097797369138602</v>
+      </c>
     </row>
     <row r="187" spans="1:57">
       <c r="A187" t="s">
         <v>241</v>
       </c>
+      <c r="B187">
+        <v>0.08755888006453</v>
+      </c>
+      <c r="C187">
+        <v>0.1055595803928</v>
+      </c>
+      <c r="D187">
+        <v>0.10439094044686</v>
+      </c>
+      <c r="F187">
+        <v>0.07621385458515</v>
+      </c>
+      <c r="G187">
+        <v>0.07748634443046799</v>
+      </c>
+      <c r="H187">
+        <v>0.086305759110459</v>
+      </c>
+      <c r="I187">
+        <v>0.069479822704674</v>
+      </c>
+      <c r="J187">
+        <v>0.049780718305272</v>
+      </c>
+      <c r="K187">
+        <v>0.057775368483819</v>
+      </c>
+      <c r="L187">
+        <v>0.078886864504447</v>
+      </c>
+      <c r="M187">
+        <v>0.09508879712222</v>
+      </c>
+      <c r="N187">
+        <v>0.079508872651957</v>
+      </c>
+      <c r="O187">
+        <v>0.09238993318100799</v>
+      </c>
+      <c r="P187">
+        <v>0.10017278469385</v>
+      </c>
+      <c r="Q187">
+        <v>0.098554146464944</v>
+      </c>
+      <c r="R187">
+        <v>0.077716570039999</v>
+      </c>
+      <c r="S187">
+        <v>0.090767924307337</v>
+      </c>
+      <c r="T187">
+        <v>0.09732876637231801</v>
+      </c>
+      <c r="U187">
+        <v>0.08643377586497999</v>
+      </c>
+      <c r="V187">
+        <v>0.097605329781913</v>
+      </c>
+      <c r="W187">
+        <v>0.062222571450636</v>
+      </c>
+      <c r="X187">
+        <v>0.051870976887232</v>
+      </c>
+      <c r="Y187">
+        <v>0.070509939810704</v>
+      </c>
+      <c r="Z187">
+        <v>0.0706006328764</v>
+      </c>
+      <c r="AA187">
+        <v>0.071521281839281</v>
+      </c>
+      <c r="AB187">
+        <v>0.085773443327647</v>
+      </c>
+      <c r="AC187">
+        <v>0.08732909313913199</v>
+      </c>
+      <c r="AD187">
+        <v>0.10987856679507</v>
+      </c>
+      <c r="AE187">
+        <v>0.090393774322862</v>
+      </c>
+      <c r="AF187">
+        <v>0.083222062274939</v>
+      </c>
+      <c r="AG187">
+        <v>0.099689077408692</v>
+      </c>
+      <c r="AH187">
+        <v>0.096636298668967</v>
+      </c>
+      <c r="AI187">
+        <v>0.066400267842294</v>
+      </c>
+      <c r="AJ187">
+        <v>0.054629096653068</v>
+      </c>
+      <c r="AK187">
+        <v>0.08250195410006</v>
+      </c>
+      <c r="AL187">
+        <v>0.070547159517583</v>
+      </c>
+      <c r="AM187">
+        <v>0.061011652038498</v>
+      </c>
+      <c r="AN187">
+        <v>0.081346891455539</v>
+      </c>
+      <c r="AO187">
+        <v>0.10461213818328</v>
+      </c>
+      <c r="AP187">
+        <v>0.080210118026645</v>
+      </c>
+      <c r="AQ187">
+        <v>0.06211595529914</v>
+      </c>
+      <c r="AR187">
+        <v>0.07737248379485601</v>
+      </c>
+      <c r="AS187">
+        <v>0.068718849549332</v>
+      </c>
+      <c r="AT187">
+        <v>0.08967200379729399</v>
+      </c>
+      <c r="AU187">
+        <v>0.096075755568854</v>
+      </c>
+      <c r="AV187">
+        <v>0.09260427380627199</v>
+      </c>
+      <c r="AW187">
+        <v>0.08429580991697699</v>
+      </c>
+      <c r="AX187">
+        <v>0.09659842393830601</v>
+      </c>
+      <c r="AY187">
+        <v>0.062137444176925</v>
+      </c>
+      <c r="AZ187">
+        <v>0.06511295138536601</v>
+      </c>
+      <c r="BA187">
+        <v>0.065025868373043</v>
+      </c>
+      <c r="BB187">
+        <v>0.072253512520964</v>
+      </c>
+      <c r="BC187">
+        <v>0.074275859670593</v>
+      </c>
+      <c r="BD187">
+        <v>0.073385357644732</v>
+      </c>
+      <c r="BE187">
+        <v>0.09866883850569801</v>
+      </c>
     </row>
     <row r="188" spans="1:57">
       <c r="A188" t="s">
         <v>242</v>
+      </c>
+      <c r="B188">
+        <v>0.07704740902346401</v>
+      </c>
+      <c r="C188">
+        <v>0.10805674914637</v>
+      </c>
+      <c r="D188">
+        <v>0.098230762322482</v>
+      </c>
+      <c r="F188">
+        <v>0.062012922128249</v>
+      </c>
+      <c r="G188">
+        <v>0.074615915556594</v>
+      </c>
+      <c r="H188">
+        <v>0.088279648087456</v>
+      </c>
+      <c r="I188">
+        <v>0.07518403786165601</v>
+      </c>
+      <c r="J188">
+        <v>0.059241536603265</v>
+      </c>
+      <c r="K188">
+        <v>0.072032742926916</v>
+      </c>
+      <c r="L188">
+        <v>0.0820809614703</v>
+      </c>
+      <c r="M188">
+        <v>0.098728382149951</v>
+      </c>
+      <c r="N188">
+        <v>0.088225178690891</v>
+      </c>
+      <c r="O188">
+        <v>0.098204980034909</v>
+      </c>
+      <c r="P188">
+        <v>0.097950426693866</v>
+      </c>
+      <c r="Q188">
+        <v>0.098967373664116</v>
+      </c>
+      <c r="R188">
+        <v>0.077250123797634</v>
+      </c>
+      <c r="S188">
+        <v>0.09157896474258299</v>
+      </c>
+      <c r="T188">
+        <v>0.096110911960398</v>
+      </c>
+      <c r="U188">
+        <v>0.087110011260909</v>
+      </c>
+      <c r="V188">
+        <v>0.09932845055212</v>
+      </c>
+      <c r="W188">
+        <v>0.067290874641304</v>
+      </c>
+      <c r="X188">
+        <v>0.065555760037057</v>
+      </c>
+      <c r="Y188">
+        <v>0.075506681320142</v>
+      </c>
+      <c r="Z188">
+        <v>0.073154971595358</v>
+      </c>
+      <c r="AA188">
+        <v>0.069487002075101</v>
+      </c>
+      <c r="AB188">
+        <v>0.086543673374605</v>
+      </c>
+      <c r="AC188">
+        <v>0.092115108360095</v>
+      </c>
+      <c r="AD188">
+        <v>0.11140639042339</v>
+      </c>
+      <c r="AE188">
+        <v>0.093566344151641</v>
+      </c>
+      <c r="AF188">
+        <v>0.09213831407218701</v>
+      </c>
+      <c r="AG188">
+        <v>0.10282199242312</v>
+      </c>
+      <c r="AH188">
+        <v>0.097280479012587</v>
+      </c>
+      <c r="AI188">
+        <v>0.072834277465888</v>
+      </c>
+      <c r="AJ188">
+        <v>0.071066277601953</v>
+      </c>
+      <c r="AK188">
+        <v>0.087425904351005</v>
+      </c>
+      <c r="AL188">
+        <v>0.073295212821026</v>
+      </c>
+      <c r="AM188">
+        <v>0.07078598696109301</v>
+      </c>
+      <c r="AN188">
+        <v>0.08628831645228099</v>
+      </c>
+      <c r="AO188">
+        <v>0.10601600872353</v>
+      </c>
+      <c r="AP188">
+        <v>0.084897554563675</v>
+      </c>
+      <c r="AQ188">
+        <v>0.07611194395594199</v>
+      </c>
+      <c r="AR188">
+        <v>0.08380122594597</v>
+      </c>
+      <c r="AS188">
+        <v>0.077620935673269</v>
+      </c>
+      <c r="AT188">
+        <v>0.095831333416369</v>
+      </c>
+      <c r="AU188">
+        <v>0.10782443279626</v>
+      </c>
+      <c r="AV188">
+        <v>0.10008232163074</v>
+      </c>
+      <c r="AW188">
+        <v>0.092299860071381</v>
+      </c>
+      <c r="AX188">
+        <v>0.1050809590033</v>
+      </c>
+      <c r="AY188">
+        <v>0.08124445120503899</v>
+      </c>
+      <c r="AZ188">
+        <v>0.08363231010660099</v>
+      </c>
+      <c r="BA188">
+        <v>0.07860810718231701</v>
+      </c>
+      <c r="BB188">
+        <v>0.080786186483274</v>
+      </c>
+      <c r="BC188">
+        <v>0.082770904934047</v>
+      </c>
+      <c r="BD188">
+        <v>0.08207694148227899</v>
+      </c>
+      <c r="BE188">
+        <v>0.11080436539134</v>
+      </c>
+    </row>
+    <row r="189" spans="1:57">
+      <c r="A189" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="190" spans="1:57">
+      <c r="A190" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="191" spans="1:57">
+      <c r="A191" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="192" spans="1:57">
+      <c r="A192" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1">
+      <c r="A193" t="s">
+        <v>247</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data up to 17th
</commit_message>
<xml_diff>
--- a/away3-6hours.xlsx
+++ b/away3-6hours.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="255">
   <si>
     <t>Alaska</t>
   </si>
@@ -759,6 +759,27 @@
   <si>
     <t>10 08 2020</t>
   </si>
+  <si>
+    <t>11 08 2020</t>
+  </si>
+  <si>
+    <t>12 08 2020</t>
+  </si>
+  <si>
+    <t>13 08 2020</t>
+  </si>
+  <si>
+    <t>14 08 2020</t>
+  </si>
+  <si>
+    <t>15 08 2020</t>
+  </si>
+  <si>
+    <t>16 08 2020</t>
+  </si>
+  <si>
+    <t>17 08 2020</t>
+  </si>
 </sst>
 </file>
 
@@ -1089,7 +1110,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BE193"/>
+  <dimension ref="A1:BE200"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -17367,6 +17388,9 @@
       <c r="D95">
         <v>0.07613204512944199</v>
       </c>
+      <c r="E95">
+        <v>0.10633903133903</v>
+      </c>
       <c r="F95">
         <v>0.055728139519302</v>
       </c>
@@ -17537,6 +17561,9 @@
       <c r="D96">
         <v>0.092518149680694</v>
       </c>
+      <c r="E96">
+        <v>0.1143475572047</v>
+      </c>
       <c r="F96">
         <v>0.06742109783813401</v>
       </c>
@@ -17707,6 +17734,9 @@
       <c r="D97">
         <v>0.09554227546562299</v>
       </c>
+      <c r="E97">
+        <v>0.12175324675325</v>
+      </c>
       <c r="F97">
         <v>0.07527645097822799</v>
       </c>
@@ -17877,6 +17907,9 @@
       <c r="D98">
         <v>0.07734849163473</v>
       </c>
+      <c r="E98">
+        <v>0.14635225885226</v>
+      </c>
       <c r="F98">
         <v>0.052724733497246</v>
       </c>
@@ -18047,6 +18080,9 @@
       <c r="D99">
         <v>0.080682708737413</v>
       </c>
+      <c r="E99">
+        <v>0.13388888888889</v>
+      </c>
       <c r="F99">
         <v>0.073703939321414</v>
       </c>
@@ -18217,6 +18253,9 @@
       <c r="D100">
         <v>0.05330423502681</v>
       </c>
+      <c r="E100">
+        <v>0.20477855477855</v>
+      </c>
       <c r="F100">
         <v>0.048685769544214</v>
       </c>
@@ -18387,6 +18426,9 @@
       <c r="D101">
         <v>0.0528459815525</v>
       </c>
+      <c r="E101">
+        <v>0.1404173312068</v>
+      </c>
       <c r="F101">
         <v>0.052712757192858</v>
       </c>
@@ -33338,25 +33380,1215 @@
       <c r="A189" t="s">
         <v>243</v>
       </c>
+      <c r="B189">
+        <v>0.08107899630349499</v>
+      </c>
+      <c r="C189">
+        <v>0.11591429841973</v>
+      </c>
+      <c r="D189">
+        <v>0.10499700295667</v>
+      </c>
+      <c r="F189">
+        <v>0.06887550555208601</v>
+      </c>
+      <c r="G189">
+        <v>0.075348475069654</v>
+      </c>
+      <c r="H189">
+        <v>0.085988401489462</v>
+      </c>
+      <c r="I189">
+        <v>0.074651434986786</v>
+      </c>
+      <c r="J189">
+        <v>0.055851976182784</v>
+      </c>
+      <c r="K189">
+        <v>0.065353484644079</v>
+      </c>
+      <c r="L189">
+        <v>0.07415608878815801</v>
+      </c>
+      <c r="M189">
+        <v>0.09335166584479</v>
+      </c>
+      <c r="N189">
+        <v>0.082456968819814</v>
+      </c>
+      <c r="O189">
+        <v>0.090581075856161</v>
+      </c>
+      <c r="P189">
+        <v>0.09146998571689501</v>
+      </c>
+      <c r="Q189">
+        <v>0.095975975266429</v>
+      </c>
+      <c r="R189">
+        <v>0.074689417529529</v>
+      </c>
+      <c r="S189">
+        <v>0.087860451557136</v>
+      </c>
+      <c r="T189">
+        <v>0.09234757097002699</v>
+      </c>
+      <c r="U189">
+        <v>0.083343419108491</v>
+      </c>
+      <c r="V189">
+        <v>0.09689934246394701</v>
+      </c>
+      <c r="W189">
+        <v>0.072183516910098</v>
+      </c>
+      <c r="X189">
+        <v>0.060639344669037</v>
+      </c>
+      <c r="Y189">
+        <v>0.07392234019983999</v>
+      </c>
+      <c r="Z189">
+        <v>0.079433118796019</v>
+      </c>
+      <c r="AA189">
+        <v>0.079049665267831</v>
+      </c>
+      <c r="AB189">
+        <v>0.093974441825938</v>
+      </c>
+      <c r="AC189">
+        <v>0.09253209669876999</v>
+      </c>
+      <c r="AD189">
+        <v>0.11926218367223</v>
+      </c>
+      <c r="AE189">
+        <v>0.10499768234359</v>
+      </c>
+      <c r="AF189">
+        <v>0.089449236967587</v>
+      </c>
+      <c r="AG189">
+        <v>0.09868705232877401</v>
+      </c>
+      <c r="AH189">
+        <v>0.10381830039617</v>
+      </c>
+      <c r="AI189">
+        <v>0.081550576068514</v>
+      </c>
+      <c r="AJ189">
+        <v>0.07312551420507001</v>
+      </c>
+      <c r="AK189">
+        <v>0.088758976723355</v>
+      </c>
+      <c r="AL189">
+        <v>0.083284006574999</v>
+      </c>
+      <c r="AM189">
+        <v>0.07078860737254999</v>
+      </c>
+      <c r="AN189">
+        <v>0.08191574338228</v>
+      </c>
+      <c r="AO189">
+        <v>0.10683028149455</v>
+      </c>
+      <c r="AP189">
+        <v>0.082329418692255</v>
+      </c>
+      <c r="AQ189">
+        <v>0.07383805025378901</v>
+      </c>
+      <c r="AR189">
+        <v>0.088430532391334</v>
+      </c>
+      <c r="AS189">
+        <v>0.081220351725054</v>
+      </c>
+      <c r="AT189">
+        <v>0.09762673995646801</v>
+      </c>
+      <c r="AU189">
+        <v>0.10583445398543</v>
+      </c>
+      <c r="AV189">
+        <v>0.098561659501007</v>
+      </c>
+      <c r="AW189">
+        <v>0.091827724410374</v>
+      </c>
+      <c r="AX189">
+        <v>0.09887131283583001</v>
+      </c>
+      <c r="AY189">
+        <v>0.077901425107677</v>
+      </c>
+      <c r="AZ189">
+        <v>0.090305908431562</v>
+      </c>
+      <c r="BA189">
+        <v>0.077783849560894</v>
+      </c>
+      <c r="BB189">
+        <v>0.079495453059255</v>
+      </c>
+      <c r="BC189">
+        <v>0.086084781057856</v>
+      </c>
+      <c r="BD189">
+        <v>0.084057544536881</v>
+      </c>
+      <c r="BE189">
+        <v>0.11410987679184</v>
+      </c>
     </row>
     <row r="190" spans="1:57">
       <c r="A190" t="s">
         <v>244</v>
       </c>
+      <c r="B190">
+        <v>0.08528850344887499</v>
+      </c>
+      <c r="C190">
+        <v>0.099239772539118</v>
+      </c>
+      <c r="D190">
+        <v>0.09555880300099701</v>
+      </c>
+      <c r="F190">
+        <v>0.07199904048404999</v>
+      </c>
+      <c r="G190">
+        <v>0.07419323521774</v>
+      </c>
+      <c r="H190">
+        <v>0.090020005537853</v>
+      </c>
+      <c r="I190">
+        <v>0.074621911022761</v>
+      </c>
+      <c r="J190">
+        <v>0.058001083898971</v>
+      </c>
+      <c r="K190">
+        <v>0.068055908782873</v>
+      </c>
+      <c r="L190">
+        <v>0.074878182232584</v>
+      </c>
+      <c r="M190">
+        <v>0.094411355066793</v>
+      </c>
+      <c r="N190">
+        <v>0.078888841425981</v>
+      </c>
+      <c r="O190">
+        <v>0.09552851384579</v>
+      </c>
+      <c r="P190">
+        <v>0.089401531729426</v>
+      </c>
+      <c r="Q190">
+        <v>0.09739233397621699</v>
+      </c>
+      <c r="R190">
+        <v>0.08134413886118699</v>
+      </c>
+      <c r="S190">
+        <v>0.09078419768699</v>
+      </c>
+      <c r="T190">
+        <v>0.08700737178451499</v>
+      </c>
+      <c r="U190">
+        <v>0.07860391165113299</v>
+      </c>
+      <c r="V190">
+        <v>0.091898104617437</v>
+      </c>
+      <c r="W190">
+        <v>0.059013424242531</v>
+      </c>
+      <c r="X190">
+        <v>0.057035348336114</v>
+      </c>
+      <c r="Y190">
+        <v>0.066586638717731</v>
+      </c>
+      <c r="Z190">
+        <v>0.06586909132287801</v>
+      </c>
+      <c r="AA190">
+        <v>0.059890897741505</v>
+      </c>
+      <c r="AB190">
+        <v>0.075349127401017</v>
+      </c>
+      <c r="AC190">
+        <v>0.098139868921782</v>
+      </c>
+      <c r="AD190">
+        <v>0.1046121447263</v>
+      </c>
+      <c r="AE190">
+        <v>0.077058441366436</v>
+      </c>
+      <c r="AF190">
+        <v>0.080020838423872</v>
+      </c>
+      <c r="AG190">
+        <v>0.085061970378634</v>
+      </c>
+      <c r="AH190">
+        <v>0.085947614900447</v>
+      </c>
+      <c r="AI190">
+        <v>0.061323427514395</v>
+      </c>
+      <c r="AJ190">
+        <v>0.053874737585808</v>
+      </c>
+      <c r="AK190">
+        <v>0.071947928756247</v>
+      </c>
+      <c r="AL190">
+        <v>0.064442951976314</v>
+      </c>
+      <c r="AM190">
+        <v>0.055882802136221</v>
+      </c>
+      <c r="AN190">
+        <v>0.07466829006351899</v>
+      </c>
+      <c r="AO190">
+        <v>0.095376007411062</v>
+      </c>
+      <c r="AP190">
+        <v>0.075515794264438</v>
+      </c>
+      <c r="AQ190">
+        <v>0.064899607102971</v>
+      </c>
+      <c r="AR190">
+        <v>0.077400798097061</v>
+      </c>
+      <c r="AS190">
+        <v>0.068104388247183</v>
+      </c>
+      <c r="AT190">
+        <v>0.086847959632756</v>
+      </c>
+      <c r="AU190">
+        <v>0.09054887556232</v>
+      </c>
+      <c r="AV190">
+        <v>0.09183917965291299</v>
+      </c>
+      <c r="AW190">
+        <v>0.083252494209392</v>
+      </c>
+      <c r="AX190">
+        <v>0.09176723757275999</v>
+      </c>
+      <c r="AY190">
+        <v>0.069553851258102</v>
+      </c>
+      <c r="AZ190">
+        <v>0.07387658758127599</v>
+      </c>
+      <c r="BA190">
+        <v>0.065359134799677</v>
+      </c>
+      <c r="BB190">
+        <v>0.06999146400527</v>
+      </c>
+      <c r="BC190">
+        <v>0.073845717217437</v>
+      </c>
+      <c r="BD190">
+        <v>0.07362619903968699</v>
+      </c>
+      <c r="BE190">
+        <v>0.10076195573437</v>
+      </c>
     </row>
     <row r="191" spans="1:57">
       <c r="A191" t="s">
         <v>245</v>
       </c>
+      <c r="B191">
+        <v>0.07057384242779401</v>
+      </c>
+      <c r="C191">
+        <v>0.073446479222755</v>
+      </c>
+      <c r="D191">
+        <v>0.066607771746537</v>
+      </c>
+      <c r="F191">
+        <v>0.069521365704694</v>
+      </c>
+      <c r="G191">
+        <v>0.06480189556687301</v>
+      </c>
+      <c r="H191">
+        <v>0.074748897821748</v>
+      </c>
+      <c r="I191">
+        <v>0.063428608119501</v>
+      </c>
+      <c r="J191">
+        <v>0.057709921654755</v>
+      </c>
+      <c r="K191">
+        <v>0.061210528117067</v>
+      </c>
+      <c r="L191">
+        <v>0.056709629974563</v>
+      </c>
+      <c r="M191">
+        <v>0.055275243638132</v>
+      </c>
+      <c r="N191">
+        <v>0.072297209963868</v>
+      </c>
+      <c r="O191">
+        <v>0.049415897399954</v>
+      </c>
+      <c r="P191">
+        <v>0.062477127153026</v>
+      </c>
+      <c r="Q191">
+        <v>0.065388352390612</v>
+      </c>
+      <c r="R191">
+        <v>0.053352267496902</v>
+      </c>
+      <c r="S191">
+        <v>0.058684003656201</v>
+      </c>
+      <c r="T191">
+        <v>0.057243974815571</v>
+      </c>
+      <c r="U191">
+        <v>0.057666876250653</v>
+      </c>
+      <c r="V191">
+        <v>0.06270173081998499</v>
+      </c>
+      <c r="W191">
+        <v>0.058582450985422</v>
+      </c>
+      <c r="X191">
+        <v>0.050740117656968</v>
+      </c>
+      <c r="Y191">
+        <v>0.060752848863968</v>
+      </c>
+      <c r="Z191">
+        <v>0.060333206625039</v>
+      </c>
+      <c r="AA191">
+        <v>0.056133631807797</v>
+      </c>
+      <c r="AB191">
+        <v>0.061057372533341</v>
+      </c>
+      <c r="AC191">
+        <v>0.08694098571525199</v>
+      </c>
+      <c r="AD191">
+        <v>0.067673132786791</v>
+      </c>
+      <c r="AE191">
+        <v>0.07229645317589301</v>
+      </c>
+      <c r="AF191">
+        <v>0.056110170655487</v>
+      </c>
+      <c r="AG191">
+        <v>0.058062509761545</v>
+      </c>
+      <c r="AH191">
+        <v>0.06339915759152499</v>
+      </c>
+      <c r="AI191">
+        <v>0.054823705133703</v>
+      </c>
+      <c r="AJ191">
+        <v>0.051290988224175</v>
+      </c>
+      <c r="AK191">
+        <v>0.061379017210957</v>
+      </c>
+      <c r="AL191">
+        <v>0.060827223949659</v>
+      </c>
+      <c r="AM191">
+        <v>0.050046952281118</v>
+      </c>
+      <c r="AN191">
+        <v>0.056554373982447</v>
+      </c>
+      <c r="AO191">
+        <v>0.059225601095127</v>
+      </c>
+      <c r="AP191">
+        <v>0.059214621469214</v>
+      </c>
+      <c r="AQ191">
+        <v>0.054141005482173</v>
+      </c>
+      <c r="AR191">
+        <v>0.07105292312801301</v>
+      </c>
+      <c r="AS191">
+        <v>0.055396485272249</v>
+      </c>
+      <c r="AT191">
+        <v>0.059644304399622</v>
+      </c>
+      <c r="AU191">
+        <v>0.058097117591717</v>
+      </c>
+      <c r="AV191">
+        <v>0.057279370171642</v>
+      </c>
+      <c r="AW191">
+        <v>0.053523146959504</v>
+      </c>
+      <c r="AX191">
+        <v>0.068075847350947</v>
+      </c>
+      <c r="AY191">
+        <v>0.050478759956058</v>
+      </c>
+      <c r="AZ191">
+        <v>0.067809418421363</v>
+      </c>
+      <c r="BA191">
+        <v>0.053701786930462</v>
+      </c>
+      <c r="BB191">
+        <v>0.054211754347248</v>
+      </c>
+      <c r="BC191">
+        <v>0.054997394381643</v>
+      </c>
+      <c r="BD191">
+        <v>0.055645618642697</v>
+      </c>
+      <c r="BE191">
+        <v>0.069840875582907</v>
+      </c>
     </row>
     <row r="192" spans="1:57">
       <c r="A192" t="s">
         <v>246</v>
       </c>
+      <c r="B192">
+        <v>0.055724591095004</v>
+      </c>
+      <c r="C192">
+        <v>0.062245607100191</v>
+      </c>
+      <c r="D192">
+        <v>0.055128404562727</v>
+      </c>
+      <c r="F192">
+        <v>0.048723777869942</v>
+      </c>
+      <c r="G192">
+        <v>0.053785348655417</v>
+      </c>
+      <c r="H192">
+        <v>0.061922221934842</v>
+      </c>
+      <c r="I192">
+        <v>0.053424594555461</v>
+      </c>
+      <c r="J192">
+        <v>0.046026417304982</v>
+      </c>
+      <c r="K192">
+        <v>0.050955585801959</v>
+      </c>
+      <c r="L192">
+        <v>0.044255913071989</v>
+      </c>
+      <c r="M192">
+        <v>0.046043568379635</v>
+      </c>
+      <c r="N192">
+        <v>0.076504129280654</v>
+      </c>
+      <c r="O192">
+        <v>0.047344160459536</v>
+      </c>
+      <c r="P192">
+        <v>0.057282588311118</v>
+      </c>
+      <c r="Q192">
+        <v>0.06082139324549</v>
+      </c>
+      <c r="R192">
+        <v>0.049898149091969</v>
+      </c>
+      <c r="S192">
+        <v>0.054829079614674</v>
+      </c>
+      <c r="T192">
+        <v>0.054386683180965</v>
+      </c>
+      <c r="U192">
+        <v>0.056183645639025</v>
+      </c>
+      <c r="V192">
+        <v>0.060639948999142</v>
+      </c>
+      <c r="W192">
+        <v>0.063424452762985</v>
+      </c>
+      <c r="X192">
+        <v>0.051678639432347</v>
+      </c>
+      <c r="Y192">
+        <v>0.06438906461914801</v>
+      </c>
+      <c r="Z192">
+        <v>0.051331610304879</v>
+      </c>
+      <c r="AA192">
+        <v>0.043952915885469</v>
+      </c>
+      <c r="AB192">
+        <v>0.050241548338897</v>
+      </c>
+      <c r="AC192">
+        <v>0.084453251080645</v>
+      </c>
+      <c r="AD192">
+        <v>0.053877120191426</v>
+      </c>
+      <c r="AE192">
+        <v>0.061769824874398</v>
+      </c>
+      <c r="AF192">
+        <v>0.056521630833433</v>
+      </c>
+      <c r="AG192">
+        <v>0.054217446650585</v>
+      </c>
+      <c r="AH192">
+        <v>0.049706893222147</v>
+      </c>
+      <c r="AI192">
+        <v>0.052259935036747</v>
+      </c>
+      <c r="AJ192">
+        <v>0.051255610098195</v>
+      </c>
+      <c r="AK192">
+        <v>0.0579596039442</v>
+      </c>
+      <c r="AL192">
+        <v>0.049960538889244</v>
+      </c>
+      <c r="AM192">
+        <v>0.056685616514887</v>
+      </c>
+      <c r="AN192">
+        <v>0.059062250874713</v>
+      </c>
+      <c r="AO192">
+        <v>0.058068266005323</v>
+      </c>
+      <c r="AP192">
+        <v>0.060485535106094</v>
+      </c>
+      <c r="AQ192">
+        <v>0.057554515467818</v>
+      </c>
+      <c r="AR192">
+        <v>0.073229481457615</v>
+      </c>
+      <c r="AS192">
+        <v>0.064819014491977</v>
+      </c>
+      <c r="AT192">
+        <v>0.054934358410342</v>
+      </c>
+      <c r="AU192">
+        <v>0.055995011787941</v>
+      </c>
+      <c r="AV192">
+        <v>0.053257650511558</v>
+      </c>
+      <c r="AW192">
+        <v>0.04733471282492</v>
+      </c>
+      <c r="AX192">
+        <v>0.056897057248801</v>
+      </c>
+      <c r="AY192">
+        <v>0.049964221919162</v>
+      </c>
+      <c r="AZ192">
+        <v>0.06663026903881999</v>
+      </c>
+      <c r="BA192">
+        <v>0.051638429643581</v>
+      </c>
+      <c r="BB192">
+        <v>0.051996817157697</v>
+      </c>
+      <c r="BC192">
+        <v>0.047389795057878</v>
+      </c>
+      <c r="BD192">
+        <v>0.050646452747949</v>
+      </c>
+      <c r="BE192">
+        <v>0.05829878569234</v>
+      </c>
     </row>
-    <row r="193" spans="1:1">
+    <row r="193" spans="1:57">
       <c r="A193" t="s">
         <v>247</v>
+      </c>
+      <c r="B193">
+        <v>0.07074734108401901</v>
+      </c>
+      <c r="C193">
+        <v>0.10315529353443</v>
+      </c>
+      <c r="D193">
+        <v>0.10262219301479</v>
+      </c>
+      <c r="F193">
+        <v>0.06274683670938599</v>
+      </c>
+      <c r="G193">
+        <v>0.084219328083076</v>
+      </c>
+      <c r="H193">
+        <v>0.091326722449651</v>
+      </c>
+      <c r="I193">
+        <v>0.078459665731685</v>
+      </c>
+      <c r="J193">
+        <v>0.06547679000399501</v>
+      </c>
+      <c r="K193">
+        <v>0.07305044054663801</v>
+      </c>
+      <c r="L193">
+        <v>0.07984434464922199</v>
+      </c>
+      <c r="M193">
+        <v>0.094563819272566</v>
+      </c>
+      <c r="N193">
+        <v>0.078646784046428</v>
+      </c>
+      <c r="O193">
+        <v>0.084398076447763</v>
+      </c>
+      <c r="P193">
+        <v>0.09504785138560599</v>
+      </c>
+      <c r="Q193">
+        <v>0.090537375417741</v>
+      </c>
+      <c r="R193">
+        <v>0.07002882203238101</v>
+      </c>
+      <c r="S193">
+        <v>0.087057787026127</v>
+      </c>
+      <c r="T193">
+        <v>0.094067245595239</v>
+      </c>
+      <c r="U193">
+        <v>0.08350342154696801</v>
+      </c>
+      <c r="V193">
+        <v>0.099304724515951</v>
+      </c>
+      <c r="W193">
+        <v>0.070627610835358</v>
+      </c>
+      <c r="X193">
+        <v>0.06596245587286199</v>
+      </c>
+      <c r="Y193">
+        <v>0.07474534285767701</v>
+      </c>
+      <c r="Z193">
+        <v>0.07293180477215901</v>
+      </c>
+      <c r="AA193">
+        <v>0.068898379725449</v>
+      </c>
+      <c r="AB193">
+        <v>0.085086315796691</v>
+      </c>
+      <c r="AC193">
+        <v>0.10306590006039</v>
+      </c>
+      <c r="AD193">
+        <v>0.11294688344378</v>
+      </c>
+      <c r="AE193">
+        <v>0.094349574922233</v>
+      </c>
+      <c r="AF193">
+        <v>0.087015190326841</v>
+      </c>
+      <c r="AG193">
+        <v>0.096427277290693</v>
+      </c>
+      <c r="AH193">
+        <v>0.09678079957671</v>
+      </c>
+      <c r="AI193">
+        <v>0.070814000670355</v>
+      </c>
+      <c r="AJ193">
+        <v>0.06674282599456299</v>
+      </c>
+      <c r="AK193">
+        <v>0.077878397757615</v>
+      </c>
+      <c r="AL193">
+        <v>0.070077722609886</v>
+      </c>
+      <c r="AM193">
+        <v>0.063474304534012</v>
+      </c>
+      <c r="AN193">
+        <v>0.07689445281337901</v>
+      </c>
+      <c r="AO193">
+        <v>0.10103120492813</v>
+      </c>
+      <c r="AP193">
+        <v>0.075969688192657</v>
+      </c>
+      <c r="AQ193">
+        <v>0.069628938490847</v>
+      </c>
+      <c r="AR193">
+        <v>0.078935703555418</v>
+      </c>
+      <c r="AS193">
+        <v>0.068328210581241</v>
+      </c>
+      <c r="AT193">
+        <v>0.094112997727203</v>
+      </c>
+      <c r="AU193">
+        <v>0.097349108549691</v>
+      </c>
+      <c r="AV193">
+        <v>0.096230210099554</v>
+      </c>
+      <c r="AW193">
+        <v>0.088483366385783</v>
+      </c>
+      <c r="AX193">
+        <v>0.099622797255232</v>
+      </c>
+      <c r="AY193">
+        <v>0.07359903095643</v>
+      </c>
+      <c r="AZ193">
+        <v>0.074978150680849</v>
+      </c>
+      <c r="BA193">
+        <v>0.07071719307813699</v>
+      </c>
+      <c r="BB193">
+        <v>0.073778250198206</v>
+      </c>
+      <c r="BC193">
+        <v>0.072805022510013</v>
+      </c>
+      <c r="BD193">
+        <v>0.076800838710472</v>
+      </c>
+      <c r="BE193">
+        <v>0.10109429318109</v>
+      </c>
+    </row>
+    <row r="194" spans="1:57">
+      <c r="A194" t="s">
+        <v>248</v>
+      </c>
+      <c r="B194">
+        <v>0.065968637136207</v>
+      </c>
+      <c r="C194">
+        <v>0.10257734045455</v>
+      </c>
+      <c r="D194">
+        <v>0.10235963858813</v>
+      </c>
+      <c r="F194">
+        <v>0.061206977897677</v>
+      </c>
+      <c r="G194">
+        <v>0.081811576839861</v>
+      </c>
+      <c r="H194">
+        <v>0.095155553988853</v>
+      </c>
+      <c r="I194">
+        <v>0.077620889470032</v>
+      </c>
+      <c r="J194">
+        <v>0.059043062315908</v>
+      </c>
+      <c r="K194">
+        <v>0.07102227309597001</v>
+      </c>
+      <c r="L194">
+        <v>0.076933030793499</v>
+      </c>
+      <c r="M194">
+        <v>0.093584849544694</v>
+      </c>
+      <c r="N194">
+        <v>0.081756363774152</v>
+      </c>
+      <c r="O194">
+        <v>0.085984373586284</v>
+      </c>
+      <c r="P194">
+        <v>0.091450434081451</v>
+      </c>
+      <c r="Q194">
+        <v>0.093337293582238</v>
+      </c>
+      <c r="R194">
+        <v>0.070891538120467</v>
+      </c>
+      <c r="S194">
+        <v>0.08830703472698199</v>
+      </c>
+      <c r="T194">
+        <v>0.094802375713805</v>
+      </c>
+      <c r="U194">
+        <v>0.08519611510583699</v>
+      </c>
+      <c r="V194">
+        <v>0.1002712782702</v>
+      </c>
+      <c r="W194">
+        <v>0.071861092083643</v>
+      </c>
+      <c r="X194">
+        <v>0.066931600822375</v>
+      </c>
+      <c r="Y194">
+        <v>0.07989529924439</v>
+      </c>
+      <c r="Z194">
+        <v>0.07510534068833</v>
+      </c>
+      <c r="AA194">
+        <v>0.073718317040503</v>
+      </c>
+      <c r="AB194">
+        <v>0.087674139073541</v>
+      </c>
+      <c r="AC194">
+        <v>0.099097141242225</v>
+      </c>
+      <c r="AD194">
+        <v>0.11699921616367</v>
+      </c>
+      <c r="AE194">
+        <v>0.09827799119463899</v>
+      </c>
+      <c r="AF194">
+        <v>0.08727088528664199</v>
+      </c>
+      <c r="AG194">
+        <v>0.096898746010312</v>
+      </c>
+      <c r="AH194">
+        <v>0.10340658710587</v>
+      </c>
+      <c r="AI194">
+        <v>0.074220670500807</v>
+      </c>
+      <c r="AJ194">
+        <v>0.068069582567262</v>
+      </c>
+      <c r="AK194">
+        <v>0.084070517713452</v>
+      </c>
+      <c r="AL194">
+        <v>0.073917217664025</v>
+      </c>
+      <c r="AM194">
+        <v>0.06342278793688701</v>
+      </c>
+      <c r="AN194">
+        <v>0.07329628696910701</v>
+      </c>
+      <c r="AO194">
+        <v>0.10191284855256</v>
+      </c>
+      <c r="AP194">
+        <v>0.076070557315013</v>
+      </c>
+      <c r="AQ194">
+        <v>0.07050997061808301</v>
+      </c>
+      <c r="AR194">
+        <v>0.07813495525705</v>
+      </c>
+      <c r="AS194">
+        <v>0.078672284958588</v>
+      </c>
+      <c r="AT194">
+        <v>0.098167602446165</v>
+      </c>
+      <c r="AU194">
+        <v>0.10925653166175</v>
+      </c>
+      <c r="AV194">
+        <v>0.10128605728976</v>
+      </c>
+      <c r="AW194">
+        <v>0.095854937341221</v>
+      </c>
+      <c r="AX194">
+        <v>0.10622272807157</v>
+      </c>
+      <c r="AY194">
+        <v>0.08051611719042299</v>
+      </c>
+      <c r="AZ194">
+        <v>0.080261235171151</v>
+      </c>
+      <c r="BA194">
+        <v>0.080458378022082</v>
+      </c>
+      <c r="BB194">
+        <v>0.079816771442508</v>
+      </c>
+      <c r="BC194">
+        <v>0.07950680027832301</v>
+      </c>
+      <c r="BD194">
+        <v>0.081168943946008</v>
+      </c>
+      <c r="BE194">
+        <v>0.10759952911945</v>
+      </c>
+    </row>
+    <row r="195" spans="1:57">
+      <c r="A195" t="s">
+        <v>249</v>
+      </c>
+      <c r="B195">
+        <v>0.08336663736240001</v>
+      </c>
+      <c r="C195">
+        <v>0.10904951748915</v>
+      </c>
+      <c r="D195">
+        <v>0.10798981511461</v>
+      </c>
+      <c r="F195">
+        <v>0.074480206263128</v>
+      </c>
+      <c r="G195">
+        <v>0.074248461816115</v>
+      </c>
+      <c r="H195">
+        <v>0.09276439303921501</v>
+      </c>
+      <c r="I195">
+        <v>0.07525249414176199</v>
+      </c>
+      <c r="J195">
+        <v>0.055501642198015</v>
+      </c>
+      <c r="K195">
+        <v>0.07444955080577501</v>
+      </c>
+      <c r="L195">
+        <v>0.080430528236246</v>
+      </c>
+      <c r="M195">
+        <v>0.094429121062074</v>
+      </c>
+      <c r="N195">
+        <v>0.08681421545378901</v>
+      </c>
+      <c r="O195">
+        <v>0.08911082669386999</v>
+      </c>
+      <c r="P195">
+        <v>0.09657899414608399</v>
+      </c>
+      <c r="Q195">
+        <v>0.094337234299675</v>
+      </c>
+      <c r="R195">
+        <v>0.072518876250192</v>
+      </c>
+      <c r="S195">
+        <v>0.093310094860151</v>
+      </c>
+      <c r="T195">
+        <v>0.097982719731585</v>
+      </c>
+      <c r="U195">
+        <v>0.08970686277222401</v>
+      </c>
+      <c r="V195">
+        <v>0.10248101172712</v>
+      </c>
+      <c r="W195">
+        <v>0.071216377883305</v>
+      </c>
+      <c r="X195">
+        <v>0.067345684469673</v>
+      </c>
+      <c r="Y195">
+        <v>0.07833128733380899</v>
+      </c>
+      <c r="Z195">
+        <v>0.07622388133371701</v>
+      </c>
+      <c r="AA195">
+        <v>0.072037290488479</v>
+      </c>
+      <c r="AB195">
+        <v>0.08993251118025</v>
+      </c>
+      <c r="AC195">
+        <v>0.09661787789544</v>
+      </c>
+      <c r="AD195">
+        <v>0.11508140648987</v>
+      </c>
+      <c r="AE195">
+        <v>0.09587145529963199</v>
+      </c>
+      <c r="AF195">
+        <v>0.093995157714217</v>
+      </c>
+      <c r="AG195">
+        <v>0.10178868736528</v>
+      </c>
+      <c r="AH195">
+        <v>0.10707359913244</v>
+      </c>
+      <c r="AI195">
+        <v>0.07727754499461</v>
+      </c>
+      <c r="AJ195">
+        <v>0.070310417782148</v>
+      </c>
+      <c r="AK195">
+        <v>0.08765623050305101</v>
+      </c>
+      <c r="AL195">
+        <v>0.07597980074051799</v>
+      </c>
+      <c r="AM195">
+        <v>0.06866872474100499</v>
+      </c>
+      <c r="AN195">
+        <v>0.079829338424067</v>
+      </c>
+      <c r="AO195">
+        <v>0.10680307398489</v>
+      </c>
+      <c r="AP195">
+        <v>0.077969732020312</v>
+      </c>
+      <c r="AQ195">
+        <v>0.071024867288851</v>
+      </c>
+      <c r="AR195">
+        <v>0.08305439129499</v>
+      </c>
+      <c r="AS195">
+        <v>0.071006212687402</v>
+      </c>
+      <c r="AT195">
+        <v>0.09619130836717001</v>
+      </c>
+      <c r="AU195">
+        <v>0.10064866379516</v>
+      </c>
+      <c r="AV195">
+        <v>0.09840847930989501</v>
+      </c>
+      <c r="AW195">
+        <v>0.08924887037575401</v>
+      </c>
+      <c r="AX195">
+        <v>0.09877492273593</v>
+      </c>
+      <c r="AY195">
+        <v>0.074619086075933</v>
+      </c>
+      <c r="AZ195">
+        <v>0.083930453836414</v>
+      </c>
+      <c r="BA195">
+        <v>0.07222480953435099</v>
+      </c>
+      <c r="BB195">
+        <v>0.074685261647728</v>
+      </c>
+      <c r="BC195">
+        <v>0.079851506754476</v>
+      </c>
+      <c r="BD195">
+        <v>0.076004341395727</v>
+      </c>
+      <c r="BE195">
+        <v>0.10780648786003</v>
+      </c>
+    </row>
+    <row r="196" spans="1:57">
+      <c r="A196" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="197" spans="1:57">
+      <c r="A197" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="198" spans="1:57">
+      <c r="A198" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="199" spans="1:57">
+      <c r="A199" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="200" spans="1:57">
+      <c r="A200" t="s">
+        <v>254</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data up to 25th aug
</commit_message>
<xml_diff>
--- a/away3-6hours.xlsx
+++ b/away3-6hours.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="263">
   <si>
     <t>Alaska</t>
   </si>
@@ -780,6 +780,30 @@
   <si>
     <t>17 08 2020</t>
   </si>
+  <si>
+    <t>18 08 2020</t>
+  </si>
+  <si>
+    <t>19 08 2020</t>
+  </si>
+  <si>
+    <t>20 08 2020</t>
+  </si>
+  <si>
+    <t>21 08 2020</t>
+  </si>
+  <si>
+    <t>22 08 2020</t>
+  </si>
+  <si>
+    <t>23 08 2020</t>
+  </si>
+  <si>
+    <t>24 08 2020</t>
+  </si>
+  <si>
+    <t>25 08 2020</t>
+  </si>
 </sst>
 </file>
 
@@ -1110,7 +1134,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BE200"/>
+  <dimension ref="A1:BE208"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -18599,6 +18623,9 @@
       <c r="D102">
         <v>0.098665199888609</v>
       </c>
+      <c r="E102">
+        <v>0.14194139194139</v>
+      </c>
       <c r="F102">
         <v>0.066145254029257</v>
       </c>
@@ -18769,6 +18796,9 @@
       <c r="D103">
         <v>0.087751753367354</v>
       </c>
+      <c r="E103">
+        <v>0.10008250938702</v>
+      </c>
       <c r="F103">
         <v>0.070547024140013</v>
       </c>
@@ -18939,6 +18969,9 @@
       <c r="D104">
         <v>0.082878999776223</v>
       </c>
+      <c r="E104">
+        <v>0.095548433048433</v>
+      </c>
       <c r="F104">
         <v>0.056507058339688</v>
       </c>
@@ -19109,6 +19142,9 @@
       <c r="D105">
         <v>0.097774086486332</v>
       </c>
+      <c r="E105">
+        <v>0.11482371794872</v>
+      </c>
       <c r="F105">
         <v>0.068388565678928</v>
       </c>
@@ -19279,6 +19315,9 @@
       <c r="D106">
         <v>0.082252377347177</v>
       </c>
+      <c r="E106">
+        <v>0.10073339359054</v>
+      </c>
       <c r="F106">
         <v>0.073144274854496</v>
       </c>
@@ -19449,6 +19488,9 @@
       <c r="D107">
         <v>0.051033280399833</v>
       </c>
+      <c r="E107">
+        <v>0.09259734196709</v>
+      </c>
       <c r="F107">
         <v>0.049024498394575</v>
       </c>
@@ -19619,6 +19661,9 @@
       <c r="D108">
         <v>0.052403806904704</v>
       </c>
+      <c r="E108">
+        <v>0.1580266955267</v>
+      </c>
       <c r="F108">
         <v>0.053647497238845</v>
       </c>
@@ -19789,6 +19834,9 @@
       <c r="D109">
         <v>0.10529471838662</v>
       </c>
+      <c r="E109">
+        <v>0.12866459520871</v>
+      </c>
       <c r="F109">
         <v>0.07542024767002201</v>
       </c>
@@ -34570,25 +34618,1385 @@
       <c r="A196" t="s">
         <v>250</v>
       </c>
+      <c r="B196">
+        <v>0.098697245679758</v>
+      </c>
+      <c r="C196">
+        <v>0.1137299179679</v>
+      </c>
+      <c r="D196">
+        <v>0.10647357868045</v>
+      </c>
+      <c r="F196">
+        <v>0.07595608881833101</v>
+      </c>
+      <c r="G196">
+        <v>0.086410320888114</v>
+      </c>
+      <c r="H196">
+        <v>0.09323298190294101</v>
+      </c>
+      <c r="I196">
+        <v>0.075868037942508</v>
+      </c>
+      <c r="J196">
+        <v>0.059826022859128</v>
+      </c>
+      <c r="K196">
+        <v>0.074018621552456</v>
+      </c>
+      <c r="L196">
+        <v>0.082503149283964</v>
+      </c>
+      <c r="M196">
+        <v>0.098355526485546</v>
+      </c>
+      <c r="N196">
+        <v>0.097752315185876</v>
+      </c>
+      <c r="O196">
+        <v>0.087164378840229</v>
+      </c>
+      <c r="P196">
+        <v>0.10127680814298</v>
+      </c>
+      <c r="Q196">
+        <v>0.094223727882684</v>
+      </c>
+      <c r="R196">
+        <v>0.077911142016555</v>
+      </c>
+      <c r="S196">
+        <v>0.099644911766052</v>
+      </c>
+      <c r="T196">
+        <v>0.10219369163065</v>
+      </c>
+      <c r="U196">
+        <v>0.090156716702745</v>
+      </c>
+      <c r="V196">
+        <v>0.10496930387805</v>
+      </c>
+      <c r="W196">
+        <v>0.07343343231376701</v>
+      </c>
+      <c r="X196">
+        <v>0.065090007174696</v>
+      </c>
+      <c r="Y196">
+        <v>0.079255835622668</v>
+      </c>
+      <c r="Z196">
+        <v>0.080182131763926</v>
+      </c>
+      <c r="AA196">
+        <v>0.077056875604765</v>
+      </c>
+      <c r="AB196">
+        <v>0.095151141830153</v>
+      </c>
+      <c r="AC196">
+        <v>0.096608718104137</v>
+      </c>
+      <c r="AD196">
+        <v>0.12094002288507</v>
+      </c>
+      <c r="AE196">
+        <v>0.10311759734884</v>
+      </c>
+      <c r="AF196">
+        <v>0.097596705009587</v>
+      </c>
+      <c r="AG196">
+        <v>0.10003188087643</v>
+      </c>
+      <c r="AH196">
+        <v>0.1189699721368</v>
+      </c>
+      <c r="AI196">
+        <v>0.084207626207213</v>
+      </c>
+      <c r="AJ196">
+        <v>0.07410050520744101</v>
+      </c>
+      <c r="AK196">
+        <v>0.09611812667844</v>
+      </c>
+      <c r="AL196">
+        <v>0.081699353296579</v>
+      </c>
+      <c r="AM196">
+        <v>0.077360804436755</v>
+      </c>
+      <c r="AN196">
+        <v>0.08576245943762301</v>
+      </c>
+      <c r="AO196">
+        <v>0.11481027199678</v>
+      </c>
+      <c r="AP196">
+        <v>0.08213115283049099</v>
+      </c>
+      <c r="AQ196">
+        <v>0.074082035853151</v>
+      </c>
+      <c r="AR196">
+        <v>0.08922991753260399</v>
+      </c>
+      <c r="AS196">
+        <v>0.076514276129604</v>
+      </c>
+      <c r="AT196">
+        <v>0.09974748394166399</v>
+      </c>
+      <c r="AU196">
+        <v>0.10897298424458</v>
+      </c>
+      <c r="AV196">
+        <v>0.10396705778722</v>
+      </c>
+      <c r="AW196">
+        <v>0.09656112316695099</v>
+      </c>
+      <c r="AX196">
+        <v>0.10754257921973</v>
+      </c>
+      <c r="AY196">
+        <v>0.080818486458665</v>
+      </c>
+      <c r="AZ196">
+        <v>0.086706317645374</v>
+      </c>
+      <c r="BA196">
+        <v>0.084476657202642</v>
+      </c>
+      <c r="BB196">
+        <v>0.08266032711785801</v>
+      </c>
+      <c r="BC196">
+        <v>0.084958049625365</v>
+      </c>
+      <c r="BD196">
+        <v>0.08538715690083699</v>
+      </c>
+      <c r="BE196">
+        <v>0.11608924909441</v>
+      </c>
     </row>
     <row r="197" spans="1:57">
       <c r="A197" t="s">
         <v>251</v>
       </c>
+      <c r="B197">
+        <v>0.079985668592953</v>
+      </c>
+      <c r="C197">
+        <v>0.10744065815235</v>
+      </c>
+      <c r="D197">
+        <v>0.10691391015506</v>
+      </c>
+      <c r="F197">
+        <v>0.073145876243445</v>
+      </c>
+      <c r="G197">
+        <v>0.08933891163201101</v>
+      </c>
+      <c r="H197">
+        <v>0.086112250362744</v>
+      </c>
+      <c r="I197">
+        <v>0.06747380393324801</v>
+      </c>
+      <c r="J197">
+        <v>0.053091254584579</v>
+      </c>
+      <c r="K197">
+        <v>0.066584690931187</v>
+      </c>
+      <c r="L197">
+        <v>0.075271757128658</v>
+      </c>
+      <c r="M197">
+        <v>0.095120806328862</v>
+      </c>
+      <c r="N197">
+        <v>0.078001461063379</v>
+      </c>
+      <c r="O197">
+        <v>0.08558094942945101</v>
+      </c>
+      <c r="P197">
+        <v>0.09713093195335799</v>
+      </c>
+      <c r="Q197">
+        <v>0.092106193460174</v>
+      </c>
+      <c r="R197">
+        <v>0.07600537811480999</v>
+      </c>
+      <c r="S197">
+        <v>0.096651444042886</v>
+      </c>
+      <c r="T197">
+        <v>0.099692760497851</v>
+      </c>
+      <c r="U197">
+        <v>0.086207561783191</v>
+      </c>
+      <c r="V197">
+        <v>0.10340840746235</v>
+      </c>
+      <c r="W197">
+        <v>0.074589252000568</v>
+      </c>
+      <c r="X197">
+        <v>0.069819607653008</v>
+      </c>
+      <c r="Y197">
+        <v>0.08421062104428299</v>
+      </c>
+      <c r="Z197">
+        <v>0.073831172043359</v>
+      </c>
+      <c r="AA197">
+        <v>0.064471970953743</v>
+      </c>
+      <c r="AB197">
+        <v>0.082460035573669</v>
+      </c>
+      <c r="AC197">
+        <v>0.094832968161028</v>
+      </c>
+      <c r="AD197">
+        <v>0.11037837464918</v>
+      </c>
+      <c r="AE197">
+        <v>0.087931786901857</v>
+      </c>
+      <c r="AF197">
+        <v>0.090748894330929</v>
+      </c>
+      <c r="AG197">
+        <v>0.092766964890592</v>
+      </c>
+      <c r="AH197">
+        <v>0.10205404868298</v>
+      </c>
+      <c r="AI197">
+        <v>0.07165786761765899</v>
+      </c>
+      <c r="AJ197">
+        <v>0.062780009904739</v>
+      </c>
+      <c r="AK197">
+        <v>0.076179742715525</v>
+      </c>
+      <c r="AL197">
+        <v>0.06925677391624301</v>
+      </c>
+      <c r="AM197">
+        <v>0.064654603363047</v>
+      </c>
+      <c r="AN197">
+        <v>0.08230403737196899</v>
+      </c>
+      <c r="AO197">
+        <v>0.11426174541434</v>
+      </c>
+      <c r="AP197">
+        <v>0.08377114524785</v>
+      </c>
+      <c r="AQ197">
+        <v>0.075412066563236</v>
+      </c>
+      <c r="AR197">
+        <v>0.0806135629665</v>
+      </c>
+      <c r="AS197">
+        <v>0.077560471272941</v>
+      </c>
+      <c r="AT197">
+        <v>0.094027478985863</v>
+      </c>
+      <c r="AU197">
+        <v>0.10293084875022</v>
+      </c>
+      <c r="AV197">
+        <v>0.098530118407685</v>
+      </c>
+      <c r="AW197">
+        <v>0.087970409869295</v>
+      </c>
+      <c r="AX197">
+        <v>0.095001640281264</v>
+      </c>
+      <c r="AY197">
+        <v>0.071763481553572</v>
+      </c>
+      <c r="AZ197">
+        <v>0.077302046921089</v>
+      </c>
+      <c r="BA197">
+        <v>0.06940476255523099</v>
+      </c>
+      <c r="BB197">
+        <v>0.073731614242644</v>
+      </c>
+      <c r="BC197">
+        <v>0.07678344488408601</v>
+      </c>
+      <c r="BD197">
+        <v>0.075001991021621</v>
+      </c>
+      <c r="BE197">
+        <v>0.10296866235293</v>
+      </c>
     </row>
     <row r="198" spans="1:57">
       <c r="A198" t="s">
         <v>252</v>
       </c>
+      <c r="B198">
+        <v>0.057746316084178</v>
+      </c>
+      <c r="C198">
+        <v>0.07107292997990799</v>
+      </c>
+      <c r="D198">
+        <v>0.072248674245238</v>
+      </c>
+      <c r="F198">
+        <v>0.066518402174172</v>
+      </c>
+      <c r="G198">
+        <v>0.073891794299784</v>
+      </c>
+      <c r="H198">
+        <v>0.07955850826788</v>
+      </c>
+      <c r="I198">
+        <v>0.06413980633456599</v>
+      </c>
+      <c r="J198">
+        <v>0.056851056776184</v>
+      </c>
+      <c r="K198">
+        <v>0.06178206336592</v>
+      </c>
+      <c r="L198">
+        <v>0.05670042732095</v>
+      </c>
+      <c r="M198">
+        <v>0.053739752727762</v>
+      </c>
+      <c r="N198">
+        <v>0.061088285007213</v>
+      </c>
+      <c r="O198">
+        <v>0.053036624614265</v>
+      </c>
+      <c r="P198">
+        <v>0.069682655941137</v>
+      </c>
+      <c r="Q198">
+        <v>0.068038942674591</v>
+      </c>
+      <c r="R198">
+        <v>0.054298005784899</v>
+      </c>
+      <c r="S198">
+        <v>0.059789468140483</v>
+      </c>
+      <c r="T198">
+        <v>0.062500420204661</v>
+      </c>
+      <c r="U198">
+        <v>0.0589705957957</v>
+      </c>
+      <c r="V198">
+        <v>0.065458277939177</v>
+      </c>
+      <c r="W198">
+        <v>0.055726042160639</v>
+      </c>
+      <c r="X198">
+        <v>0.050341298049364</v>
+      </c>
+      <c r="Y198">
+        <v>0.061111424299957</v>
+      </c>
+      <c r="Z198">
+        <v>0.053326898711915</v>
+      </c>
+      <c r="AA198">
+        <v>0.052080981540569</v>
+      </c>
+      <c r="AB198">
+        <v>0.060000726940659</v>
+      </c>
+      <c r="AC198">
+        <v>0.07991922487132</v>
+      </c>
+      <c r="AD198">
+        <v>0.061598430109882</v>
+      </c>
+      <c r="AE198">
+        <v>0.070800330169106</v>
+      </c>
+      <c r="AF198">
+        <v>0.053385290147881</v>
+      </c>
+      <c r="AG198">
+        <v>0.060659555829506</v>
+      </c>
+      <c r="AH198">
+        <v>0.064366418362426</v>
+      </c>
+      <c r="AI198">
+        <v>0.05837748870877</v>
+      </c>
+      <c r="AJ198">
+        <v>0.054689376779261</v>
+      </c>
+      <c r="AK198">
+        <v>0.067062475962521</v>
+      </c>
+      <c r="AL198">
+        <v>0.059553116068583</v>
+      </c>
+      <c r="AM198">
+        <v>0.055745140540474</v>
+      </c>
+      <c r="AN198">
+        <v>0.056115939455002</v>
+      </c>
+      <c r="AO198">
+        <v>0.064246271956306</v>
+      </c>
+      <c r="AP198">
+        <v>0.0660467979044</v>
+      </c>
+      <c r="AQ198">
+        <v>0.057150474757797</v>
+      </c>
+      <c r="AR198">
+        <v>0.06577077210022</v>
+      </c>
+      <c r="AS198">
+        <v>0.05958981905244</v>
+      </c>
+      <c r="AT198">
+        <v>0.060405259590669</v>
+      </c>
+      <c r="AU198">
+        <v>0.07014536062087701</v>
+      </c>
+      <c r="AV198">
+        <v>0.059604066037247</v>
+      </c>
+      <c r="AW198">
+        <v>0.056159974731519</v>
+      </c>
+      <c r="AX198">
+        <v>0.072981724762386</v>
+      </c>
+      <c r="AY198">
+        <v>0.044311193614133</v>
+      </c>
+      <c r="AZ198">
+        <v>0.062497878986658</v>
+      </c>
+      <c r="BA198">
+        <v>0.050996439065134</v>
+      </c>
+      <c r="BB198">
+        <v>0.055978831417392</v>
+      </c>
+      <c r="BC198">
+        <v>0.053145283164567</v>
+      </c>
+      <c r="BD198">
+        <v>0.04471324630965</v>
+      </c>
+      <c r="BE198">
+        <v>0.067488595624789</v>
+      </c>
     </row>
     <row r="199" spans="1:57">
       <c r="A199" t="s">
         <v>253</v>
       </c>
+      <c r="B199">
+        <v>0.090577082105758</v>
+      </c>
+      <c r="C199">
+        <v>0.065118432656828</v>
+      </c>
+      <c r="D199">
+        <v>0.062825709734683</v>
+      </c>
+      <c r="F199">
+        <v>0.073555559063533</v>
+      </c>
+      <c r="G199">
+        <v>0.057092136349849</v>
+      </c>
+      <c r="H199">
+        <v>0.059219200398814</v>
+      </c>
+      <c r="I199">
+        <v>0.040169706731656</v>
+      </c>
+      <c r="J199">
+        <v>0.043694011754975</v>
+      </c>
+      <c r="K199">
+        <v>0.036895395718438</v>
+      </c>
+      <c r="L199">
+        <v>0.044143753772746</v>
+      </c>
+      <c r="M199">
+        <v>0.046830117423561</v>
+      </c>
+      <c r="N199">
+        <v>0.078287940966648</v>
+      </c>
+      <c r="O199">
+        <v>0.050456313827705</v>
+      </c>
+      <c r="P199">
+        <v>0.05590309365537</v>
+      </c>
+      <c r="Q199">
+        <v>0.06298915054661</v>
+      </c>
+      <c r="R199">
+        <v>0.05174704845061</v>
+      </c>
+      <c r="S199">
+        <v>0.051299047614377</v>
+      </c>
+      <c r="T199">
+        <v>0.050180516026672</v>
+      </c>
+      <c r="U199">
+        <v>0.047933644398543</v>
+      </c>
+      <c r="V199">
+        <v>0.054243020843947</v>
+      </c>
+      <c r="W199">
+        <v>0.046241341486769</v>
+      </c>
+      <c r="X199">
+        <v>0.03954735561804</v>
+      </c>
+      <c r="Y199">
+        <v>0.050104726812685</v>
+      </c>
+      <c r="Z199">
+        <v>0.043577108514576</v>
+      </c>
+      <c r="AA199">
+        <v>0.042942651846122</v>
+      </c>
+      <c r="AB199">
+        <v>0.050912497455641</v>
+      </c>
+      <c r="AC199">
+        <v>0.09529848405251901</v>
+      </c>
+      <c r="AD199">
+        <v>0.052246982222475</v>
+      </c>
+      <c r="AE199">
+        <v>0.058862254462461</v>
+      </c>
+      <c r="AF199">
+        <v>0.045188471150507</v>
+      </c>
+      <c r="AG199">
+        <v>0.047057344404957</v>
+      </c>
+      <c r="AH199">
+        <v>0.048784984472795</v>
+      </c>
+      <c r="AI199">
+        <v>0.045863517624138</v>
+      </c>
+      <c r="AJ199">
+        <v>0.037702160835375</v>
+      </c>
+      <c r="AK199">
+        <v>0.057857565183644</v>
+      </c>
+      <c r="AL199">
+        <v>0.052202289281095</v>
+      </c>
+      <c r="AM199">
+        <v>0.04349928238478</v>
+      </c>
+      <c r="AN199">
+        <v>0.045035876256642</v>
+      </c>
+      <c r="AO199">
+        <v>0.050569009057285</v>
+      </c>
+      <c r="AP199">
+        <v>0.052703910423396</v>
+      </c>
+      <c r="AQ199">
+        <v>0.043091344753512</v>
+      </c>
+      <c r="AR199">
+        <v>0.07568037103577301</v>
+      </c>
+      <c r="AS199">
+        <v>0.046276470260031</v>
+      </c>
+      <c r="AT199">
+        <v>0.051256032011896</v>
+      </c>
+      <c r="AU199">
+        <v>0.055592760153891</v>
+      </c>
+      <c r="AV199">
+        <v>0.053391860276097</v>
+      </c>
+      <c r="AW199">
+        <v>0.049872002604374</v>
+      </c>
+      <c r="AX199">
+        <v>0.065774411619423</v>
+      </c>
+      <c r="AY199">
+        <v>0.048448995494785</v>
+      </c>
+      <c r="AZ199">
+        <v>0.064814586531452</v>
+      </c>
+      <c r="BA199">
+        <v>0.060662892697297</v>
+      </c>
+      <c r="BB199">
+        <v>0.063500185831175</v>
+      </c>
+      <c r="BC199">
+        <v>0.055700611212118</v>
+      </c>
+      <c r="BD199">
+        <v>0.051905488586423</v>
+      </c>
+      <c r="BE199">
+        <v>0.069936782311633</v>
+      </c>
     </row>
     <row r="200" spans="1:57">
       <c r="A200" t="s">
         <v>254</v>
+      </c>
+      <c r="B200">
+        <v>0.10286997217635</v>
+      </c>
+      <c r="C200">
+        <v>0.11889032943269</v>
+      </c>
+      <c r="D200">
+        <v>0.12470553140788</v>
+      </c>
+      <c r="F200">
+        <v>0.09063603059596501</v>
+      </c>
+      <c r="G200">
+        <v>0.078602937454942</v>
+      </c>
+      <c r="H200">
+        <v>0.09229282537429299</v>
+      </c>
+      <c r="I200">
+        <v>0.070736919510303</v>
+      </c>
+      <c r="J200">
+        <v>0.053986478200076</v>
+      </c>
+      <c r="K200">
+        <v>0.07104028597925199</v>
+      </c>
+      <c r="L200">
+        <v>0.07422293909957201</v>
+      </c>
+      <c r="M200">
+        <v>0.09487554020059601</v>
+      </c>
+      <c r="N200">
+        <v>0.080294041012746</v>
+      </c>
+      <c r="O200">
+        <v>0.08747424389983199</v>
+      </c>
+      <c r="P200">
+        <v>0.10315534029892</v>
+      </c>
+      <c r="Q200">
+        <v>0.095906792491058</v>
+      </c>
+      <c r="R200">
+        <v>0.081247066093002</v>
+      </c>
+      <c r="S200">
+        <v>0.1023226018617</v>
+      </c>
+      <c r="T200">
+        <v>0.10524252483979</v>
+      </c>
+      <c r="U200">
+        <v>0.09402798268571699</v>
+      </c>
+      <c r="V200">
+        <v>0.10457547182393</v>
+      </c>
+      <c r="W200">
+        <v>0.06434483083666</v>
+      </c>
+      <c r="X200">
+        <v>0.06655259646822501</v>
+      </c>
+      <c r="Y200">
+        <v>0.079389327466987</v>
+      </c>
+      <c r="Z200">
+        <v>0.071314435720959</v>
+      </c>
+      <c r="AA200">
+        <v>0.071476118350542</v>
+      </c>
+      <c r="AB200">
+        <v>0.09070942650203601</v>
+      </c>
+      <c r="AC200">
+        <v>0.096153311620603</v>
+      </c>
+      <c r="AD200">
+        <v>0.12137049952485</v>
+      </c>
+      <c r="AE200">
+        <v>0.09819374842784399</v>
+      </c>
+      <c r="AF200">
+        <v>0.092943654071677</v>
+      </c>
+      <c r="AG200">
+        <v>0.10154846855319</v>
+      </c>
+      <c r="AH200">
+        <v>0.11204554855825</v>
+      </c>
+      <c r="AI200">
+        <v>0.07664237578413</v>
+      </c>
+      <c r="AJ200">
+        <v>0.071340979114111</v>
+      </c>
+      <c r="AK200">
+        <v>0.085616121964182</v>
+      </c>
+      <c r="AL200">
+        <v>0.07461085007707</v>
+      </c>
+      <c r="AM200">
+        <v>0.070808291361196</v>
+      </c>
+      <c r="AN200">
+        <v>0.08136163741883599</v>
+      </c>
+      <c r="AO200">
+        <v>0.11088264667628</v>
+      </c>
+      <c r="AP200">
+        <v>0.076124473908983</v>
+      </c>
+      <c r="AQ200">
+        <v>0.067936370905698</v>
+      </c>
+      <c r="AR200">
+        <v>0.086724422215594</v>
+      </c>
+      <c r="AS200">
+        <v>0.06714068881367399</v>
+      </c>
+      <c r="AT200">
+        <v>0.094953302737304</v>
+      </c>
+      <c r="AU200">
+        <v>0.10150626433664</v>
+      </c>
+      <c r="AV200">
+        <v>0.097291439052863</v>
+      </c>
+      <c r="AW200">
+        <v>0.087267520930967</v>
+      </c>
+      <c r="AX200">
+        <v>0.10117582291113</v>
+      </c>
+      <c r="AY200">
+        <v>0.07884668518374401</v>
+      </c>
+      <c r="AZ200">
+        <v>0.09062730389757399</v>
+      </c>
+      <c r="BA200">
+        <v>0.069065069109446</v>
+      </c>
+      <c r="BB200">
+        <v>0.078102675677075</v>
+      </c>
+      <c r="BC200">
+        <v>0.080290626200215</v>
+      </c>
+      <c r="BD200">
+        <v>0.084639145040181</v>
+      </c>
+      <c r="BE200">
+        <v>0.11079753748433</v>
+      </c>
+    </row>
+    <row r="201" spans="1:57">
+      <c r="A201" t="s">
+        <v>255</v>
+      </c>
+      <c r="B201">
+        <v>0.090062751126906</v>
+      </c>
+      <c r="C201">
+        <v>0.13018861257895</v>
+      </c>
+      <c r="D201">
+        <v>0.11068785495577</v>
+      </c>
+      <c r="F201">
+        <v>0.07141492088857999</v>
+      </c>
+      <c r="G201">
+        <v>0.082401451730211</v>
+      </c>
+      <c r="H201">
+        <v>0.09791813333874599</v>
+      </c>
+      <c r="I201">
+        <v>0.078499019029499</v>
+      </c>
+      <c r="J201">
+        <v>0.060203039225373</v>
+      </c>
+      <c r="K201">
+        <v>0.078778113872348</v>
+      </c>
+      <c r="L201">
+        <v>0.084088695867754</v>
+      </c>
+      <c r="M201">
+        <v>0.10047219594801</v>
+      </c>
+      <c r="N201">
+        <v>0.079947058870334</v>
+      </c>
+      <c r="O201">
+        <v>0.093154421958818</v>
+      </c>
+      <c r="P201">
+        <v>0.10560718237179</v>
+      </c>
+      <c r="Q201">
+        <v>0.10061164902327</v>
+      </c>
+      <c r="R201">
+        <v>0.081779533369202</v>
+      </c>
+      <c r="S201">
+        <v>0.1004684812838</v>
+      </c>
+      <c r="T201">
+        <v>0.10933629113448</v>
+      </c>
+      <c r="U201">
+        <v>0.09667024325196601</v>
+      </c>
+      <c r="V201">
+        <v>0.11049134522446</v>
+      </c>
+      <c r="W201">
+        <v>0.080269526502166</v>
+      </c>
+      <c r="X201">
+        <v>0.07540819165431401</v>
+      </c>
+      <c r="Y201">
+        <v>0.082833100844726</v>
+      </c>
+      <c r="Z201">
+        <v>0.08602948330068499</v>
+      </c>
+      <c r="AA201">
+        <v>0.085245168123467</v>
+      </c>
+      <c r="AB201">
+        <v>0.10158093398627</v>
+      </c>
+      <c r="AC201">
+        <v>0.08301412539154999</v>
+      </c>
+      <c r="AD201">
+        <v>0.13261449037126</v>
+      </c>
+      <c r="AE201">
+        <v>0.10951152595262</v>
+      </c>
+      <c r="AF201">
+        <v>0.095674883517085</v>
+      </c>
+      <c r="AG201">
+        <v>0.10268398714434</v>
+      </c>
+      <c r="AH201">
+        <v>0.12223344683311</v>
+      </c>
+      <c r="AI201">
+        <v>0.078712240935728</v>
+      </c>
+      <c r="AJ201">
+        <v>0.077426656099132</v>
+      </c>
+      <c r="AK201">
+        <v>0.092789363146052</v>
+      </c>
+      <c r="AL201">
+        <v>0.085365512327275</v>
+      </c>
+      <c r="AM201">
+        <v>0.07281033648228601</v>
+      </c>
+      <c r="AN201">
+        <v>0.08400012147862999</v>
+      </c>
+      <c r="AO201">
+        <v>0.11981438917753</v>
+      </c>
+      <c r="AP201">
+        <v>0.085389162210881</v>
+      </c>
+      <c r="AQ201">
+        <v>0.07537814878065301</v>
+      </c>
+      <c r="AR201">
+        <v>0.084523702809429</v>
+      </c>
+      <c r="AS201">
+        <v>0.076840418476291</v>
+      </c>
+      <c r="AT201">
+        <v>0.099198208863103</v>
+      </c>
+      <c r="AU201">
+        <v>0.10944418545801</v>
+      </c>
+      <c r="AV201">
+        <v>0.103961782343</v>
+      </c>
+      <c r="AW201">
+        <v>0.09246127865708299</v>
+      </c>
+      <c r="AX201">
+        <v>0.10598983367165</v>
+      </c>
+      <c r="AY201">
+        <v>0.076823316148667</v>
+      </c>
+      <c r="AZ201">
+        <v>0.085256380237016</v>
+      </c>
+      <c r="BA201">
+        <v>0.074065893181972</v>
+      </c>
+      <c r="BB201">
+        <v>0.076781589336701</v>
+      </c>
+      <c r="BC201">
+        <v>0.080478664606078</v>
+      </c>
+      <c r="BD201">
+        <v>0.079479681728579</v>
+      </c>
+      <c r="BE201">
+        <v>0.1143210727315</v>
+      </c>
+    </row>
+    <row r="202" spans="1:57">
+      <c r="A202" t="s">
+        <v>256</v>
+      </c>
+      <c r="B202">
+        <v>0.086683436125654</v>
+      </c>
+      <c r="C202">
+        <v>0.11857231880763</v>
+      </c>
+      <c r="D202">
+        <v>0.11230022432776</v>
+      </c>
+      <c r="F202">
+        <v>0.07261398328438599</v>
+      </c>
+      <c r="G202">
+        <v>0.076294198253509</v>
+      </c>
+      <c r="H202">
+        <v>0.09733903715874501</v>
+      </c>
+      <c r="I202">
+        <v>0.07330554994326199</v>
+      </c>
+      <c r="J202">
+        <v>0.052293909952121</v>
+      </c>
+      <c r="K202">
+        <v>0.073195843306349</v>
+      </c>
+      <c r="L202">
+        <v>0.078105498176135</v>
+      </c>
+      <c r="M202">
+        <v>0.097078589764603</v>
+      </c>
+      <c r="N202">
+        <v>0.08243417866476099</v>
+      </c>
+      <c r="O202">
+        <v>0.084397524517274</v>
+      </c>
+      <c r="P202">
+        <v>0.099699228387269</v>
+      </c>
+      <c r="Q202">
+        <v>0.097210879126329</v>
+      </c>
+      <c r="R202">
+        <v>0.079747432456651</v>
+      </c>
+      <c r="S202">
+        <v>0.097954922321357</v>
+      </c>
+      <c r="T202">
+        <v>0.10231579962529</v>
+      </c>
+      <c r="U202">
+        <v>0.08775308230412</v>
+      </c>
+      <c r="V202">
+        <v>0.098128717440641</v>
+      </c>
+      <c r="W202">
+        <v>0.060447616145256</v>
+      </c>
+      <c r="X202">
+        <v>0.057872305618277</v>
+      </c>
+      <c r="Y202">
+        <v>0.073343665263296</v>
+      </c>
+      <c r="Z202">
+        <v>0.068208502553447</v>
+      </c>
+      <c r="AA202">
+        <v>0.068268087289289</v>
+      </c>
+      <c r="AB202">
+        <v>0.089117347262766</v>
+      </c>
+      <c r="AC202">
+        <v>0.09443602976581</v>
+      </c>
+      <c r="AD202">
+        <v>0.11790649917505</v>
+      </c>
+      <c r="AE202">
+        <v>0.09407926078838399</v>
+      </c>
+      <c r="AF202">
+        <v>0.09316493664698999</v>
+      </c>
+      <c r="AG202">
+        <v>0.10673683803586</v>
+      </c>
+      <c r="AH202">
+        <v>0.11260676415615</v>
+      </c>
+      <c r="AI202">
+        <v>0.073531701692677</v>
+      </c>
+      <c r="AJ202">
+        <v>0.06428849829175901</v>
+      </c>
+      <c r="AK202">
+        <v>0.083358082119907</v>
+      </c>
+      <c r="AL202">
+        <v>0.072050339402658</v>
+      </c>
+      <c r="AM202">
+        <v>0.066082513957069</v>
+      </c>
+      <c r="AN202">
+        <v>0.085061808334692</v>
+      </c>
+      <c r="AO202">
+        <v>0.12105849433739</v>
+      </c>
+      <c r="AP202">
+        <v>0.083858703242684</v>
+      </c>
+      <c r="AQ202">
+        <v>0.075879633127841</v>
+      </c>
+      <c r="AR202">
+        <v>0.088542698323523</v>
+      </c>
+      <c r="AS202">
+        <v>0.077173916066099</v>
+      </c>
+      <c r="AT202">
+        <v>0.1035881979863</v>
+      </c>
+      <c r="AU202">
+        <v>0.11868820244423</v>
+      </c>
+      <c r="AV202">
+        <v>0.10753762798302</v>
+      </c>
+      <c r="AW202">
+        <v>0.09718218163959499</v>
+      </c>
+      <c r="AX202">
+        <v>0.11290615352689</v>
+      </c>
+      <c r="AY202">
+        <v>0.08002883793103301</v>
+      </c>
+      <c r="AZ202">
+        <v>0.080299300918386</v>
+      </c>
+      <c r="BA202">
+        <v>0.082367932649315</v>
+      </c>
+      <c r="BB202">
+        <v>0.081845263352769</v>
+      </c>
+      <c r="BC202">
+        <v>0.084374972275683</v>
+      </c>
+      <c r="BD202">
+        <v>0.085663844503337</v>
+      </c>
+      <c r="BE202">
+        <v>0.11862635525065</v>
+      </c>
+    </row>
+    <row r="203" spans="1:57">
+      <c r="A203" t="s">
+        <v>257</v>
+      </c>
+      <c r="B203">
+        <v>0.083477057524132</v>
+      </c>
+      <c r="C203">
+        <v>0.11576493614048</v>
+      </c>
+      <c r="D203">
+        <v>0.11326763177968</v>
+      </c>
+      <c r="F203">
+        <v>0.07386616564497001</v>
+      </c>
+      <c r="G203">
+        <v>0.074107166486769</v>
+      </c>
+      <c r="H203">
+        <v>0.09189759199757599</v>
+      </c>
+      <c r="I203">
+        <v>0.072505303284519</v>
+      </c>
+      <c r="J203">
+        <v>0.056017825137149</v>
+      </c>
+      <c r="K203">
+        <v>0.073468334609483</v>
+      </c>
+      <c r="L203">
+        <v>0.07819077846306099</v>
+      </c>
+      <c r="M203">
+        <v>0.09825525180514399</v>
+      </c>
+      <c r="N203">
+        <v>0.084800780306686</v>
+      </c>
+      <c r="O203">
+        <v>0.087604019712652</v>
+      </c>
+      <c r="P203">
+        <v>0.1076652948446</v>
+      </c>
+      <c r="Q203">
+        <v>0.099649245096013</v>
+      </c>
+      <c r="R203">
+        <v>0.085247451834206</v>
+      </c>
+      <c r="S203">
+        <v>0.10391812993348</v>
+      </c>
+      <c r="T203">
+        <v>0.11028956775354</v>
+      </c>
+      <c r="U203">
+        <v>0.09672917542569701</v>
+      </c>
+      <c r="V203">
+        <v>0.10951542590527</v>
+      </c>
+      <c r="W203">
+        <v>0.075979419905201</v>
+      </c>
+      <c r="X203">
+        <v>0.072387291463912</v>
+      </c>
+      <c r="Y203">
+        <v>0.084317556537754</v>
+      </c>
+      <c r="Z203">
+        <v>0.07863990550274801</v>
+      </c>
+      <c r="AA203">
+        <v>0.07468500291474001</v>
+      </c>
+      <c r="AB203">
+        <v>0.095373000376135</v>
+      </c>
+      <c r="AC203">
+        <v>0.10204907504468</v>
+      </c>
+      <c r="AD203">
+        <v>0.12593344728701</v>
+      </c>
+      <c r="AE203">
+        <v>0.098803212993146</v>
+      </c>
+      <c r="AF203">
+        <v>0.096843483550083</v>
+      </c>
+      <c r="AG203">
+        <v>0.10443537014127</v>
+      </c>
+      <c r="AH203">
+        <v>0.11898656592657</v>
+      </c>
+      <c r="AI203">
+        <v>0.077316706289853</v>
+      </c>
+      <c r="AJ203">
+        <v>0.071954485115357</v>
+      </c>
+      <c r="AK203">
+        <v>0.084407132611602</v>
+      </c>
+      <c r="AL203">
+        <v>0.077161940176861</v>
+      </c>
+      <c r="AM203">
+        <v>0.071433547368074</v>
+      </c>
+      <c r="AN203">
+        <v>0.091503745254021</v>
+      </c>
+      <c r="AO203">
+        <v>0.12502724867919</v>
+      </c>
+      <c r="AP203">
+        <v>0.091168775362924</v>
+      </c>
+      <c r="AQ203">
+        <v>0.08273450067520501</v>
+      </c>
+      <c r="AR203">
+        <v>0.089715163025987</v>
+      </c>
+      <c r="AS203">
+        <v>0.082902261927962</v>
+      </c>
+      <c r="AT203">
+        <v>0.10432594077709</v>
+      </c>
+      <c r="AU203">
+        <v>0.11926625380325</v>
+      </c>
+      <c r="AV203">
+        <v>0.10791388245505</v>
+      </c>
+      <c r="AW203">
+        <v>0.09664066380407201</v>
+      </c>
+      <c r="AX203">
+        <v>0.10827071625145</v>
+      </c>
+      <c r="AY203">
+        <v>0.07952447560445799</v>
+      </c>
+      <c r="AZ203">
+        <v>0.083462576466415</v>
+      </c>
+      <c r="BA203">
+        <v>0.073739853513361</v>
+      </c>
+      <c r="BB203">
+        <v>0.078603919220867</v>
+      </c>
+      <c r="BC203">
+        <v>0.082149867479439</v>
+      </c>
+      <c r="BD203">
+        <v>0.085863891605662</v>
+      </c>
+      <c r="BE203">
+        <v>0.1150908168307</v>
+      </c>
+    </row>
+    <row r="204" spans="1:57">
+      <c r="A204" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="205" spans="1:57">
+      <c r="A205" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="206" spans="1:57">
+      <c r="A206" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="207" spans="1:57">
+      <c r="A207" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="208" spans="1:57">
+      <c r="A208" t="s">
+        <v>262</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data up to 7th
</commit_message>
<xml_diff>
--- a/away3-6hours.xlsx
+++ b/away3-6hours.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="276">
   <si>
     <t>Alaska</t>
   </si>
@@ -825,6 +825,24 @@
   <si>
     <t>01 09 2020</t>
   </si>
+  <si>
+    <t>02 09 2020</t>
+  </si>
+  <si>
+    <t>03 09 2020</t>
+  </si>
+  <si>
+    <t>04 09 2020</t>
+  </si>
+  <si>
+    <t>05 09 2020</t>
+  </si>
+  <si>
+    <t>06 09 2020</t>
+  </si>
+  <si>
+    <t>07 09 2020</t>
+  </si>
 </sst>
 </file>
 
@@ -1155,7 +1173,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BE215"/>
+  <dimension ref="A1:BE221"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -21239,6 +21257,9 @@
       <c r="D117">
         <v>0.09347407579316599</v>
       </c>
+      <c r="E117">
+        <v>0.11989087301587</v>
+      </c>
       <c r="F117">
         <v>0.073114996334344</v>
       </c>
@@ -21409,6 +21430,9 @@
       <c r="D118">
         <v>0.097691498468344</v>
       </c>
+      <c r="E118">
+        <v>0.1210729746444</v>
+      </c>
       <c r="F118">
         <v>0.070182841072106</v>
       </c>
@@ -21579,6 +21603,9 @@
       <c r="D119">
         <v>0.10062030700624</v>
       </c>
+      <c r="E119">
+        <v>0.11715888278388</v>
+      </c>
       <c r="F119">
         <v>0.08117727292926601</v>
       </c>
@@ -21749,6 +21776,9 @@
       <c r="D120">
         <v>0.092306498870283</v>
       </c>
+      <c r="E120">
+        <v>0.1140380713689</v>
+      </c>
       <c r="F120">
         <v>0.066283592065039</v>
       </c>
@@ -21919,6 +21949,9 @@
       <c r="D121">
         <v>0.057818688325361</v>
       </c>
+      <c r="E121">
+        <v>0.15305435305435</v>
+      </c>
       <c r="F121">
         <v>0.059465674946912</v>
       </c>
@@ -22089,6 +22122,9 @@
       <c r="D122">
         <v>0.048163755979489</v>
       </c>
+      <c r="E122">
+        <v>0.13011363636364</v>
+      </c>
       <c r="F122">
         <v>0.047777327168157</v>
       </c>
@@ -37210,25 +37246,1045 @@
       <c r="A211" t="s">
         <v>265</v>
       </c>
+      <c r="B211">
+        <v>0.091160503022997</v>
+      </c>
+      <c r="C211">
+        <v>0.14436631900024</v>
+      </c>
+      <c r="D211">
+        <v>0.13339322109074</v>
+      </c>
+      <c r="F211">
+        <v>0.076195584316284</v>
+      </c>
+      <c r="G211">
+        <v>0.079655343431943</v>
+      </c>
+      <c r="H211">
+        <v>0.09014129873695199</v>
+      </c>
+      <c r="I211">
+        <v>0.07448583955876401</v>
+      </c>
+      <c r="J211">
+        <v>0.055435220688306</v>
+      </c>
+      <c r="K211">
+        <v>0.072669419347552</v>
+      </c>
+      <c r="L211">
+        <v>0.085631755911595</v>
+      </c>
+      <c r="M211">
+        <v>0.10057078838248</v>
+      </c>
+      <c r="N211">
+        <v>0.074342342324696</v>
+      </c>
+      <c r="O211">
+        <v>0.079998866293551</v>
+      </c>
+      <c r="P211">
+        <v>0.12620138017397</v>
+      </c>
+      <c r="Q211">
+        <v>0.091820372021712</v>
+      </c>
+      <c r="R211">
+        <v>0.090557550574135</v>
+      </c>
+      <c r="S211">
+        <v>0.10046082487603</v>
+      </c>
+      <c r="T211">
+        <v>0.11770119834686</v>
+      </c>
+      <c r="U211">
+        <v>0.092837786185005</v>
+      </c>
+      <c r="V211">
+        <v>0.10024097294727</v>
+      </c>
+      <c r="W211">
+        <v>0.074180616050156</v>
+      </c>
+      <c r="X211">
+        <v>0.06859331304727399</v>
+      </c>
+      <c r="Y211">
+        <v>0.08378107244272801</v>
+      </c>
+      <c r="Z211">
+        <v>0.07640825037325601</v>
+      </c>
+      <c r="AA211">
+        <v>0.083058633495533</v>
+      </c>
+      <c r="AB211">
+        <v>0.11171896693013</v>
+      </c>
+      <c r="AC211">
+        <v>0.080958537659389</v>
+      </c>
+      <c r="AD211">
+        <v>0.13406335881384</v>
+      </c>
+      <c r="AE211">
+        <v>0.10404795648269</v>
+      </c>
+      <c r="AF211">
+        <v>0.09499580871857601</v>
+      </c>
+      <c r="AG211">
+        <v>0.11766561364629</v>
+      </c>
+      <c r="AH211">
+        <v>0.13098338384321</v>
+      </c>
+      <c r="AI211">
+        <v>0.08032110160457499</v>
+      </c>
+      <c r="AJ211">
+        <v>0.07111936328985601</v>
+      </c>
+      <c r="AK211">
+        <v>0.081329656390967</v>
+      </c>
+      <c r="AL211">
+        <v>0.072985260062744</v>
+      </c>
+      <c r="AM211">
+        <v>0.06938511668493499</v>
+      </c>
+      <c r="AN211">
+        <v>0.089518383531228</v>
+      </c>
+      <c r="AO211">
+        <v>0.13271075194164</v>
+      </c>
+      <c r="AP211">
+        <v>0.08017026410255</v>
+      </c>
+      <c r="AQ211">
+        <v>0.07833361304380999</v>
+      </c>
+      <c r="AR211">
+        <v>0.093474602193795</v>
+      </c>
+      <c r="AS211">
+        <v>0.077398519806433</v>
+      </c>
+      <c r="AT211">
+        <v>0.10431931920196</v>
+      </c>
+      <c r="AU211">
+        <v>0.1157254291327</v>
+      </c>
+      <c r="AV211">
+        <v>0.10851662129536</v>
+      </c>
+      <c r="AW211">
+        <v>0.1015695130062</v>
+      </c>
+      <c r="AX211">
+        <v>0.10237736269644</v>
+      </c>
+      <c r="AY211">
+        <v>0.08026388911283899</v>
+      </c>
+      <c r="AZ211">
+        <v>0.08438236306249799</v>
+      </c>
+      <c r="BA211">
+        <v>0.078667241037551</v>
+      </c>
+      <c r="BB211">
+        <v>0.07425457657885701</v>
+      </c>
+      <c r="BC211">
+        <v>0.09016508449786199</v>
+      </c>
+      <c r="BD211">
+        <v>0.087062263338543</v>
+      </c>
+      <c r="BE211">
+        <v>0.12200014425304</v>
+      </c>
     </row>
     <row r="212" spans="1:57">
       <c r="A212" t="s">
         <v>266</v>
       </c>
+      <c r="B212">
+        <v>0.090951197386741</v>
+      </c>
+      <c r="C212">
+        <v>0.08758286120105099</v>
+      </c>
+      <c r="D212">
+        <v>0.062972067285486</v>
+      </c>
+      <c r="F212">
+        <v>0.07041045652406</v>
+      </c>
+      <c r="G212">
+        <v>0.065406261182633</v>
+      </c>
+      <c r="H212">
+        <v>0.076029164488341</v>
+      </c>
+      <c r="I212">
+        <v>0.053305859523713</v>
+      </c>
+      <c r="J212">
+        <v>0.057072725191514</v>
+      </c>
+      <c r="K212">
+        <v>0.05025142372602</v>
+      </c>
+      <c r="L212">
+        <v>0.060464900833542</v>
+      </c>
+      <c r="M212">
+        <v>0.061134088780444</v>
+      </c>
+      <c r="N212">
+        <v>0.078113551412702</v>
+      </c>
+      <c r="O212">
+        <v>0.058203018989916</v>
+      </c>
+      <c r="P212">
+        <v>0.08194345058265699</v>
+      </c>
+      <c r="Q212">
+        <v>0.081017148120732</v>
+      </c>
+      <c r="R212">
+        <v>0.06612537465036999</v>
+      </c>
+      <c r="S212">
+        <v>0.069776258000011</v>
+      </c>
+      <c r="T212">
+        <v>0.067738229481469</v>
+      </c>
+      <c r="U212">
+        <v>0.06315890295990401</v>
+      </c>
+      <c r="V212">
+        <v>0.072873671189992</v>
+      </c>
+      <c r="W212">
+        <v>0.060806289260301</v>
+      </c>
+      <c r="X212">
+        <v>0.055684454400932</v>
+      </c>
+      <c r="Y212">
+        <v>0.065921316340589</v>
+      </c>
+      <c r="Z212">
+        <v>0.061284829809193</v>
+      </c>
+      <c r="AA212">
+        <v>0.063166379407987</v>
+      </c>
+      <c r="AB212">
+        <v>0.06608548506715201</v>
+      </c>
+      <c r="AC212">
+        <v>0.09257585688965</v>
+      </c>
+      <c r="AD212">
+        <v>0.068382585162341</v>
+      </c>
+      <c r="AE212">
+        <v>0.08500204559993101</v>
+      </c>
+      <c r="AF212">
+        <v>0.060089849847192</v>
+      </c>
+      <c r="AG212">
+        <v>0.06742910805406099</v>
+      </c>
+      <c r="AH212">
+        <v>0.07147337611197301</v>
+      </c>
+      <c r="AI212">
+        <v>0.056325042414266</v>
+      </c>
+      <c r="AJ212">
+        <v>0.053512799707223</v>
+      </c>
+      <c r="AK212">
+        <v>0.072649554829504</v>
+      </c>
+      <c r="AL212">
+        <v>0.066000410124539</v>
+      </c>
+      <c r="AM212">
+        <v>0.056674210318516</v>
+      </c>
+      <c r="AN212">
+        <v>0.060721426530042</v>
+      </c>
+      <c r="AO212">
+        <v>0.06614408514509799</v>
+      </c>
+      <c r="AP212">
+        <v>0.067952861541428</v>
+      </c>
+      <c r="AQ212">
+        <v>0.05761380441479</v>
+      </c>
+      <c r="AR212">
+        <v>0.078365516118098</v>
+      </c>
+      <c r="AS212">
+        <v>0.059780145915509</v>
+      </c>
+      <c r="AT212">
+        <v>0.066794749742853</v>
+      </c>
+      <c r="AU212">
+        <v>0.075138997330714</v>
+      </c>
+      <c r="AV212">
+        <v>0.06497745595587601</v>
+      </c>
+      <c r="AW212">
+        <v>0.063773778158527</v>
+      </c>
+      <c r="AX212">
+        <v>0.085816785680188</v>
+      </c>
+      <c r="AY212">
+        <v>0.057016068681163</v>
+      </c>
+      <c r="AZ212">
+        <v>0.077919078148626</v>
+      </c>
+      <c r="BA212">
+        <v>0.064957536278029</v>
+      </c>
+      <c r="BB212">
+        <v>0.070608385624934</v>
+      </c>
+      <c r="BC212">
+        <v>0.06758859925994599</v>
+      </c>
+      <c r="BD212">
+        <v>0.057423908629954</v>
+      </c>
+      <c r="BE212">
+        <v>0.09092787968611001</v>
+      </c>
     </row>
     <row r="213" spans="1:57">
       <c r="A213" t="s">
         <v>267</v>
       </c>
+      <c r="B213">
+        <v>0.07722624407013801</v>
+      </c>
+      <c r="C213">
+        <v>0.067096197876128</v>
+      </c>
+      <c r="D213">
+        <v>0.059141264201759</v>
+      </c>
+      <c r="F213">
+        <v>0.067077766015121</v>
+      </c>
+      <c r="G213">
+        <v>0.060404390416145</v>
+      </c>
+      <c r="H213">
+        <v>0.06945255468149</v>
+      </c>
+      <c r="I213">
+        <v>0.055854996843605</v>
+      </c>
+      <c r="J213">
+        <v>0.056943610039147</v>
+      </c>
+      <c r="K213">
+        <v>0.056038773538383</v>
+      </c>
+      <c r="L213">
+        <v>0.045288276575819</v>
+      </c>
+      <c r="M213">
+        <v>0.043992166265906</v>
+      </c>
+      <c r="N213">
+        <v>0.07307412363780499</v>
+      </c>
+      <c r="O213">
+        <v>0.042358668509701</v>
+      </c>
+      <c r="P213">
+        <v>0.053717656093572</v>
+      </c>
+      <c r="Q213">
+        <v>0.056438061336859</v>
+      </c>
+      <c r="R213">
+        <v>0.045243461177322</v>
+      </c>
+      <c r="S213">
+        <v>0.04927331248094</v>
+      </c>
+      <c r="T213">
+        <v>0.049759111914003</v>
+      </c>
+      <c r="U213">
+        <v>0.05050144465755</v>
+      </c>
+      <c r="V213">
+        <v>0.056654069903717</v>
+      </c>
+      <c r="W213">
+        <v>0.053407544393188</v>
+      </c>
+      <c r="X213">
+        <v>0.047112859460228</v>
+      </c>
+      <c r="Y213">
+        <v>0.054447320161754</v>
+      </c>
+      <c r="Z213">
+        <v>0.047451672553534</v>
+      </c>
+      <c r="AA213">
+        <v>0.046949716619034</v>
+      </c>
+      <c r="AB213">
+        <v>0.054513180395716</v>
+      </c>
+      <c r="AC213">
+        <v>0.10523050045389</v>
+      </c>
+      <c r="AD213">
+        <v>0.052748467118161</v>
+      </c>
+      <c r="AE213">
+        <v>0.06922123530356999</v>
+      </c>
+      <c r="AF213">
+        <v>0.056698457377588</v>
+      </c>
+      <c r="AG213">
+        <v>0.049359659957464</v>
+      </c>
+      <c r="AH213">
+        <v>0.05518243538945</v>
+      </c>
+      <c r="AI213">
+        <v>0.058959137951034</v>
+      </c>
+      <c r="AJ213">
+        <v>0.0609470348846</v>
+      </c>
+      <c r="AK213">
+        <v>0.073160574722023</v>
+      </c>
+      <c r="AL213">
+        <v>0.058551529823119</v>
+      </c>
+      <c r="AM213">
+        <v>0.06542034278386299</v>
+      </c>
+      <c r="AN213">
+        <v>0.05343725455796</v>
+      </c>
+      <c r="AO213">
+        <v>0.052123453206227</v>
+      </c>
+      <c r="AP213">
+        <v>0.052937494651485</v>
+      </c>
+      <c r="AQ213">
+        <v>0.04791699922931</v>
+      </c>
+      <c r="AR213">
+        <v>0.077067789750097</v>
+      </c>
+      <c r="AS213">
+        <v>0.051873171191007</v>
+      </c>
+      <c r="AT213">
+        <v>0.049215770417817</v>
+      </c>
+      <c r="AU213">
+        <v>0.049412890583126</v>
+      </c>
+      <c r="AV213">
+        <v>0.049276502889787</v>
+      </c>
+      <c r="AW213">
+        <v>0.043994961224885</v>
+      </c>
+      <c r="AX213">
+        <v>0.059352313894281</v>
+      </c>
+      <c r="AY213">
+        <v>0.048918282160112</v>
+      </c>
+      <c r="AZ213">
+        <v>0.071534246827664</v>
+      </c>
+      <c r="BA213">
+        <v>0.051746210459417</v>
+      </c>
+      <c r="BB213">
+        <v>0.054785301583838</v>
+      </c>
+      <c r="BC213">
+        <v>0.053578265765766</v>
+      </c>
+      <c r="BD213">
+        <v>0.051993929718068</v>
+      </c>
+      <c r="BE213">
+        <v>0.06964790790438</v>
+      </c>
     </row>
     <row r="214" spans="1:57">
       <c r="A214" t="s">
         <v>268</v>
       </c>
+      <c r="B214">
+        <v>0.10971337650102</v>
+      </c>
+      <c r="C214">
+        <v>0.12197129041411</v>
+      </c>
+      <c r="D214">
+        <v>0.13329526129196</v>
+      </c>
+      <c r="F214">
+        <v>0.09124387464455599</v>
+      </c>
+      <c r="G214">
+        <v>0.083448957641741</v>
+      </c>
+      <c r="H214">
+        <v>0.095053007095668</v>
+      </c>
+      <c r="I214">
+        <v>0.075845440622181</v>
+      </c>
+      <c r="J214">
+        <v>0.054481106411887</v>
+      </c>
+      <c r="K214">
+        <v>0.075766568996347</v>
+      </c>
+      <c r="L214">
+        <v>0.082280218300047</v>
+      </c>
+      <c r="M214">
+        <v>0.097933890305533</v>
+      </c>
+      <c r="N214">
+        <v>0.075901522605289</v>
+      </c>
+      <c r="O214">
+        <v>0.08494218147575799</v>
+      </c>
+      <c r="P214">
+        <v>0.11657017962912</v>
+      </c>
+      <c r="Q214">
+        <v>0.10608734384083</v>
+      </c>
+      <c r="R214">
+        <v>0.087088339936137</v>
+      </c>
+      <c r="S214">
+        <v>0.1028421199264</v>
+      </c>
+      <c r="T214">
+        <v>0.10611414069857</v>
+      </c>
+      <c r="U214">
+        <v>0.088201639025156</v>
+      </c>
+      <c r="V214">
+        <v>0.099828748559909</v>
+      </c>
+      <c r="W214">
+        <v>0.06690391354160199</v>
+      </c>
+      <c r="X214">
+        <v>0.061393513000419</v>
+      </c>
+      <c r="Y214">
+        <v>0.076580877342703</v>
+      </c>
+      <c r="Z214">
+        <v>0.077823958284102</v>
+      </c>
+      <c r="AA214">
+        <v>0.0757675957977</v>
+      </c>
+      <c r="AB214">
+        <v>0.099704015931282</v>
+      </c>
+      <c r="AC214">
+        <v>0.079376984850653</v>
+      </c>
+      <c r="AD214">
+        <v>0.12562761528984</v>
+      </c>
+      <c r="AE214">
+        <v>0.11238346019661</v>
+      </c>
+      <c r="AF214">
+        <v>0.09116962497084</v>
+      </c>
+      <c r="AG214">
+        <v>0.11607428417781</v>
+      </c>
+      <c r="AH214">
+        <v>0.11883847008221</v>
+      </c>
+      <c r="AI214">
+        <v>0.082828474501538</v>
+      </c>
+      <c r="AJ214">
+        <v>0.069434308235526</v>
+      </c>
+      <c r="AK214">
+        <v>0.088597998550419</v>
+      </c>
+      <c r="AL214">
+        <v>0.078641135021985</v>
+      </c>
+      <c r="AM214">
+        <v>0.068249641017639</v>
+      </c>
+      <c r="AN214">
+        <v>0.09183895434273701</v>
+      </c>
+      <c r="AO214">
+        <v>0.11815440814549</v>
+      </c>
+      <c r="AP214">
+        <v>0.083816888697006</v>
+      </c>
+      <c r="AQ214">
+        <v>0.077039187782838</v>
+      </c>
+      <c r="AR214">
+        <v>0.081645993686478</v>
+      </c>
+      <c r="AS214">
+        <v>0.07122449322923601</v>
+      </c>
+      <c r="AT214">
+        <v>0.10115617189001</v>
+      </c>
+      <c r="AU214">
+        <v>0.1149314102667</v>
+      </c>
+      <c r="AV214">
+        <v>0.10145397692363</v>
+      </c>
+      <c r="AW214">
+        <v>0.09224189877919101</v>
+      </c>
+      <c r="AX214">
+        <v>0.11368904483561</v>
+      </c>
+      <c r="AY214">
+        <v>0.074354107283576</v>
+      </c>
+      <c r="AZ214">
+        <v>0.081160091804291</v>
+      </c>
+      <c r="BA214">
+        <v>0.074134139719071</v>
+      </c>
+      <c r="BB214">
+        <v>0.075417435261334</v>
+      </c>
+      <c r="BC214">
+        <v>0.080012894509355</v>
+      </c>
+      <c r="BD214">
+        <v>0.079154674129952</v>
+      </c>
+      <c r="BE214">
+        <v>0.11751041457798</v>
+      </c>
     </row>
     <row r="215" spans="1:57">
       <c r="A215" t="s">
         <v>269</v>
+      </c>
+      <c r="B215">
+        <v>0.071656644912978</v>
+      </c>
+      <c r="C215">
+        <v>0.11514264674101</v>
+      </c>
+      <c r="D215">
+        <v>0.11728369557904</v>
+      </c>
+      <c r="F215">
+        <v>0.06671294203488599</v>
+      </c>
+      <c r="G215">
+        <v>0.07641698298273999</v>
+      </c>
+      <c r="H215">
+        <v>0.09864195635749801</v>
+      </c>
+      <c r="I215">
+        <v>0.08545064425186299</v>
+      </c>
+      <c r="J215">
+        <v>0.062674318589397</v>
+      </c>
+      <c r="K215">
+        <v>0.084266569331998</v>
+      </c>
+      <c r="L215">
+        <v>0.09190908516375799</v>
+      </c>
+      <c r="M215">
+        <v>0.10746362916289</v>
+      </c>
+      <c r="N215">
+        <v>0.085426450462603</v>
+      </c>
+      <c r="O215">
+        <v>0.089428654717105</v>
+      </c>
+      <c r="P215">
+        <v>0.11413662173604</v>
+      </c>
+      <c r="Q215">
+        <v>0.11423260062487</v>
+      </c>
+      <c r="R215">
+        <v>0.087283429716633</v>
+      </c>
+      <c r="S215">
+        <v>0.10113022871188</v>
+      </c>
+      <c r="T215">
+        <v>0.10622508924233</v>
+      </c>
+      <c r="U215">
+        <v>0.088967899908086</v>
+      </c>
+      <c r="V215">
+        <v>0.10191469289892</v>
+      </c>
+      <c r="W215">
+        <v>0.073338231396814</v>
+      </c>
+      <c r="X215">
+        <v>0.066086905038686</v>
+      </c>
+      <c r="Y215">
+        <v>0.082394289605163</v>
+      </c>
+      <c r="Z215">
+        <v>0.08262609941381099</v>
+      </c>
+      <c r="AA215">
+        <v>0.08218796265157401</v>
+      </c>
+      <c r="AB215">
+        <v>0.10079911283249</v>
+      </c>
+      <c r="AC215">
+        <v>0.10497854001961</v>
+      </c>
+      <c r="AD215">
+        <v>0.12817192740367</v>
+      </c>
+      <c r="AE215">
+        <v>0.11306955144533</v>
+      </c>
+      <c r="AF215">
+        <v>0.091658002710411</v>
+      </c>
+      <c r="AG215">
+        <v>0.11434055816064</v>
+      </c>
+      <c r="AH215">
+        <v>0.12486600829312</v>
+      </c>
+      <c r="AI215">
+        <v>0.082224321925604</v>
+      </c>
+      <c r="AJ215">
+        <v>0.072422219350134</v>
+      </c>
+      <c r="AK215">
+        <v>0.08627675172810401</v>
+      </c>
+      <c r="AL215">
+        <v>0.078928603887918</v>
+      </c>
+      <c r="AM215">
+        <v>0.067464924133763</v>
+      </c>
+      <c r="AN215">
+        <v>0.090831133200206</v>
+      </c>
+      <c r="AO215">
+        <v>0.11674737341344</v>
+      </c>
+      <c r="AP215">
+        <v>0.088895925546859</v>
+      </c>
+      <c r="AQ215">
+        <v>0.081249257507226</v>
+      </c>
+      <c r="AR215">
+        <v>0.084111620491903</v>
+      </c>
+      <c r="AS215">
+        <v>0.080085597547358</v>
+      </c>
+      <c r="AT215">
+        <v>0.1052701225728</v>
+      </c>
+      <c r="AU215">
+        <v>0.12526187971202</v>
+      </c>
+      <c r="AV215">
+        <v>0.10895378554662</v>
+      </c>
+      <c r="AW215">
+        <v>0.09621873645010399</v>
+      </c>
+      <c r="AX215">
+        <v>0.11633192437292</v>
+      </c>
+      <c r="AY215">
+        <v>0.077936794517037</v>
+      </c>
+      <c r="AZ215">
+        <v>0.077848591165569</v>
+      </c>
+      <c r="BA215">
+        <v>0.08329506617303099</v>
+      </c>
+      <c r="BB215">
+        <v>0.077177500722329</v>
+      </c>
+      <c r="BC215">
+        <v>0.087529890926791</v>
+      </c>
+      <c r="BD215">
+        <v>0.08365249373913</v>
+      </c>
+      <c r="BE215">
+        <v>0.12036639729355</v>
+      </c>
+    </row>
+    <row r="216" spans="1:57">
+      <c r="A216" t="s">
+        <v>270</v>
+      </c>
+      <c r="B216">
+        <v>0.094235027961606</v>
+      </c>
+      <c r="C216">
+        <v>0.11839466954152</v>
+      </c>
+      <c r="D216">
+        <v>0.12530298582001</v>
+      </c>
+      <c r="F216">
+        <v>0.07890550873268901</v>
+      </c>
+      <c r="G216">
+        <v>0.072313362018451</v>
+      </c>
+      <c r="H216">
+        <v>0.086184001311187</v>
+      </c>
+      <c r="I216">
+        <v>0.066871109037553</v>
+      </c>
+      <c r="J216">
+        <v>0.049184931139857</v>
+      </c>
+      <c r="K216">
+        <v>0.070482032253063</v>
+      </c>
+      <c r="L216">
+        <v>0.083297133424792</v>
+      </c>
+      <c r="M216">
+        <v>0.10185374397948</v>
+      </c>
+      <c r="N216">
+        <v>0.071895327627782</v>
+      </c>
+      <c r="O216">
+        <v>0.084656653981367</v>
+      </c>
+      <c r="P216">
+        <v>0.12444245829502</v>
+      </c>
+      <c r="Q216">
+        <v>0.10487086502707</v>
+      </c>
+      <c r="R216">
+        <v>0.08603248499244499</v>
+      </c>
+      <c r="S216">
+        <v>0.10320089527669</v>
+      </c>
+      <c r="T216">
+        <v>0.11753072001344</v>
+      </c>
+      <c r="U216">
+        <v>0.095136744392518</v>
+      </c>
+      <c r="V216">
+        <v>0.11093350521934</v>
+      </c>
+      <c r="W216">
+        <v>0.079714210708069</v>
+      </c>
+      <c r="X216">
+        <v>0.07381781225228499</v>
+      </c>
+      <c r="Y216">
+        <v>0.091963997419264</v>
+      </c>
+      <c r="Z216">
+        <v>0.088541014062524</v>
+      </c>
+      <c r="AA216">
+        <v>0.08523826654595</v>
+      </c>
+      <c r="AB216">
+        <v>0.10608397606774</v>
+      </c>
+      <c r="AC216">
+        <v>0.085366670194547</v>
+      </c>
+      <c r="AD216">
+        <v>0.13140234472487</v>
+      </c>
+      <c r="AE216">
+        <v>0.11557281718307</v>
+      </c>
+      <c r="AF216">
+        <v>0.09107946995246601</v>
+      </c>
+      <c r="AG216">
+        <v>0.11679562486638</v>
+      </c>
+      <c r="AH216">
+        <v>0.12800388267189</v>
+      </c>
+      <c r="AI216">
+        <v>0.08274485353746899</v>
+      </c>
+      <c r="AJ216">
+        <v>0.07039159785902201</v>
+      </c>
+      <c r="AK216">
+        <v>0.085304565439682</v>
+      </c>
+      <c r="AL216">
+        <v>0.07775267139183099</v>
+      </c>
+      <c r="AM216">
+        <v>0.067940466707752</v>
+      </c>
+      <c r="AN216">
+        <v>0.08668843907608</v>
+      </c>
+      <c r="AO216">
+        <v>0.11864128076216</v>
+      </c>
+      <c r="AP216">
+        <v>0.08133933593116099</v>
+      </c>
+      <c r="AQ216">
+        <v>0.071090875494212</v>
+      </c>
+      <c r="AR216">
+        <v>0.086581546959404</v>
+      </c>
+      <c r="AS216">
+        <v>0.06505326336792699</v>
+      </c>
+      <c r="AT216">
+        <v>0.09878999836252</v>
+      </c>
+      <c r="AU216">
+        <v>0.11417546076272</v>
+      </c>
+      <c r="AV216">
+        <v>0.10081423248645</v>
+      </c>
+      <c r="AW216">
+        <v>0.090169475986866</v>
+      </c>
+      <c r="AX216">
+        <v>0.1130274928121</v>
+      </c>
+      <c r="AY216">
+        <v>0.07708422534616</v>
+      </c>
+      <c r="AZ216">
+        <v>0.076860277021783</v>
+      </c>
+      <c r="BA216">
+        <v>0.07209607933696</v>
+      </c>
+      <c r="BB216">
+        <v>0.076801634002246</v>
+      </c>
+      <c r="BC216">
+        <v>0.092557461443025</v>
+      </c>
+      <c r="BD216">
+        <v>0.08507831424894501</v>
+      </c>
+      <c r="BE216">
+        <v>0.1259786063693</v>
+      </c>
+    </row>
+    <row r="217" spans="1:57">
+      <c r="A217" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="218" spans="1:57">
+      <c r="A218" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="219" spans="1:57">
+      <c r="A219" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="220" spans="1:57">
+      <c r="A220" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="221" spans="1:57">
+      <c r="A221" t="s">
+        <v>275</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data up otto 14th
</commit_message>
<xml_diff>
--- a/away3-6hours.xlsx
+++ b/away3-6hours.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="283">
   <si>
     <t>Alaska</t>
   </si>
@@ -843,6 +843,27 @@
   <si>
     <t>07 09 2020</t>
   </si>
+  <si>
+    <t>08 09 2020</t>
+  </si>
+  <si>
+    <t>09 09 2020</t>
+  </si>
+  <si>
+    <t>10 09 2020</t>
+  </si>
+  <si>
+    <t>11 09 2020</t>
+  </si>
+  <si>
+    <t>12 09 2020</t>
+  </si>
+  <si>
+    <t>13 09 2020</t>
+  </si>
+  <si>
+    <t>14 09 2020</t>
+  </si>
 </sst>
 </file>
 
@@ -1173,7 +1194,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BE221"/>
+  <dimension ref="A1:BE228"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -22295,6 +22316,9 @@
       <c r="D123">
         <v>0.095382947203816</v>
       </c>
+      <c r="E123">
+        <v>0.08824855699855701</v>
+      </c>
       <c r="F123">
         <v>0.07843939613291299</v>
       </c>
@@ -22465,6 +22489,9 @@
       <c r="D124">
         <v>0.10155884318818</v>
       </c>
+      <c r="E124">
+        <v>0.066666666666667</v>
+      </c>
       <c r="F124">
         <v>0.07363115137845599</v>
       </c>
@@ -22635,6 +22662,9 @@
       <c r="D125">
         <v>0.096301981916615</v>
       </c>
+      <c r="E125">
+        <v>0.07142857142857099</v>
+      </c>
       <c r="F125">
         <v>0.068121780816658</v>
       </c>
@@ -22805,6 +22835,9 @@
       <c r="D126">
         <v>0.09917703819384401</v>
       </c>
+      <c r="E126">
+        <v>0.055555555555556</v>
+      </c>
       <c r="F126">
         <v>0.082192626983876</v>
       </c>
@@ -22975,6 +23008,9 @@
       <c r="D127">
         <v>0.08507824230503901</v>
       </c>
+      <c r="E127">
+        <v>0.04</v>
+      </c>
       <c r="F127">
         <v>0.072393166909466</v>
       </c>
@@ -23145,6 +23181,9 @@
       <c r="D128">
         <v>0.057311532513036</v>
       </c>
+      <c r="E128">
+        <v>0.04</v>
+      </c>
       <c r="F128">
         <v>0.056910389288764</v>
       </c>
@@ -23315,6 +23354,9 @@
       <c r="D129">
         <v>0.048926448638687</v>
       </c>
+      <c r="E129">
+        <v>0.03448275862069</v>
+      </c>
       <c r="F129">
         <v>0.055730447706029</v>
       </c>
@@ -38266,25 +38308,1215 @@
       <c r="A217" t="s">
         <v>271</v>
       </c>
+      <c r="B217">
+        <v>0.080546918556421</v>
+      </c>
+      <c r="C217">
+        <v>0.12631787452441</v>
+      </c>
+      <c r="D217">
+        <v>0.13105850854141</v>
+      </c>
+      <c r="F217">
+        <v>0.076521557736573</v>
+      </c>
+      <c r="G217">
+        <v>0.089226096716679</v>
+      </c>
+      <c r="H217">
+        <v>0.09738985428784</v>
+      </c>
+      <c r="I217">
+        <v>0.081603555378684</v>
+      </c>
+      <c r="J217">
+        <v>0.056076189486637</v>
+      </c>
+      <c r="K217">
+        <v>0.079995278128505</v>
+      </c>
+      <c r="L217">
+        <v>0.09134230358753199</v>
+      </c>
+      <c r="M217">
+        <v>0.10586894216811</v>
+      </c>
+      <c r="N217">
+        <v>0.07688121592185999</v>
+      </c>
+      <c r="O217">
+        <v>0.088703796904363</v>
+      </c>
+      <c r="P217">
+        <v>0.12948991747404</v>
+      </c>
+      <c r="Q217">
+        <v>0.11042712642318</v>
+      </c>
+      <c r="R217">
+        <v>0.091853601448539</v>
+      </c>
+      <c r="S217">
+        <v>0.10914650772821</v>
+      </c>
+      <c r="T217">
+        <v>0.12274351314045</v>
+      </c>
+      <c r="U217">
+        <v>0.098356526489197</v>
+      </c>
+      <c r="V217">
+        <v>0.11214259557451</v>
+      </c>
+      <c r="W217">
+        <v>0.075702093331253</v>
+      </c>
+      <c r="X217">
+        <v>0.07071396862356701</v>
+      </c>
+      <c r="Y217">
+        <v>0.091626252570451</v>
+      </c>
+      <c r="Z217">
+        <v>0.085504062274658</v>
+      </c>
+      <c r="AA217">
+        <v>0.084024379294787</v>
+      </c>
+      <c r="AB217">
+        <v>0.10876727286396</v>
+      </c>
+      <c r="AC217">
+        <v>0.0999285408472</v>
+      </c>
+      <c r="AD217">
+        <v>0.1312038875393</v>
+      </c>
+      <c r="AE217">
+        <v>0.11957378878738</v>
+      </c>
+      <c r="AF217">
+        <v>0.09442992273930501</v>
+      </c>
+      <c r="AG217">
+        <v>0.11852841720654</v>
+      </c>
+      <c r="AH217">
+        <v>0.12869191822963</v>
+      </c>
+      <c r="AI217">
+        <v>0.08856502973585299</v>
+      </c>
+      <c r="AJ217">
+        <v>0.079542196518161</v>
+      </c>
+      <c r="AK217">
+        <v>0.095685570296694</v>
+      </c>
+      <c r="AL217">
+        <v>0.085220125115472</v>
+      </c>
+      <c r="AM217">
+        <v>0.075919093737165</v>
+      </c>
+      <c r="AN217">
+        <v>0.089640072949897</v>
+      </c>
+      <c r="AO217">
+        <v>0.12414192055525</v>
+      </c>
+      <c r="AP217">
+        <v>0.088743614339442</v>
+      </c>
+      <c r="AQ217">
+        <v>0.078569128999625</v>
+      </c>
+      <c r="AR217">
+        <v>0.087323330509</v>
+      </c>
+      <c r="AS217">
+        <v>0.07758418745562801</v>
+      </c>
+      <c r="AT217">
+        <v>0.10589672454596</v>
+      </c>
+      <c r="AU217">
+        <v>0.12511013424269</v>
+      </c>
+      <c r="AV217">
+        <v>0.11006028748554</v>
+      </c>
+      <c r="AW217">
+        <v>0.098790349609614</v>
+      </c>
+      <c r="AX217">
+        <v>0.11947257069944</v>
+      </c>
+      <c r="AY217">
+        <v>0.081669909000334</v>
+      </c>
+      <c r="AZ217">
+        <v>0.09515943760546</v>
+      </c>
+      <c r="BA217">
+        <v>0.078705413163715</v>
+      </c>
+      <c r="BB217">
+        <v>0.084981132301525</v>
+      </c>
+      <c r="BC217">
+        <v>0.094173860549168</v>
+      </c>
+      <c r="BD217">
+        <v>0.081535728956993</v>
+      </c>
+      <c r="BE217">
+        <v>0.12899406505731</v>
+      </c>
     </row>
     <row r="218" spans="1:57">
       <c r="A218" t="s">
         <v>272</v>
       </c>
+      <c r="B218">
+        <v>0.070150944910221</v>
+      </c>
+      <c r="C218">
+        <v>0.114667207104</v>
+      </c>
+      <c r="D218">
+        <v>0.11775052338716</v>
+      </c>
+      <c r="F218">
+        <v>0.064101342480139</v>
+      </c>
+      <c r="G218">
+        <v>0.083003375472501</v>
+      </c>
+      <c r="H218">
+        <v>0.097414106115156</v>
+      </c>
+      <c r="I218">
+        <v>0.090991360017544</v>
+      </c>
+      <c r="J218">
+        <v>0.070581113056173</v>
+      </c>
+      <c r="K218">
+        <v>0.082476261354845</v>
+      </c>
+      <c r="L218">
+        <v>0.09104810167286401</v>
+      </c>
+      <c r="M218">
+        <v>0.09249528804872199</v>
+      </c>
+      <c r="N218">
+        <v>0.07747943636672</v>
+      </c>
+      <c r="O218">
+        <v>0.07249371703369401</v>
+      </c>
+      <c r="P218">
+        <v>0.10441339906536</v>
+      </c>
+      <c r="Q218">
+        <v>0.090501490056802</v>
+      </c>
+      <c r="R218">
+        <v>0.075207183007364</v>
+      </c>
+      <c r="S218">
+        <v>0.089159220099237</v>
+      </c>
+      <c r="T218">
+        <v>0.097603410376997</v>
+      </c>
+      <c r="U218">
+        <v>0.078348668033911</v>
+      </c>
+      <c r="V218">
+        <v>0.093317969901374</v>
+      </c>
+      <c r="W218">
+        <v>0.07044666226075701</v>
+      </c>
+      <c r="X218">
+        <v>0.061323860877873</v>
+      </c>
+      <c r="Y218">
+        <v>0.076401107723972</v>
+      </c>
+      <c r="Z218">
+        <v>0.073417547862741</v>
+      </c>
+      <c r="AA218">
+        <v>0.07672037989395999</v>
+      </c>
+      <c r="AB218">
+        <v>0.10183340784132</v>
+      </c>
+      <c r="AC218">
+        <v>0.07555615362937899</v>
+      </c>
+      <c r="AD218">
+        <v>0.12284302445139</v>
+      </c>
+      <c r="AE218">
+        <v>0.11124550055119</v>
+      </c>
+      <c r="AF218">
+        <v>0.090787781730731</v>
+      </c>
+      <c r="AG218">
+        <v>0.11071295671826</v>
+      </c>
+      <c r="AH218">
+        <v>0.12161360675646</v>
+      </c>
+      <c r="AI218">
+        <v>0.07977462148608599</v>
+      </c>
+      <c r="AJ218">
+        <v>0.074145350896043</v>
+      </c>
+      <c r="AK218">
+        <v>0.085541357212463</v>
+      </c>
+      <c r="AL218">
+        <v>0.078684778590581</v>
+      </c>
+      <c r="AM218">
+        <v>0.072017824427019</v>
+      </c>
+      <c r="AN218">
+        <v>0.08894058237437601</v>
+      </c>
+      <c r="AO218">
+        <v>0.11150838638037</v>
+      </c>
+      <c r="AP218">
+        <v>0.079719309566516</v>
+      </c>
+      <c r="AQ218">
+        <v>0.07189558462456</v>
+      </c>
+      <c r="AR218">
+        <v>0.08542326733861701</v>
+      </c>
+      <c r="AS218">
+        <v>0.07310804088586401</v>
+      </c>
+      <c r="AT218">
+        <v>0.09337434721922</v>
+      </c>
+      <c r="AU218">
+        <v>0.099176695241595</v>
+      </c>
+      <c r="AV218">
+        <v>0.09646057160874801</v>
+      </c>
+      <c r="AW218">
+        <v>0.08891091821384101</v>
+      </c>
+      <c r="AX218">
+        <v>0.10540564406028</v>
+      </c>
+      <c r="AY218">
+        <v>0.074141596118207</v>
+      </c>
+      <c r="AZ218">
+        <v>0.08846626263001001</v>
+      </c>
+      <c r="BA218">
+        <v>0.07154857701471699</v>
+      </c>
+      <c r="BB218">
+        <v>0.073936826884962</v>
+      </c>
+      <c r="BC218">
+        <v>0.087018407098924</v>
+      </c>
+      <c r="BD218">
+        <v>0.07602833964800899</v>
+      </c>
+      <c r="BE218">
+        <v>0.12356749184644</v>
+      </c>
     </row>
     <row r="219" spans="1:57">
       <c r="A219" t="s">
         <v>273</v>
       </c>
+      <c r="B219">
+        <v>0.052841056412051</v>
+      </c>
+      <c r="C219">
+        <v>0.07147403858547199</v>
+      </c>
+      <c r="D219">
+        <v>0.056216428774658</v>
+      </c>
+      <c r="F219">
+        <v>0.053916445848977</v>
+      </c>
+      <c r="G219">
+        <v>0.074128450081418</v>
+      </c>
+      <c r="H219">
+        <v>0.07472019516923301</v>
+      </c>
+      <c r="I219">
+        <v>0.05347668683156</v>
+      </c>
+      <c r="J219">
+        <v>0.048915481442165</v>
+      </c>
+      <c r="K219">
+        <v>0.05805740966965</v>
+      </c>
+      <c r="L219">
+        <v>0.05691341177006</v>
+      </c>
+      <c r="M219">
+        <v>0.06288174960979</v>
+      </c>
+      <c r="N219">
+        <v>0.070297156773532</v>
+      </c>
+      <c r="O219">
+        <v>0.057893645083494</v>
+      </c>
+      <c r="P219">
+        <v>0.07067173234917901</v>
+      </c>
+      <c r="Q219">
+        <v>0.07893967455156101</v>
+      </c>
+      <c r="R219">
+        <v>0.06553782751977801</v>
+      </c>
+      <c r="S219">
+        <v>0.06286445479550801</v>
+      </c>
+      <c r="T219">
+        <v>0.062561830392641</v>
+      </c>
+      <c r="U219">
+        <v>0.058214583310609</v>
+      </c>
+      <c r="V219">
+        <v>0.066628534965915</v>
+      </c>
+      <c r="W219">
+        <v>0.055745913974856</v>
+      </c>
+      <c r="X219">
+        <v>0.051474639864099</v>
+      </c>
+      <c r="Y219">
+        <v>0.059390073493542</v>
+      </c>
+      <c r="Z219">
+        <v>0.050125620693576</v>
+      </c>
+      <c r="AA219">
+        <v>0.051277188839859</v>
+      </c>
+      <c r="AB219">
+        <v>0.057908550017535</v>
+      </c>
+      <c r="AC219">
+        <v>0.032258064516129</v>
+      </c>
+      <c r="AD219">
+        <v>0.063472551103792</v>
+      </c>
+      <c r="AE219">
+        <v>0.067149696997776</v>
+      </c>
+      <c r="AF219">
+        <v>0.061028925476496</v>
+      </c>
+      <c r="AG219">
+        <v>0.060648986947216</v>
+      </c>
+      <c r="AH219">
+        <v>0.06283114225473201</v>
+      </c>
+      <c r="AI219">
+        <v>0.053480424285866</v>
+      </c>
+      <c r="AJ219">
+        <v>0.05352851783154</v>
+      </c>
+      <c r="AK219">
+        <v>0.066979708353103</v>
+      </c>
+      <c r="AL219">
+        <v>0.060353808272722</v>
+      </c>
+      <c r="AM219">
+        <v>0.054101772525993</v>
+      </c>
+      <c r="AN219">
+        <v>0.059489793856016</v>
+      </c>
+      <c r="AO219">
+        <v>0.064628763283905</v>
+      </c>
+      <c r="AP219">
+        <v>0.06708504871745199</v>
+      </c>
+      <c r="AQ219">
+        <v>0.059847408507789</v>
+      </c>
+      <c r="AR219">
+        <v>0.077732168655165</v>
+      </c>
+      <c r="AS219">
+        <v>0.062505191142811</v>
+      </c>
+      <c r="AT219">
+        <v>0.063808460184569</v>
+      </c>
+      <c r="AU219">
+        <v>0.07273171789558799</v>
+      </c>
+      <c r="AV219">
+        <v>0.063659565049428</v>
+      </c>
+      <c r="AW219">
+        <v>0.05992216826089</v>
+      </c>
+      <c r="AX219">
+        <v>0.081782430727377</v>
+      </c>
+      <c r="AY219">
+        <v>0.05914962475543</v>
+      </c>
+      <c r="AZ219">
+        <v>0.076627164391276</v>
+      </c>
+      <c r="BA219">
+        <v>0.06284327754341799</v>
+      </c>
+      <c r="BB219">
+        <v>0.067760466526786</v>
+      </c>
+      <c r="BC219">
+        <v>0.061058441875329</v>
+      </c>
+      <c r="BD219">
+        <v>0.060960136184346</v>
+      </c>
+      <c r="BE219">
+        <v>0.080772282704192</v>
+      </c>
     </row>
     <row r="220" spans="1:57">
       <c r="A220" t="s">
         <v>274</v>
       </c>
+      <c r="B220">
+        <v>0.059569884187024</v>
+      </c>
+      <c r="C220">
+        <v>0.068311222387393</v>
+      </c>
+      <c r="D220">
+        <v>0.059136487734949</v>
+      </c>
+      <c r="F220">
+        <v>0.059407090448432</v>
+      </c>
+      <c r="G220">
+        <v>0.057276870712931</v>
+      </c>
+      <c r="H220">
+        <v>0.06841744630303701</v>
+      </c>
+      <c r="I220">
+        <v>0.051519814921016</v>
+      </c>
+      <c r="J220">
+        <v>0.050138667341041</v>
+      </c>
+      <c r="K220">
+        <v>0.056181995637697</v>
+      </c>
+      <c r="L220">
+        <v>0.052969175752447</v>
+      </c>
+      <c r="M220">
+        <v>0.054572961826168</v>
+      </c>
+      <c r="N220">
+        <v>0.058738768889774</v>
+      </c>
+      <c r="O220">
+        <v>0.047514603096116</v>
+      </c>
+      <c r="P220">
+        <v>0.055436266150989</v>
+      </c>
+      <c r="Q220">
+        <v>0.068777806716766</v>
+      </c>
+      <c r="R220">
+        <v>0.050150897416634</v>
+      </c>
+      <c r="S220">
+        <v>0.053200030273692</v>
+      </c>
+      <c r="T220">
+        <v>0.056321879370839</v>
+      </c>
+      <c r="U220">
+        <v>0.05298595833064</v>
+      </c>
+      <c r="V220">
+        <v>0.060966470081529</v>
+      </c>
+      <c r="W220">
+        <v>0.049891974210304</v>
+      </c>
+      <c r="X220">
+        <v>0.046265803147136</v>
+      </c>
+      <c r="Y220">
+        <v>0.053886610414135</v>
+      </c>
+      <c r="Z220">
+        <v>0.043850323870919</v>
+      </c>
+      <c r="AA220">
+        <v>0.04563838134002</v>
+      </c>
+      <c r="AB220">
+        <v>0.055216492555534</v>
+      </c>
+      <c r="AC220">
+        <v>0.045454545454545</v>
+      </c>
+      <c r="AD220">
+        <v>0.058145112434461</v>
+      </c>
+      <c r="AE220">
+        <v>0.064389595393817</v>
+      </c>
+      <c r="AF220">
+        <v>0.058377276847369</v>
+      </c>
+      <c r="AG220">
+        <v>0.059076102609648</v>
+      </c>
+      <c r="AH220">
+        <v>0.057268439469003</v>
+      </c>
+      <c r="AI220">
+        <v>0.053421755355878</v>
+      </c>
+      <c r="AJ220">
+        <v>0.053594578913</v>
+      </c>
+      <c r="AK220">
+        <v>0.067605658581182</v>
+      </c>
+      <c r="AL220">
+        <v>0.057977302934424</v>
+      </c>
+      <c r="AM220">
+        <v>0.056952929400953</v>
+      </c>
+      <c r="AN220">
+        <v>0.057810862968188</v>
+      </c>
+      <c r="AO220">
+        <v>0.061767336809467</v>
+      </c>
+      <c r="AP220">
+        <v>0.06336386497707901</v>
+      </c>
+      <c r="AQ220">
+        <v>0.054144536206126</v>
+      </c>
+      <c r="AR220">
+        <v>0.068999559208953</v>
+      </c>
+      <c r="AS220">
+        <v>0.059109291863263</v>
+      </c>
+      <c r="AT220">
+        <v>0.054595336810273</v>
+      </c>
+      <c r="AU220">
+        <v>0.061610206101517</v>
+      </c>
+      <c r="AV220">
+        <v>0.055593480102205</v>
+      </c>
+      <c r="AW220">
+        <v>0.04785270317525</v>
+      </c>
+      <c r="AX220">
+        <v>0.062116093291731</v>
+      </c>
+      <c r="AY220">
+        <v>0.048434831538889</v>
+      </c>
+      <c r="AZ220">
+        <v>0.06486707428477601</v>
+      </c>
+      <c r="BA220">
+        <v>0.051047064590233</v>
+      </c>
+      <c r="BB220">
+        <v>0.058197077184282</v>
+      </c>
+      <c r="BC220">
+        <v>0.053047738501672</v>
+      </c>
+      <c r="BD220">
+        <v>0.051953034985002</v>
+      </c>
+      <c r="BE220">
+        <v>0.071116811884345</v>
+      </c>
     </row>
     <row r="221" spans="1:57">
       <c r="A221" t="s">
         <v>275</v>
+      </c>
+      <c r="B221">
+        <v>0.057907954115047</v>
+      </c>
+      <c r="C221">
+        <v>0.060618396298331</v>
+      </c>
+      <c r="D221">
+        <v>0.045376190485629</v>
+      </c>
+      <c r="F221">
+        <v>0.047513524938037</v>
+      </c>
+      <c r="G221">
+        <v>0.054752320429088</v>
+      </c>
+      <c r="H221">
+        <v>0.061057471181488</v>
+      </c>
+      <c r="I221">
+        <v>0.053284964456149</v>
+      </c>
+      <c r="J221">
+        <v>0.059510230177909</v>
+      </c>
+      <c r="K221">
+        <v>0.053840598382896</v>
+      </c>
+      <c r="L221">
+        <v>0.056450460699473</v>
+      </c>
+      <c r="M221">
+        <v>0.055690285454405</v>
+      </c>
+      <c r="N221">
+        <v>0.057495289151705</v>
+      </c>
+      <c r="O221">
+        <v>0.053372791830511</v>
+      </c>
+      <c r="P221">
+        <v>0.045667442761794</v>
+      </c>
+      <c r="Q221">
+        <v>0.066529234902555</v>
+      </c>
+      <c r="R221">
+        <v>0.049365889782814</v>
+      </c>
+      <c r="S221">
+        <v>0.044962279665043</v>
+      </c>
+      <c r="T221">
+        <v>0.044539250880897</v>
+      </c>
+      <c r="U221">
+        <v>0.046186720728996</v>
+      </c>
+      <c r="V221">
+        <v>0.057571037492883</v>
+      </c>
+      <c r="W221">
+        <v>0.050443508791014</v>
+      </c>
+      <c r="X221">
+        <v>0.044947286287756</v>
+      </c>
+      <c r="Y221">
+        <v>0.049122777014731</v>
+      </c>
+      <c r="Z221">
+        <v>0.042593038716024</v>
+      </c>
+      <c r="AA221">
+        <v>0.040917268314806</v>
+      </c>
+      <c r="AB221">
+        <v>0.04845937615514</v>
+      </c>
+      <c r="AC221">
+        <v>0.10714285714286</v>
+      </c>
+      <c r="AD221">
+        <v>0.055758417480546</v>
+      </c>
+      <c r="AE221">
+        <v>0.0582285946337</v>
+      </c>
+      <c r="AF221">
+        <v>0.054211265190906</v>
+      </c>
+      <c r="AG221">
+        <v>0.051044649816527</v>
+      </c>
+      <c r="AH221">
+        <v>0.049012342887169</v>
+      </c>
+      <c r="AI221">
+        <v>0.049733782831814</v>
+      </c>
+      <c r="AJ221">
+        <v>0.053988645678723</v>
+      </c>
+      <c r="AK221">
+        <v>0.06497150591029401</v>
+      </c>
+      <c r="AL221">
+        <v>0.054711142379704</v>
+      </c>
+      <c r="AM221">
+        <v>0.060103663684809</v>
+      </c>
+      <c r="AN221">
+        <v>0.049106868872383</v>
+      </c>
+      <c r="AO221">
+        <v>0.053228913323072</v>
+      </c>
+      <c r="AP221">
+        <v>0.053806245643449</v>
+      </c>
+      <c r="AQ221">
+        <v>0.05011386089773</v>
+      </c>
+      <c r="AR221">
+        <v>0.068676819930949</v>
+      </c>
+      <c r="AS221">
+        <v>0.054540380611512</v>
+      </c>
+      <c r="AT221">
+        <v>0.052922017251684</v>
+      </c>
+      <c r="AU221">
+        <v>0.054325841304622</v>
+      </c>
+      <c r="AV221">
+        <v>0.055374815187519</v>
+      </c>
+      <c r="AW221">
+        <v>0.050979264795364</v>
+      </c>
+      <c r="AX221">
+        <v>0.06505087158417799</v>
+      </c>
+      <c r="AY221">
+        <v>0.04757508724543</v>
+      </c>
+      <c r="AZ221">
+        <v>0.073296832340425</v>
+      </c>
+      <c r="BA221">
+        <v>0.051889857743866</v>
+      </c>
+      <c r="BB221">
+        <v>0.05353949013986</v>
+      </c>
+      <c r="BC221">
+        <v>0.046178346931998</v>
+      </c>
+      <c r="BD221">
+        <v>0.048719210398439</v>
+      </c>
+      <c r="BE221">
+        <v>0.060174257730679</v>
+      </c>
+    </row>
+    <row r="222" spans="1:57">
+      <c r="A222" t="s">
+        <v>276</v>
+      </c>
+      <c r="B222">
+        <v>0.077823177907532</v>
+      </c>
+      <c r="C222">
+        <v>0.11810031339239</v>
+      </c>
+      <c r="D222">
+        <v>0.11931952948388</v>
+      </c>
+      <c r="F222">
+        <v>0.062030804456152</v>
+      </c>
+      <c r="G222">
+        <v>0.07911861274611</v>
+      </c>
+      <c r="H222">
+        <v>0.08898557083514599</v>
+      </c>
+      <c r="I222">
+        <v>0.087012181825543</v>
+      </c>
+      <c r="J222">
+        <v>0.059207719470813</v>
+      </c>
+      <c r="K222">
+        <v>0.075239479354202</v>
+      </c>
+      <c r="L222">
+        <v>0.08902960281454</v>
+      </c>
+      <c r="M222">
+        <v>0.10289643758368</v>
+      </c>
+      <c r="N222">
+        <v>0.084851734637647</v>
+      </c>
+      <c r="O222">
+        <v>0.08397300951820399</v>
+      </c>
+      <c r="P222">
+        <v>0.11634629897268</v>
+      </c>
+      <c r="Q222">
+        <v>0.11076830222563</v>
+      </c>
+      <c r="R222">
+        <v>0.084573593745526</v>
+      </c>
+      <c r="S222">
+        <v>0.10313755431652</v>
+      </c>
+      <c r="T222">
+        <v>0.111831965472</v>
+      </c>
+      <c r="U222">
+        <v>0.095799839153571</v>
+      </c>
+      <c r="V222">
+        <v>0.10994977533393</v>
+      </c>
+      <c r="W222">
+        <v>0.07673034070747101</v>
+      </c>
+      <c r="X222">
+        <v>0.068601264723869</v>
+      </c>
+      <c r="Y222">
+        <v>0.090879271097349</v>
+      </c>
+      <c r="Z222">
+        <v>0.084588408468424</v>
+      </c>
+      <c r="AA222">
+        <v>0.088812249966467</v>
+      </c>
+      <c r="AB222">
+        <v>0.10499224844496</v>
+      </c>
+      <c r="AC222">
+        <v>0.10714285714286</v>
+      </c>
+      <c r="AD222">
+        <v>0.13305620872125</v>
+      </c>
+      <c r="AE222">
+        <v>0.12003039057499</v>
+      </c>
+      <c r="AF222">
+        <v>0.093380006937822</v>
+      </c>
+      <c r="AG222">
+        <v>0.11478889712615</v>
+      </c>
+      <c r="AH222">
+        <v>0.11865709013159</v>
+      </c>
+      <c r="AI222">
+        <v>0.082476288316951</v>
+      </c>
+      <c r="AJ222">
+        <v>0.074769803516924</v>
+      </c>
+      <c r="AK222">
+        <v>0.086635594556827</v>
+      </c>
+      <c r="AL222">
+        <v>0.076225835166675</v>
+      </c>
+      <c r="AM222">
+        <v>0.07383577054221201</v>
+      </c>
+      <c r="AN222">
+        <v>0.09002011394387301</v>
+      </c>
+      <c r="AO222">
+        <v>0.11787340709556</v>
+      </c>
+      <c r="AP222">
+        <v>0.08004998620390499</v>
+      </c>
+      <c r="AQ222">
+        <v>0.07584106635459301</v>
+      </c>
+      <c r="AR222">
+        <v>0.076056024168798</v>
+      </c>
+      <c r="AS222">
+        <v>0.07184316118845301</v>
+      </c>
+      <c r="AT222">
+        <v>0.10200233995815</v>
+      </c>
+      <c r="AU222">
+        <v>0.11610164350544</v>
+      </c>
+      <c r="AV222">
+        <v>0.10673967037876</v>
+      </c>
+      <c r="AW222">
+        <v>0.10014804078882</v>
+      </c>
+      <c r="AX222">
+        <v>0.11389764677897</v>
+      </c>
+      <c r="AY222">
+        <v>0.08224866890390301</v>
+      </c>
+      <c r="AZ222">
+        <v>0.0647962607101</v>
+      </c>
+      <c r="BA222">
+        <v>0.092258416494363</v>
+      </c>
+      <c r="BB222">
+        <v>0.082880098314169</v>
+      </c>
+      <c r="BC222">
+        <v>0.09172329078557</v>
+      </c>
+      <c r="BD222">
+        <v>0.090070012408837</v>
+      </c>
+      <c r="BE222">
+        <v>0.11786223122549</v>
+      </c>
+    </row>
+    <row r="223" spans="1:57">
+      <c r="A223" t="s">
+        <v>277</v>
+      </c>
+      <c r="B223">
+        <v>0.08922043908769201</v>
+      </c>
+      <c r="C223">
+        <v>0.12975926770722</v>
+      </c>
+      <c r="D223">
+        <v>0.13734150318426</v>
+      </c>
+      <c r="F223">
+        <v>0.077894974659519</v>
+      </c>
+      <c r="G223">
+        <v>0.081436462607257</v>
+      </c>
+      <c r="H223">
+        <v>0.081807441857218</v>
+      </c>
+      <c r="I223">
+        <v>0.073914565197749</v>
+      </c>
+      <c r="J223">
+        <v>0.046686413769026</v>
+      </c>
+      <c r="K223">
+        <v>0.06797176988518799</v>
+      </c>
+      <c r="L223">
+        <v>0.081023739165662</v>
+      </c>
+      <c r="M223">
+        <v>0.098840709180177</v>
+      </c>
+      <c r="N223">
+        <v>0.059210857310304</v>
+      </c>
+      <c r="O223">
+        <v>0.07399482261278501</v>
+      </c>
+      <c r="P223">
+        <v>0.11122329138644</v>
+      </c>
+      <c r="Q223">
+        <v>0.10181416694488</v>
+      </c>
+      <c r="R223">
+        <v>0.07897068192635</v>
+      </c>
+      <c r="S223">
+        <v>0.10129265493631</v>
+      </c>
+      <c r="T223">
+        <v>0.10700492720126</v>
+      </c>
+      <c r="U223">
+        <v>0.09101005675926099</v>
+      </c>
+      <c r="V223">
+        <v>0.10353592395755</v>
+      </c>
+      <c r="W223">
+        <v>0.06731411097041599</v>
+      </c>
+      <c r="X223">
+        <v>0.06243288008042</v>
+      </c>
+      <c r="Y223">
+        <v>0.08183252258926001</v>
+      </c>
+      <c r="Z223">
+        <v>0.0796934551384</v>
+      </c>
+      <c r="AA223">
+        <v>0.081273921777012</v>
+      </c>
+      <c r="AB223">
+        <v>0.10225678657451</v>
+      </c>
+      <c r="AC223">
+        <v>0.032258064516129</v>
+      </c>
+      <c r="AD223">
+        <v>0.13006675901652</v>
+      </c>
+      <c r="AE223">
+        <v>0.11501400964894</v>
+      </c>
+      <c r="AF223">
+        <v>0.090841789380255</v>
+      </c>
+      <c r="AG223">
+        <v>0.11954276474863</v>
+      </c>
+      <c r="AH223">
+        <v>0.1168285879978</v>
+      </c>
+      <c r="AI223">
+        <v>0.08628010871073601</v>
+      </c>
+      <c r="AJ223">
+        <v>0.076396897708881</v>
+      </c>
+      <c r="AK223">
+        <v>0.084528894902534</v>
+      </c>
+      <c r="AL223">
+        <v>0.076146602278652</v>
+      </c>
+      <c r="AM223">
+        <v>0.077144883133744</v>
+      </c>
+      <c r="AN223">
+        <v>0.091333019745215</v>
+      </c>
+      <c r="AO223">
+        <v>0.11355142424529</v>
+      </c>
+      <c r="AP223">
+        <v>0.075026630864569</v>
+      </c>
+      <c r="AQ223">
+        <v>0.07490870546028</v>
+      </c>
+      <c r="AR223">
+        <v>0.067570076155437</v>
+      </c>
+      <c r="AS223">
+        <v>0.073210819290301</v>
+      </c>
+      <c r="AT223">
+        <v>0.10172926921491</v>
+      </c>
+      <c r="AU223">
+        <v>0.11557876514312</v>
+      </c>
+      <c r="AV223">
+        <v>0.10467036428253</v>
+      </c>
+      <c r="AW223">
+        <v>0.09667340308639701</v>
+      </c>
+      <c r="AX223">
+        <v>0.11037119050772</v>
+      </c>
+      <c r="AY223">
+        <v>0.076683385647284</v>
+      </c>
+      <c r="AZ223">
+        <v>0.061740543902011</v>
+      </c>
+      <c r="BA223">
+        <v>0.07759327208738601</v>
+      </c>
+      <c r="BB223">
+        <v>0.07476624676076001</v>
+      </c>
+      <c r="BC223">
+        <v>0.08458549483254001</v>
+      </c>
+      <c r="BD223">
+        <v>0.083740135382133</v>
+      </c>
+      <c r="BE223">
+        <v>0.11442422988874</v>
+      </c>
+    </row>
+    <row r="224" spans="1:57">
+      <c r="A224" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="225" spans="1:1">
+      <c r="A225" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="226" spans="1:1">
+      <c r="A226" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="227" spans="1:1">
+      <c r="A227" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="228" spans="1:1">
+      <c r="A228" t="s">
+        <v>282</v>
       </c>
     </row>
   </sheetData>

</xml_diff>